<commit_message>
[24.02.06 15:44] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="490" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87E7EE5A-77EB-4CFF-B3F2-50080EF77B55}"/>
+  <xr:revisionPtr revIDLastSave="504" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7C56D4D-0218-4BE4-B173-289C4AA63644}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="705" windowWidth="25860" windowHeight="14580" firstSheet="13" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="1659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2034" uniqueCount="1678">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -4279,133 +4279,283 @@
     <t>Information non connue lors de l’appel</t>
   </si>
   <si>
-    <t>CodeLien_patients-victimes</t>
+    <t>SI-SAMU</t>
+  </si>
+  <si>
+    <t>TYPAPPLT</t>
   </si>
   <si>
     <t>Daphné Leccia</t>
   </si>
   <si>
+    <t>SUJET</t>
+  </si>
+  <si>
+    <t>Le patient lui-même</t>
+  </si>
+  <si>
+    <t>Le patient lui-même, victime de l’événement signalé et bénéficiaire des moyens qui pourraient être décidés même s’il a une des fonctions ou titres ci-dessous.</t>
+  </si>
+  <si>
+    <t>FAMILLE</t>
+  </si>
+  <si>
+    <t>Famille ou proche du patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requérant qui se présente comme membre de la famille ou proche (concubin, compagnon, colocataire, ...) de la victime de l’événement signalé même s’il a un des titres ou une des fonctions ci-dessous. </t>
+  </si>
+  <si>
+    <t>TIERS</t>
+  </si>
+  <si>
+    <t>Autre particulier ou passant</t>
+  </si>
+  <si>
+    <t>Particulier qui n’a pas une des fonctions ou titres ci-dessous et qui ne fait pas partie de la famille de la victime.</t>
+  </si>
+  <si>
+    <t>POMPIER</t>
+  </si>
+  <si>
+    <t>Pompier</t>
+  </si>
+  <si>
+    <t>Le requérant est un pompier professionnel ou volontaire en activité et agissant dans le cadre de sa profession au moment de l’appel.</t>
+  </si>
+  <si>
+    <t>AMBULANC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambulancier </t>
+  </si>
+  <si>
+    <t>Le requérant est un ambulancier agissant dans le cadre de sa profession au moment de l’appel.</t>
+  </si>
+  <si>
+    <t>SECOUR</t>
+  </si>
+  <si>
+    <t>Secouriste actif</t>
+  </si>
+  <si>
+    <t>Pour tout secouriste actif (ambulancier, secouriste agissant pour une société ou une association de secourisme) mais uniquement s’il est en activité et n’est pas un professionnel de santé.</t>
+  </si>
+  <si>
+    <t>MED</t>
+  </si>
+  <si>
+    <t>Médecin</t>
+  </si>
+  <si>
+    <t>Regroupe les médecins de toute spécialité, de tout statut mais uniquement s’ils sont en activité et agissent dans le cadre de leur profession au moment de l’appel.</t>
+  </si>
+  <si>
+    <t>MEDSOS</t>
+  </si>
+  <si>
+    <t>Médecin SOS ou association PDS</t>
+  </si>
+  <si>
+    <t>Déclinaison du type Médecin : Regroupe les médecins SOS, uniquement s’ils sont en activité et agissent dans le cadre de leur profession au moment de l’appel.</t>
+  </si>
+  <si>
+    <t>MRL</t>
+  </si>
+  <si>
+    <t>Médecin régulateur libéral</t>
+  </si>
+  <si>
+    <t>Déclinaison du type Médecin : Regroupe les demandes issues des médecins régulateurs généralistes lorsque le DRM n’est pas encore créé dans le SI-Samu (par exemple quand il a été jusque-là uniquement renseigné dans un SI-PDSA).</t>
+  </si>
+  <si>
+    <t>EFFML</t>
+  </si>
+  <si>
+    <t>Effecteur de médecine libérale</t>
+  </si>
+  <si>
+    <t>Déclinaison du type Médecin : Regroupe les demandes issues des médecins effecteurs de médecine générale (hors médecins de SOS ou association de PDSA) lorsque le DRM n’est pas encore créé dans le SI-Samu (par exemple quand il a été jusque-là uniquement renseigné dans un SI-PDSA).</t>
+  </si>
+  <si>
+    <t>SANTE</t>
+  </si>
+  <si>
+    <t>Autre acteur de santé</t>
+  </si>
+  <si>
+    <t>Regroupe tous les autres professionnels de santé, de toute spécialité, de tout statut mais uniquement s’ils sont en activité et agissent dans le cadre de leur profession au moment de l’appel.</t>
+  </si>
+  <si>
+    <t>INF</t>
+  </si>
+  <si>
+    <t>Infirmier</t>
+  </si>
+  <si>
+    <t>Regroupe les infirmiers de toute spécialité, de tout statut mais uniquement s’ils sont en activité et agissent dans le cadre de leur profession au moment de l’appel.</t>
+  </si>
+  <si>
+    <t>AIDESOIN</t>
+  </si>
+  <si>
+    <t>Aide-soignant</t>
+  </si>
+  <si>
+    <t>Regroupe les aides-soignants, de tout statut mais uniquement s’ils sont en activité et agissent dans le cadre de leur profession au moment de l’appel.</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>Sage-femme</t>
+  </si>
+  <si>
+    <t>Regroupe les sage-femmes, de tout statut mais uniquement s’ils sont en activité et agissent dans le cadre de leur profession au moment de l’appel.</t>
+  </si>
+  <si>
+    <t>AIDEDOM</t>
+  </si>
+  <si>
+    <t>Aide à domicile</t>
+  </si>
+  <si>
+    <t>Regroupe les aides à domicile, de tout statut mais uniquement s’ils sont en activité et agissent dans le cadre de leur profession au moment de l’appel.</t>
+  </si>
+  <si>
+    <t>FDO-MILI</t>
+  </si>
+  <si>
+    <t>Policier Gendarme Militaire</t>
+  </si>
+  <si>
+    <t>Regroupe tout policier, gendarme, militaire de tout statut et de tout grade mais uniquement s’il est en activité et n’est pas un professionnel de santé ou un secouriste actif.</t>
+  </si>
+  <si>
+    <t>ADM-TUTL</t>
+  </si>
+  <si>
+    <t>Membre d'une autorité administrative</t>
+  </si>
+  <si>
+    <t>L’appelant est issu d’une autorité administrative (de tutelle) et appelle les services d’urgence dans le cadre de ses fonctions (ex : ARS, Ministère de la santé, HAS…)</t>
+  </si>
+  <si>
+    <t>VIP</t>
+  </si>
+  <si>
+    <t>Personne publique, de notoriété</t>
+  </si>
+  <si>
+    <t>OBJCONNC</t>
+  </si>
+  <si>
+    <t>Objets connectés</t>
+  </si>
+  <si>
+    <t>L’appelant initial n’est pas une personne physique mais un objet connecté en mesure de passer des appels d’urgences (ex : automobile dans le cadre des appels e-call)</t>
+  </si>
+  <si>
     <t>AUTRE</t>
   </si>
   <si>
-    <t>Autre</t>
-  </si>
-  <si>
-    <t>BEAUF  </t>
-  </si>
-  <si>
-    <t>Beau fils</t>
-  </si>
-  <si>
-    <t>BEAU  </t>
-  </si>
-  <si>
-    <t>Beau père</t>
-  </si>
-  <si>
-    <t>BELLE  </t>
-  </si>
-  <si>
-    <t>Belle mère</t>
-  </si>
-  <si>
-    <t>DIVERS  </t>
-  </si>
-  <si>
-    <t>EPOUSE  </t>
-  </si>
-  <si>
-    <t>Epouse</t>
-  </si>
-  <si>
-    <t>EPOUX  </t>
-  </si>
-  <si>
-    <t>Epoux</t>
-  </si>
-  <si>
-    <t>FILLE </t>
-  </si>
-  <si>
-    <t>Fille</t>
-  </si>
-  <si>
-    <t>FILS  </t>
-  </si>
-  <si>
-    <t>Fils</t>
-  </si>
-  <si>
-    <t>FRERE  </t>
-  </si>
-  <si>
-    <t>Frère</t>
-  </si>
-  <si>
-    <t>ONCLE  </t>
-  </si>
-  <si>
-    <t>Oncle</t>
-  </si>
-  <si>
-    <t>PETIT</t>
-  </si>
-  <si>
-    <t>Petit-fils</t>
-  </si>
-  <si>
-    <t>PETITE  </t>
-  </si>
-  <si>
-    <t>Petite-fille</t>
-  </si>
-  <si>
-    <t>PERE  </t>
-  </si>
-  <si>
-    <t>Père</t>
-  </si>
-  <si>
-    <t>MERE  </t>
-  </si>
-  <si>
-    <t>Mère</t>
-  </si>
-  <si>
-    <t>SOEUR  </t>
-  </si>
-  <si>
-    <t>Soeur</t>
-  </si>
-  <si>
-    <t>TANTE  </t>
-  </si>
-  <si>
-    <t>Tante</t>
-  </si>
-  <si>
-    <t>VOISIN  </t>
-  </si>
-  <si>
-    <t>Voisin</t>
-  </si>
-  <si>
-    <t>GRANDM  </t>
-  </si>
-  <si>
-    <t>Grand-mère</t>
-  </si>
-  <si>
-    <t>GRANDP  </t>
-  </si>
-  <si>
-    <t>Grand-père</t>
-  </si>
-  <si>
-    <t>SELF  </t>
-  </si>
-  <si>
-    <t>L'appelant est le patient</t>
+    <t>Autre type d’appelant</t>
+  </si>
+  <si>
+    <t>Pour toutes les fonctions non prévues ci-dessus.</t>
+  </si>
+  <si>
+    <t>INCONNU</t>
+  </si>
+  <si>
+    <t>Type d'appelant indéterminé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si la fonction ou le titre de l'appelant est inconnu. </t>
+  </si>
+  <si>
+    <t>PBAPL</t>
+  </si>
+  <si>
+    <t>Daphné Leccia/ Elodie Falcioni</t>
+  </si>
+  <si>
+    <t>AUCUNE</t>
+  </si>
+  <si>
+    <t>Aucune difficulté de communication</t>
+  </si>
+  <si>
+    <t>Aucune difficulté de communication rencontrée entre l’appelant et la personne qualifiant ou régulant le dossier.</t>
+  </si>
+  <si>
+    <t>MUET</t>
+  </si>
+  <si>
+    <t>Muet ou malentendant (troubles de la parole ou de l'audition)</t>
+  </si>
+  <si>
+    <t>Difficultés de communication liées aux caractéristiques de l’appelant, muet ou ayant des troubles prononcés de l’élocution, malentendant ou ayant des troubles prononcés de l’audition ne lui permettant pas d’interagir dans de bonnes conditions avec son interlocuteur du CRRA</t>
+  </si>
+  <si>
+    <t>VISION</t>
+  </si>
+  <si>
+    <t>Malvoyant, troubles de la vision</t>
+  </si>
+  <si>
+    <t>Difficultés de communication liées aux caractéristiques de l’appelant, malvoyant ou ayant des troubles prononcés de la vue ne lui permettant pas de décrire correctement la situation pour laquelle il appelle</t>
+  </si>
+  <si>
+    <t>LANGUE</t>
+  </si>
+  <si>
+    <t>Barrière de la langue (langue étrangère)</t>
+  </si>
+  <si>
+    <t>Difficultés de communication avec l’appelant liées au fait que l’appelant ne comprend pas ou mal le français ou ne le parle pas ou mal</t>
+  </si>
+  <si>
+    <t>PANIQUE</t>
+  </si>
+  <si>
+    <t>Panique de l’appelant</t>
+  </si>
+  <si>
+    <t>Difficultés de communication avec l’appelant liées à une situation de stress extrême ou de panique de l’appelant, du patient ou de l’entourage ne lui permettant pas de décrire correctement la situation pour laquelle il appelle</t>
+  </si>
+  <si>
+    <t>HOSTILE</t>
+  </si>
+  <si>
+    <t>Appelant hostile, agressif</t>
+  </si>
+  <si>
+    <t>Difficultés de communication avec l’appelant liées à une situation d’hostilité ou d’agressivité de l’appelant ne permettant pas une bonne compréhension du problème pour lequel il appelle</t>
+  </si>
+  <si>
+    <t>AGITE</t>
+  </si>
+  <si>
+    <t>Incohérence, agitation, intoxication</t>
+  </si>
+  <si>
+    <t>Patient psychiatrique ayant des difficultés pour exprimer sa plainte ou patient alcoolisé, agité et incohérent dans l’incapacité de formuler les raisons de son appel</t>
+  </si>
+  <si>
+    <t>Autres difficultés de communication</t>
+  </si>
+  <si>
+    <t>Autres troubles humains ou techniques, de l’appelant ou de l’entourage, empêchant la bonne interaction entre l’appelant et la personne qualifiant ou régulant le dossier et la bonne compréhension de la situation pour laquelle il appelle</t>
+  </si>
+  <si>
+    <t>IMPOSS</t>
+  </si>
+  <si>
+    <t>Absence de communication</t>
+  </si>
+  <si>
+    <t>Pas de communication possible avec l’appelant (ex : pas d'echange vocal, appel raccroché prématurement sans contre appel possible, ...)</t>
   </si>
   <si>
     <t>CodeEffet_a_obtenir</t>
@@ -4705,7 +4855,7 @@
     <t>EO.07.02</t>
   </si>
   <si>
-    <t>SI-SAMU</t>
+    <t>DEVENIRD</t>
   </si>
   <si>
     <t xml:space="preserve">Elodie Falcioni </t>
@@ -4714,471 +4864,429 @@
     <t>DRM</t>
   </si>
   <si>
+    <t>Dossier de régulation médicale</t>
+  </si>
+  <si>
     <t>DRMMRU</t>
   </si>
   <si>
+    <t>DRM MRU</t>
+  </si>
+  <si>
+    <t>Dossier de type médecine d’urgence</t>
+  </si>
+  <si>
     <t>MU</t>
   </si>
   <si>
+    <t>Régulation MU</t>
+  </si>
+  <si>
+    <t>Dossier de type médecine d’urgence régulé par un médecin urgentiste. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>DENT</t>
   </si>
   <si>
+    <t>Régulation dentaire</t>
+  </si>
+  <si>
+    <t>Dossier régulé par un chirurgien dentiste au sein du CRRA. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>GERIA</t>
   </si>
   <si>
+    <t>Régulation gériatrique</t>
+  </si>
+  <si>
+    <t>Dossier régulé par un gériatre au sein du CRRA. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>PEDIA</t>
   </si>
   <si>
+    <t>Régulation pédiatrie</t>
+  </si>
+  <si>
+    <t>Dossier régulé par un pédiatre au sein du CRRA. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>PSY</t>
   </si>
   <si>
+    <t>Régulation psychiatrie</t>
+  </si>
+  <si>
+    <t>Dossier régulé par un psychiatre au sein du CRRA. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>TOXICOL</t>
   </si>
   <si>
+    <t>Régulation toxicologique</t>
+  </si>
+  <si>
+    <t>Dossier régulé par un toxicologue au sein du CRRA. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>INDISPMU</t>
   </si>
   <si>
+    <t>Régulation ML par indisponibilité MU</t>
+  </si>
+  <si>
+    <t>Dossier de type médecine d'urgence régulé par un médecin libéral du fait de l’indisponibilité des MU. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>SSE</t>
   </si>
   <si>
+    <t>Régulation de crise - NOVI</t>
+  </si>
+  <si>
+    <t>Dossier relevant de la gestion de crise – NOmbreuses Victimes. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>PLANBLAN</t>
   </si>
   <si>
+    <t>Régulation Plan Blanc</t>
+  </si>
+  <si>
+    <t>Dossier régulé dans le cadre d’ un dispositif plan blanc. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>PCSAMU</t>
   </si>
   <si>
+    <t>Régulation par un PC mobile</t>
+  </si>
+  <si>
+    <t>Dossier régulé depuis un poste de commandement  mobile. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>DRMMRL</t>
   </si>
   <si>
+    <t>DRM MRL</t>
+  </si>
+  <si>
+    <t>Dossier de type médecine libérale</t>
+  </si>
+  <si>
     <t>MG</t>
   </si>
   <si>
+    <t>Régulation ML</t>
+  </si>
+  <si>
+    <t>Dossier de type médecine libérale régulé par un médecin libéral. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>INDISPMG</t>
   </si>
   <si>
+    <t>Régulation MU par indisponibilité ML</t>
+  </si>
+  <si>
+    <t>Dossier de type médecine libérale régulé par un médecin urgentiste du fait de l’indisponibilité des ML. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>ABSML</t>
   </si>
   <si>
+    <t>Régulation MU par absence de régulation ML</t>
+  </si>
+  <si>
+    <t>Dossier de type médecine libérale régulé par un médecin urgentiste du fait de l’absence de régulation ML. Le dossier devient de type DRM</t>
+  </si>
+  <si>
     <t>DR</t>
   </si>
   <si>
+    <t>Dossier de régulation</t>
+  </si>
+  <si>
     <t>DREG</t>
   </si>
   <si>
+    <t>Dossier Régulation</t>
+  </si>
+  <si>
     <t>DRARM</t>
   </si>
   <si>
+    <t>Pas d’acte de régulation médicale - Prise en charge ARM</t>
+  </si>
+  <si>
+    <t>Dossier ne relevant pas de la régulation médicale et pas dans le cadre des autre cas identifié (voir cas suivant). Le dossier est de type DR</t>
+  </si>
+  <si>
     <t>DRMED</t>
   </si>
   <si>
+    <t>Pas d’acte de régulation médicale - Transmission d'informations sur un médecin (procédure dégradée)</t>
+  </si>
+  <si>
+    <t>Dossier ne relevant pas de la régulation médicale – réponse apportée à une demande de renseignements sur un médecin. Le dossier est de type DR</t>
+  </si>
+  <si>
     <t>DRPHARMA</t>
   </si>
   <si>
+    <t>Pas d’acte de régulation médicale - Transmission d'informations sur une pharmacie</t>
+  </si>
+  <si>
+    <t>Dossier ne relevant pas de la régulation médicale – réponse apportée à une demande de renseignements sur une pharmacie. Le dossier est de type DR</t>
+  </si>
+  <si>
     <t>DRDENT</t>
   </si>
   <si>
+    <t>Pas d’acte de régulation médicale - Transmission d'informations sur un dentiste</t>
+  </si>
+  <si>
+    <t>Dossier ne relevant pas de la régulation médicale – réponse apportée à une demande de renseignements sur un dentiste. Le dossier est de type DR</t>
+  </si>
+  <si>
     <t>DRINFO</t>
   </si>
   <si>
+    <t>Pas d’acte de régulation médicale - Information générale</t>
+  </si>
+  <si>
+    <t>Dossier ne relevant pas de la régulation médicale – réponse apportée à une demande de renseignements d’ordre général. Le dossier est de type DR</t>
+  </si>
+  <si>
     <t>DOS-SIS</t>
   </si>
   <si>
+    <t>Pas d’acte de régulation médicale - Appel pour les pompiers</t>
+  </si>
+  <si>
+    <t>Dossier ne rentrant pas dans le cadre des missions du Samu et confié aux pompiers. Le dossier est de type DR</t>
+  </si>
+  <si>
     <t>DOS-FDO</t>
   </si>
   <si>
+    <t>Pas d’acte de régulation médicale - Appel pour les forces de l’ordre</t>
+  </si>
+  <si>
+    <t>Dossier ne rentrant pas dans le cadre des missions du Samu et confié aux forces de l'ordre. Le dossier est de type DR</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
+    <t>Dossier</t>
+  </si>
+  <si>
     <t>D-MALV</t>
   </si>
   <si>
+    <t>Erreur / Malveillant</t>
+  </si>
+  <si>
+    <t>Dossier de type erreur ou appel malveillant</t>
+  </si>
+  <si>
     <t>ERR</t>
   </si>
   <si>
+    <t>Erreur de numéro, erreur d'acheminement</t>
+  </si>
+  <si>
+    <t>Le requérant s’est trompé de numéro de téléphone ou a mal été orienté par un interlocuteur précédent. Le dossier reste de type D</t>
+  </si>
+  <si>
     <t>NRP</t>
   </si>
   <si>
+    <t xml:space="preserve">Appel raccroché / pas de réponse </t>
+  </si>
+  <si>
+    <t>L’appel est raccroché ou sans réponse de l’appelant à l’ouverture du dossier. Le dossier reste de type D</t>
+  </si>
+  <si>
     <t>MALV</t>
   </si>
   <si>
+    <t>Appel malveillant, canular</t>
+  </si>
+  <si>
+    <t>Appel malveillant : insultes, canular, fausses informations. Il ne s’agit pas d’une erreur de numéro. Le dossier reste de type D</t>
+  </si>
+  <si>
     <t>FAX</t>
   </si>
   <si>
+    <t>Tonalité de fax, porteuse</t>
+  </si>
+  <si>
+    <t>Tonalité de fax ou d’une porteuse  présente au décroché. Le dossier reste de type D</t>
+  </si>
+  <si>
     <t>ITERATIF</t>
   </si>
   <si>
+    <t>Dossier existant, appel itératif (hors SI-Samu)</t>
+  </si>
+  <si>
+    <t>Appels pour un dossier déjà existant. Entraine la recherche et l’ouverture du dossier préexistant avec rattachement de l’appel à ce dossier (option à supprimer dès l'intégration au SI-Samu)</t>
+  </si>
+  <si>
     <t>D-IDENT</t>
   </si>
   <si>
+    <t>Appel identifié</t>
+  </si>
+  <si>
+    <t>Dossier en rapport avec un appel qui n'est ni un DR ni un DRM</t>
+  </si>
+  <si>
     <t>ADMIN</t>
   </si>
   <si>
+    <t>Appel administratif</t>
+  </si>
+  <si>
+    <t>Dossier ne relevant pas de la régulation médicale – et concerne la gestion administrative d’un dossier clôturé. Le dossier reste de type D</t>
+  </si>
+  <si>
     <t>PERSO</t>
   </si>
   <si>
-    <t>DRM MRU</t>
-  </si>
-  <si>
-    <t>Régulation MU</t>
-  </si>
-  <si>
-    <t>Régulation dentaire</t>
-  </si>
-  <si>
-    <t>Régulation gériatrique</t>
-  </si>
-  <si>
-    <t>Régulation pédiatrie</t>
-  </si>
-  <si>
-    <t>Régulation psychiatrie</t>
-  </si>
-  <si>
-    <t>Régulation toxicologique</t>
-  </si>
-  <si>
-    <t>Régulation ML par indisponibilité MU</t>
-  </si>
-  <si>
-    <t>Régulation de crise - NOVI</t>
-  </si>
-  <si>
-    <t>Régulation Plan Blanc</t>
-  </si>
-  <si>
-    <t>Régulation par un PC mobile</t>
-  </si>
-  <si>
-    <t>DRM MRL</t>
-  </si>
-  <si>
-    <t>Régulation ML</t>
-  </si>
-  <si>
-    <t>Régulation MU par indisponibilité ML</t>
-  </si>
-  <si>
-    <t>Régulation MU par absence de régulation ML</t>
-  </si>
-  <si>
-    <t>Dossier Régulation</t>
-  </si>
-  <si>
-    <t>Pas d’acte de régulation médicale - Prise en charge ARM</t>
-  </si>
-  <si>
-    <t>Pas d’acte de régulation médicale - Transmission d'informations sur un médecin (procédure dégradée)</t>
-  </si>
-  <si>
-    <t>Pas d’acte de régulation médicale - Transmission d'informations sur une pharmacie</t>
-  </si>
-  <si>
-    <t>Pas d’acte de régulation médicale - Transmission d'informations sur un dentiste</t>
-  </si>
-  <si>
-    <t>Pas d’acte de régulation médicale - Information générale</t>
-  </si>
-  <si>
-    <t>Pas d’acte de régulation médicale - Appel pour les pompiers</t>
-  </si>
-  <si>
-    <t>Pas d’acte de régulation médicale - Appel pour les forces de l’ordre</t>
-  </si>
-  <si>
-    <t>Erreur / Malveillant</t>
-  </si>
-  <si>
-    <t>Erreur de numéro, erreur d'acheminement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Appel raccroché / pas de réponse </t>
-  </si>
-  <si>
-    <t>Appel malveillant, canular</t>
-  </si>
-  <si>
-    <t>Tonalité de fax, porteuse</t>
-  </si>
-  <si>
-    <t>Dossier existant, appel itératif (hors SI-Samu)</t>
-  </si>
-  <si>
-    <t>Appel identifié</t>
-  </si>
-  <si>
-    <t>Appel administratif</t>
-  </si>
-  <si>
     <t>Appel personnel</t>
   </si>
   <si>
+    <t>L’appel concerne une communication pour un membre du personnel et a un caractère privé. Le dossier reste de type D</t>
+  </si>
+  <si>
     <t>Autre type d’appel</t>
   </si>
   <si>
-    <t>Dossier de régulation médicale</t>
-  </si>
-  <si>
-    <t>Dossier de type médecine d’urgence</t>
-  </si>
-  <si>
-    <t>Dossier de type médecine d’urgence régulé par un médecin urgentiste. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier régulé par un chirurgien dentiste au sein du CRRA. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier régulé par un gériatre au sein du CRRA. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier régulé par un pédiatre au sein du CRRA. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier régulé par un psychiatre au sein du CRRA. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier régulé par un toxicologue au sein du CRRA. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier de type médecine d'urgence régulé par un médecin libéral du fait de l’indisponibilité des MU. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier relevant de la gestion de crise – NOmbreuses Victimes. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier régulé dans le cadre d’ un dispositif plan blanc. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier régulé depuis un poste de commandement  mobile. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier de type médecine libérale</t>
-  </si>
-  <si>
-    <t>Dossier de type médecine libérale régulé par un médecin libéral. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier de type médecine libérale régulé par un médecin urgentiste du fait de l’indisponibilité des ML. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier de type médecine libérale régulé par un médecin urgentiste du fait de l’absence de régulation ML. Le dossier devient de type DRM</t>
-  </si>
-  <si>
-    <t>Dossier de régulation</t>
-  </si>
-  <si>
-    <t>Dossier ne relevant pas de la régulation médicale et pas dans le cadre des autre cas identifié (voir cas suivant). Le dossier est de type DR</t>
-  </si>
-  <si>
-    <t>Dossier ne relevant pas de la régulation médicale – réponse apportée à une demande de renseignements sur un médecin. Le dossier est de type DR</t>
-  </si>
-  <si>
-    <t>Dossier ne relevant pas de la régulation médicale – réponse apportée à une demande de renseignements sur une pharmacie. Le dossier est de type DR</t>
-  </si>
-  <si>
-    <t>Dossier ne relevant pas de la régulation médicale – réponse apportée à une demande de renseignements sur un dentiste. Le dossier est de type DR</t>
-  </si>
-  <si>
-    <t>Dossier ne relevant pas de la régulation médicale – réponse apportée à une demande de renseignements d’ordre général. Le dossier est de type DR</t>
-  </si>
-  <si>
-    <t>Dossier ne rentrant pas dans le cadre des missions du Samu et confié aux pompiers. Le dossier est de type DR</t>
-  </si>
-  <si>
-    <t>Dossier ne rentrant pas dans le cadre des missions du Samu et confié aux forces de l'ordre. Le dossier est de type DR</t>
-  </si>
-  <si>
-    <t>Dossier</t>
-  </si>
-  <si>
-    <t>Dossier de type erreur ou appel malveillant</t>
-  </si>
-  <si>
-    <t>Le requérant s’est trompé de numéro de téléphone ou a mal été orienté par un interlocuteur précédent. Le dossier reste de type D</t>
-  </si>
-  <si>
-    <t>L’appel est raccroché ou sans réponse de l’appelant à l’ouverture du dossier. Le dossier reste de type D</t>
-  </si>
-  <si>
-    <t>Appel malveillant : insultes, canular, fausses informations. Il ne s’agit pas d’une erreur de numéro. Le dossier reste de type D</t>
-  </si>
-  <si>
-    <t>Tonalité de fax ou d’une porteuse  présente au décroché. Le dossier reste de type D</t>
-  </si>
-  <si>
-    <t>Appels pour un dossier déjà existant. Entraine la recherche et l’ouverture du dossier préexistant avec rattachement de l’appel à ce dossier (option à supprimer dès l'intégration au SI-Samu)</t>
-  </si>
-  <si>
-    <t>Dossier en rapport avec un appel qui n'est ni un DR ni un DRM</t>
-  </si>
-  <si>
-    <t>Dossier ne relevant pas de la régulation médicale – et concerne la gestion administrative d’un dossier clôturé. Le dossier reste de type D</t>
-  </si>
-  <si>
-    <t>L’appel concerne une communication pour un membre du personnel et a un caractère privé. Le dossier reste de type D</t>
-  </si>
-  <si>
     <t>Autre type d’appel non régulé et relevant pas d’un problème médical, social ou sanitaire. Le dossier reste de type D</t>
   </si>
   <si>
-    <t>PBAPL</t>
-  </si>
-  <si>
-    <t>DEVENIRD</t>
-  </si>
-  <si>
-    <t>AUCUNE</t>
-  </si>
-  <si>
-    <t>MUET</t>
-  </si>
-  <si>
-    <t>VISION</t>
-  </si>
-  <si>
-    <t>LANGUE</t>
-  </si>
-  <si>
-    <t>PANIQUE</t>
-  </si>
-  <si>
-    <t>HOSTILE</t>
-  </si>
-  <si>
-    <t>AGITE</t>
-  </si>
-  <si>
-    <t>IMPOSS</t>
-  </si>
-  <si>
-    <t>Aucune difficulté de communication</t>
-  </si>
-  <si>
-    <t>Muet ou malentendant (troubles de la parole ou de l'audition)</t>
-  </si>
-  <si>
-    <t>Malvoyant, troubles de la vision</t>
-  </si>
-  <si>
-    <t>Barrière de la langue (langue étrangère)</t>
-  </si>
-  <si>
-    <t>Panique de l’appelant</t>
-  </si>
-  <si>
-    <t>Appelant hostile, agressif</t>
-  </si>
-  <si>
-    <t>Incohérence, agitation, intoxication</t>
-  </si>
-  <si>
-    <t>Autres difficultés de communication</t>
-  </si>
-  <si>
-    <t>Absence de communication</t>
-  </si>
-  <si>
-    <t>Aucune difficulté de communication rencontrée entre l’appelant et la personne qualifiant ou régulant le dossier.</t>
-  </si>
-  <si>
-    <t>Difficultés de communication liées aux caractéristiques de l’appelant, muet ou ayant des troubles prononcés de l’élocution, malentendant ou ayant des troubles prononcés de l’audition ne lui permettant pas d’interagir dans de bonnes conditions avec son interlocuteur du CRRA</t>
-  </si>
-  <si>
-    <t>Difficultés de communication liées aux caractéristiques de l’appelant, malvoyant ou ayant des troubles prononcés de la vue ne lui permettant pas de décrire correctement la situation pour laquelle il appelle</t>
-  </si>
-  <si>
-    <t>Difficultés de communication avec l’appelant liées au fait que l’appelant ne comprend pas ou mal le français ou ne le parle pas ou mal</t>
-  </si>
-  <si>
-    <t>Difficultés de communication avec l’appelant liées à une situation de stress extrême ou de panique de l’appelant, du patient ou de l’entourage ne lui permettant pas de décrire correctement la situation pour laquelle il appelle</t>
-  </si>
-  <si>
-    <t>Difficultés de communication avec l’appelant liées à une situation d’hostilité ou d’agressivité de l’appelant ne permettant pas une bonne compréhension du problème pour lequel il appelle</t>
-  </si>
-  <si>
-    <t>Patient psychiatrique ayant des difficultés pour exprimer sa plainte ou patient alcoolisé, agité et incohérent dans l’incapacité de formuler les raisons de son appel</t>
-  </si>
-  <si>
-    <t>Autres troubles humains ou techniques, de l’appelant ou de l’entourage, empêchant la bonne interaction entre l’appelant et la personne qualifiant ou régulant le dossier et la bonne compréhension de la situation pour laquelle il appelle</t>
-  </si>
-  <si>
-    <t>Pas de communication possible avec l’appelant (ex : pas d'echange vocal, appel raccroché prématurement sans contre appel possible, ...)</t>
-  </si>
-  <si>
-    <t>Daphné Leccia/ Elodie Falcioni</t>
+    <t>PRIORITE</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>Ultra-Prioritaire</t>
+  </si>
+  <si>
+    <t>Régulation médicale ultra prioritaire</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Prioritaire</t>
+  </si>
+  <si>
+    <t>Régulation médicale prioritaire</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>Non Urgent</t>
+  </si>
+  <si>
+    <t>Régulation médicale non urgente (valeur attribuée par défaut)</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Différé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Régulation médicale différée </t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>Non régulé</t>
+  </si>
+  <si>
+    <t>Pas d’acte de régulation médicale</t>
+  </si>
+  <si>
+    <t>NOMENC_SEXE</t>
   </si>
   <si>
     <t>MASC</t>
   </si>
   <si>
+    <t>Masculin</t>
+  </si>
+  <si>
+    <t>Qualifie les individus de sexe masculin</t>
+  </si>
+  <si>
     <t>FEM</t>
   </si>
   <si>
-    <t>INCONNU</t>
-  </si>
-  <si>
-    <t>Masculin</t>
-  </si>
-  <si>
     <t>Féminin</t>
   </si>
   <si>
+    <t>Qualifie les individus de sexe féminin</t>
+  </si>
+  <si>
     <t>Autre sexe (ni masculin, ni féminin)</t>
   </si>
   <si>
+    <t>Qualifie les individus de troisième genre (individu considéré comme n ’étant ni homme ni femme, à la fois homme et femme, ou neutre)</t>
+  </si>
+  <si>
     <t>Inconnu</t>
   </si>
   <si>
-    <t>Qualifie les individus de sexe masculin</t>
-  </si>
-  <si>
-    <t>Qualifie les individus de sexe féminin</t>
-  </si>
-  <si>
-    <t>Qualifie les individus de troisième genre (individu considéré comme n ’étant ni homme ni femme, à la fois homme et femme, ou neutre)</t>
-  </si>
-  <si>
     <t>Le sexe de la personne n'est pas connu</t>
   </si>
   <si>
-    <t>NOMENC_SEXE</t>
-  </si>
-  <si>
     <t>GRAVITE</t>
   </si>
   <si>
     <t>R1</t>
   </si>
   <si>
+    <t>Urgence Vitale</t>
+  </si>
+  <si>
+    <t>Urgence vitale patente ou latente imposant l’envoi du Smur</t>
+  </si>
+  <si>
     <t>R2</t>
   </si>
   <si>
+    <t>Urgence vraie</t>
+  </si>
+  <si>
+    <t>Urgence vraie sans détresse vitale nécessitant l’envoi d’un médecin, d’une ambulance ou d’un VSAV. Le délai d’intervention est immédiat par défaut ou contractualisé entre le médecin régulateur et le requérant</t>
+  </si>
+  <si>
     <t>R3</t>
   </si>
   <si>
+    <t>Continuité de soins</t>
+  </si>
+  <si>
+    <t>Situation relevant de la continuité de soins. Le délai ne constituant pas un facteur de risque</t>
+  </si>
+  <si>
     <t>R4</t>
   </si>
   <si>
-    <t>Urgence Vitale</t>
-  </si>
-  <si>
-    <t>Urgence vraie</t>
-  </si>
-  <si>
-    <t>Continuité de soins</t>
-  </si>
-  <si>
     <t>Conseil ou PMT</t>
   </si>
   <si>
-    <t>Urgence vitale patente ou latente imposant l’envoi du Smur</t>
-  </si>
-  <si>
-    <t>Urgence vraie sans détresse vitale nécessitant l’envoi d’un médecin, d’une ambulance ou d’un VSAV. Le délai d’intervention est immédiat par défaut ou contractualisé entre le médecin régulateur et le requérant</t>
-  </si>
-  <si>
-    <t>Situation relevant de la continuité de soins. Le délai ne constituant pas un facteur de risque</t>
-  </si>
-  <si>
     <t>Situation pouvant être traitée par un conseil médical ou prescription médicamenteuse par téléphone</t>
   </si>
   <si>
@@ -5188,139 +5296,88 @@
     <t>CONSEIL</t>
   </si>
   <si>
+    <t>Conseil Médical</t>
+  </si>
+  <si>
+    <t>#Conseil Médical</t>
+  </si>
+  <si>
+    <t>Conduite à tenir donnée à distance par le médecin régulateur sans intervention d’un tiers. Le conseil médical peut être donné à la demande du patient ou à chaque fois que le médecin régulateur juge que l’appel ne nécessite pas un examen médical. Cette décision peut être accompagnée ou non d’une prescription médicamenteuse téléphonique. </t>
+  </si>
+  <si>
     <t>PMT</t>
   </si>
   <si>
+    <t>Prescription médicamenteuse téléphonique</t>
+  </si>
+  <si>
+    <t>#PMT</t>
+  </si>
+  <si>
+    <t>Réalisation d'une prescription médicamenteuse téléphonique</t>
+  </si>
+  <si>
     <t>INTER</t>
   </si>
   <si>
+    <t>Décision d’intervention</t>
+  </si>
+  <si>
+    <t>#Intervention</t>
+  </si>
+  <si>
+    <t>Décision qui implique l’envoi d’un moyen d’intervention (ressource mobile) : Smur, médical, paramédical, pompier ous transporteur sanitaire.</t>
+  </si>
+  <si>
     <t>ORIENT</t>
   </si>
   <si>
-    <t>Conseil Médical</t>
-  </si>
-  <si>
-    <t>#Conseil Médical</t>
-  </si>
-  <si>
-    <t>Prescription médicamenteuse téléphonique</t>
-  </si>
-  <si>
-    <t>#PMT</t>
-  </si>
-  <si>
-    <t>Décision d’intervention</t>
-  </si>
-  <si>
-    <t>#Intervention</t>
-  </si>
-  <si>
     <t xml:space="preserve">Décision d’orientation ou de transport </t>
   </si>
   <si>
     <t>#Orientation Transport</t>
   </si>
   <si>
+    <t>La décision d’orientation est caractérisée par le fait de renseigner la destination du patient (vers un acteur de santé, vers une structure ou activité de soins, vers un autre lieu). La décision de transport permet, en complément, de décider de la prise en charge du transport du patient vers ce lieu de destination et de décider du niveau de soin du transport.</t>
+  </si>
+  <si>
+    <t>PASPLUS</t>
+  </si>
+  <si>
     <t>Pas de décision supplémentaire</t>
   </si>
   <si>
     <t>#Décision</t>
   </si>
   <si>
-    <t>Conduite à tenir donnée à distance par le médecin régulateur sans intervention d’un tiers. Le conseil médical peut être donné à la demande du patient ou à chaque fois que le médecin régulateur juge que l’appel ne nécessite pas un examen médical. Cette décision peut être accompagnée ou non d’une prescription médicamenteuse téléphonique. </t>
-  </si>
-  <si>
-    <t>Réalisation d'une prescription médicamenteuse téléphonique</t>
-  </si>
-  <si>
-    <t>Décision qui implique l’envoi d’un moyen d’intervention (ressource mobile) : Smur, médical, paramédical, pompier ous transporteur sanitaire.</t>
-  </si>
-  <si>
-    <t>La décision d’orientation est caractérisée par le fait de renseigner la destination du patient (vers un acteur de santé, vers une structure ou activité de soins, vers un autre lieu). La décision de transport permet, en complément, de décider de la prise en charge du transport du patient vers ce lieu de destination et de décider du niveau de soin du transport.</t>
-  </si>
-  <si>
     <t>En raison des décisions déjà prises par un tiers, des éventuels moyens d’intervention déjà présents sur place, le médecin régulateur en charge de la régulation du dossier ne prend pas de décision supplémentaire en attendant l’évolution de la situation. </t>
   </si>
   <si>
-    <t>PASPLUS</t>
-  </si>
-  <si>
     <t>NIVSOIN</t>
   </si>
   <si>
-    <t>MED</t>
+    <t>Médicalisé</t>
+  </si>
+  <si>
+    <t>L'équipage du vecteur est composé d'au moins un médecin</t>
   </si>
   <si>
     <t>PARAMED</t>
   </si>
   <si>
+    <t>Paramédicalisé</t>
+  </si>
+  <si>
+    <t>L'équipage du vecteur ne comporte pas de médecin. Il est uniquement composé d'infirmier(e)s.</t>
+  </si>
+  <si>
     <t>SECOURS</t>
   </si>
   <si>
-    <t>Médicalisé</t>
-  </si>
-  <si>
-    <t>Paramédicalisé</t>
-  </si>
-  <si>
     <t>Secouriste</t>
   </si>
   <si>
-    <t>L'équipage du vecteur est composé d'au moins un médecin</t>
-  </si>
-  <si>
-    <t>L'équipage du vecteur ne comporte pas de médecin. Il est uniquement composé d'infirmier(e)s.</t>
-  </si>
-  <si>
     <t>L'équipage du vecteur ne comporte que des secouristes professionnnels ni médecin, ni infimier</t>
-  </si>
-  <si>
-    <t>P0</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>NR</t>
-  </si>
-  <si>
-    <t>Ultra-Prioritaire</t>
-  </si>
-  <si>
-    <t>Prioritaire</t>
-  </si>
-  <si>
-    <t>Non Urgent</t>
-  </si>
-  <si>
-    <t>Différé</t>
-  </si>
-  <si>
-    <t>Non régulé</t>
-  </si>
-  <si>
-    <t>PRIORITE</t>
-  </si>
-  <si>
-    <t>Régulation médicale ultra prioritaire</t>
-  </si>
-  <si>
-    <t>Régulation médicale prioritaire</t>
-  </si>
-  <si>
-    <t>Régulation médicale non urgente (valeur attribuée par défaut)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Régulation médicale différée </t>
-  </si>
-  <si>
-    <t>Pas d’acte de régulation médicale</t>
   </si>
 </sst>
 </file>
@@ -5512,7 +5569,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="59">
     <dxf>
       <font>
         <b val="0"/>
@@ -5768,41 +5825,7 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -6870,94 +6893,95 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A9:D27" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}" name="Table137" displayName="Table137" ref="A9:F308" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}" name="Table137" displayName="Table137" ref="A9:F308" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A9:F308" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F19F314C-B88E-48A0-9134-0480F8CF5303}" name="Code" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{600128F5-608F-4F75-ADD7-09E47F508C64}" name="Libellé niveau 1" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{69B015DB-FEAC-41E1-97CC-32D2D70D1E5F}" name="Libellé niveau 2" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{DDCC42E9-EE40-4BB4-8B10-7F7964B45C24}" name="Libellé niveau 3" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{B18EF0E1-670C-4280-93AF-67B4FB66EE2F}" name="Description" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{B87504F2-E81C-4AC3-AFB9-7F1544707E97}" name="Commentaire" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{F19F314C-B88E-48A0-9134-0480F8CF5303}" name="Code" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{600128F5-608F-4F75-ADD7-09E47F508C64}" name="Libellé niveau 1" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{69B015DB-FEAC-41E1-97CC-32D2D70D1E5F}" name="Libellé niveau 2" dataDxfId="48"/>
+    <tableColumn id="7" xr3:uid="{DDCC42E9-EE40-4BB4-8B10-7F7964B45C24}" name="Libellé niveau 3" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{B18EF0E1-670C-4280-93AF-67B4FB66EE2F}" name="Description" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{B87504F2-E81C-4AC3-AFB9-7F1544707E97}" name="Commentaire" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}" name="Table138" displayName="Table138" ref="A9:F188" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}" name="Table138" displayName="Table138" ref="A9:F188" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="A9:F188" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{68E43B73-9A3F-4404-BFFA-9D2C83024853}" name="Code" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{4EE1502F-9D93-480B-9E76-CF9D4340C70D}" name="Libellé niveau 1" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{7B9C8786-A455-41BE-8B0E-D205B49FACF5}" name="Libellé niveau 2" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{254DB673-9BA3-42AE-9511-308D7BCD2FC5}" name="Libellé niveau 3" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{704D9D94-904F-4137-9FA6-AF5A0D326491}" name="Description" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{E0842B8F-A591-4C1E-A821-41D16E287145}" name="Commentaire" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{68E43B73-9A3F-4404-BFFA-9D2C83024853}" name="Code" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{4EE1502F-9D93-480B-9E76-CF9D4340C70D}" name="Libellé niveau 1" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{7B9C8786-A455-41BE-8B0E-D205B49FACF5}" name="Libellé niveau 2" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{254DB673-9BA3-42AE-9511-308D7BCD2FC5}" name="Libellé niveau 3" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{704D9D94-904F-4137-9FA6-AF5A0D326491}" name="Description" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{E0842B8F-A591-4C1E-A821-41D16E287145}" name="Commentaire" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}" name="Table1" displayName="Table1" ref="A9:D46" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}" name="Table1" displayName="Table1" ref="A9:D46" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A9:D46" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{41A202AF-0A91-4C8F-B1DD-1D8B78C88B67}" name="Code" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{787839B6-641F-4C38-B883-AA61D5F0F7BA}" name="Libellé niveau 1" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{EA8B2165-6449-4C73-AB38-E548BEDD1CC6}" name="Description" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{E8FC5318-5334-4D19-B99B-DF7F88C59DC8}" name="Commentaire" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{41A202AF-0A91-4C8F-B1DD-1D8B78C88B67}" name="Code" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{787839B6-641F-4C38-B883-AA61D5F0F7BA}" name="Libellé niveau 1" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{EA8B2165-6449-4C73-AB38-E548BEDD1CC6}" name="Description" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{E8FC5318-5334-4D19-B99B-DF7F88C59DC8}" name="Commentaire" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}" name="Table139" displayName="Table139" ref="A9:E61" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}" name="Table139" displayName="Table139" ref="A9:E61" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A9:E61" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1E16E225-2AC0-42BC-891A-DE42FEC023D6}" name="Code" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{EAF0C6A6-B766-472E-B250-B4F25993D46E}" name="Libellé niveau 1" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{81750735-53CA-440E-972E-333E415A08B6}" name="Libellé niveau 2" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{D8928B6E-6058-44ED-A422-FB52AA55B676}" name="Description" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{8EE4E12B-725F-47C8-B534-7688D1544C58}" name="Commentaire" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{1E16E225-2AC0-42BC-891A-DE42FEC023D6}" name="Code" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{EAF0C6A6-B766-472E-B250-B4F25993D46E}" name="Libellé niveau 1" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{81750735-53CA-440E-972E-333E415A08B6}" name="Libellé niveau 2" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{D8928B6E-6058-44ED-A422-FB52AA55B676}" name="Description" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{8EE4E12B-725F-47C8-B534-7688D1544C58}" name="Commentaire" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8BF6ADF-B677-473E-8ABE-51264084FE99}" name="Table13" displayName="Table13" ref="A9:D14" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8BF6ADF-B677-473E-8ABE-51264084FE99}" name="Table13" displayName="Table13" ref="A9:D14" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A9:D14" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{98FD5D52-1BC0-4054-8358-F924F6A4BAB5}" name="Code" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{09CB4271-3531-437E-96F1-FF338E0F430E}" name="Libellé niveau 1" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{2E9B13FA-3333-42A6-BF3A-F3B7AD42D98A}" name="Description" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{EBA22499-7DD5-405F-82CA-7058FFC1AB2F}" name="Commentaire" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{98FD5D52-1BC0-4054-8358-F924F6A4BAB5}" name="Code" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{09CB4271-3531-437E-96F1-FF338E0F430E}" name="Libellé niveau 1" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{2E9B13FA-3333-42A6-BF3A-F3B7AD42D98A}" name="Description" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{EBA22499-7DD5-405F-82CA-7058FFC1AB2F}" name="Commentaire" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}" name="Table134" displayName="Table134" ref="A9:D30" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A9:D30" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}" name="Table134" displayName="Table134" ref="A9:E30" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A9:E30" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{865D8B57-135B-4BFA-938D-B62BC39AC970}" name="Code"/>
-    <tableColumn id="2" xr3:uid="{E07D1CE2-997E-4A59-9869-D1EFB60F0809}" name="Libellé niveau 1" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{E07D1CE2-997E-4A59-9869-D1EFB60F0809}" name="Libellé niveau 1"/>
+    <tableColumn id="5" xr3:uid="{A8693491-C517-461F-B62C-F068AE507B25}" name="Libellé niveau 2"/>
     <tableColumn id="3" xr3:uid="{5BEB0E75-8B05-44A8-99B9-CB9CB8DD7E0C}" name="Description" dataDxfId="15"/>
     <tableColumn id="4" xr3:uid="{0C12ADAB-8B2E-4D44-B007-B1D25D7BAB07}" name="Commentaire" dataDxfId="14"/>
   </tableColumns>
@@ -7263,7 +7287,7 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -7448,7 +7472,7 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -7463,7 +7487,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1453</v>
+        <v>1311</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -7473,7 +7497,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1559</v>
+        <v>1503</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -7493,7 +7517,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1454</v>
+        <v>1504</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -7554,505 +7578,505 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="18" t="s">
-        <v>1455</v>
+        <v>1505</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>1455</v>
+        <v>1505</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="18" t="s">
-        <v>1523</v>
+        <v>1506</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="18" t="s">
-        <v>1456</v>
+        <v>1507</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18" t="s">
-        <v>1490</v>
+        <v>1508</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18" t="s">
-        <v>1524</v>
+        <v>1509</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="18" t="s">
-        <v>1457</v>
+        <v>1510</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18" t="s">
-        <v>1491</v>
+        <v>1511</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>1525</v>
+        <v>1512</v>
       </c>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="18" t="s">
-        <v>1458</v>
+        <v>1513</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18" t="s">
-        <v>1492</v>
+        <v>1514</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>1526</v>
+        <v>1515</v>
       </c>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="18" t="s">
-        <v>1459</v>
+        <v>1516</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18" t="s">
-        <v>1493</v>
+        <v>1517</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>1527</v>
+        <v>1518</v>
       </c>
       <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="18" t="s">
-        <v>1460</v>
+        <v>1519</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="s">
-        <v>1494</v>
+        <v>1520</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>1528</v>
+        <v>1521</v>
       </c>
       <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="18" t="s">
-        <v>1461</v>
+        <v>1522</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18" t="s">
-        <v>1495</v>
+        <v>1523</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>1529</v>
+        <v>1524</v>
       </c>
       <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="18" t="s">
-        <v>1462</v>
+        <v>1525</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
       <c r="D17" s="18" t="s">
-        <v>1496</v>
+        <v>1526</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>1530</v>
+        <v>1527</v>
       </c>
       <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="18" t="s">
-        <v>1463</v>
+        <v>1528</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18" t="s">
-        <v>1497</v>
+        <v>1529</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="18" t="s">
-        <v>1464</v>
+        <v>1531</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18" t="s">
-        <v>1498</v>
+        <v>1532</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="18" t="s">
-        <v>1465</v>
+        <v>1534</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="D20" s="18" t="s">
-        <v>1499</v>
+        <v>1535</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>1533</v>
+        <v>1536</v>
       </c>
       <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="18" t="s">
-        <v>1466</v>
+        <v>1537</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
       <c r="D21" s="18" t="s">
-        <v>1500</v>
+        <v>1538</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>1534</v>
+        <v>1539</v>
       </c>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="18" t="s">
-        <v>1467</v>
+        <v>1540</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18" t="s">
-        <v>1501</v>
+        <v>1541</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18" t="s">
-        <v>1535</v>
+        <v>1542</v>
       </c>
       <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="18" t="s">
-        <v>1468</v>
+        <v>1543</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18" t="s">
-        <v>1502</v>
+        <v>1544</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>1536</v>
+        <v>1545</v>
       </c>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="18" t="s">
-        <v>1469</v>
+        <v>1546</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
       <c r="D24" s="18" t="s">
-        <v>1503</v>
+        <v>1547</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>1537</v>
+        <v>1548</v>
       </c>
       <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="18" t="s">
-        <v>1470</v>
+        <v>1549</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18" t="s">
-        <v>1504</v>
+        <v>1550</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>1538</v>
+        <v>1551</v>
       </c>
       <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="18" t="s">
-        <v>1471</v>
+        <v>1552</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>1471</v>
+        <v>1552</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18" t="s">
-        <v>1539</v>
+        <v>1553</v>
       </c>
       <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="18" t="s">
-        <v>1472</v>
+        <v>1554</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="18" t="s">
-        <v>1505</v>
+        <v>1555</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18" t="s">
-        <v>1539</v>
+        <v>1553</v>
       </c>
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="18" t="s">
-        <v>1473</v>
+        <v>1556</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18" t="s">
-        <v>1506</v>
+        <v>1557</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>1540</v>
+        <v>1558</v>
       </c>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="18" t="s">
-        <v>1474</v>
+        <v>1559</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18" t="s">
-        <v>1507</v>
+        <v>1560</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>1541</v>
+        <v>1561</v>
       </c>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="18" t="s">
-        <v>1475</v>
+        <v>1562</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
       <c r="D30" s="18" t="s">
-        <v>1508</v>
+        <v>1563</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>1542</v>
+        <v>1564</v>
       </c>
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="18" t="s">
-        <v>1476</v>
+        <v>1565</v>
       </c>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
       <c r="D31" s="18" t="s">
-        <v>1509</v>
+        <v>1566</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>1543</v>
+        <v>1567</v>
       </c>
       <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="18" t="s">
-        <v>1477</v>
+        <v>1568</v>
       </c>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
       <c r="D32" s="18" t="s">
-        <v>1510</v>
+        <v>1569</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>1544</v>
+        <v>1570</v>
       </c>
       <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="18" t="s">
-        <v>1478</v>
+        <v>1571</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18" t="s">
-        <v>1511</v>
+        <v>1572</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>1545</v>
+        <v>1573</v>
       </c>
       <c r="F33" s="18"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="18" t="s">
-        <v>1479</v>
+        <v>1574</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18" t="s">
-        <v>1512</v>
+        <v>1575</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>1546</v>
+        <v>1576</v>
       </c>
       <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="18" t="s">
-        <v>1480</v>
+        <v>1577</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>1480</v>
+        <v>1577</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
       <c r="E35" s="18" t="s">
-        <v>1547</v>
+        <v>1578</v>
       </c>
       <c r="F35" s="18"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="18" t="s">
-        <v>1481</v>
+        <v>1579</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18" t="s">
-        <v>1513</v>
+        <v>1580</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18" t="s">
-        <v>1548</v>
+        <v>1581</v>
       </c>
       <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="18" t="s">
-        <v>1482</v>
+        <v>1582</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
       <c r="D37" s="18" t="s">
-        <v>1514</v>
+        <v>1583</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>1549</v>
+        <v>1584</v>
       </c>
       <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="18" t="s">
-        <v>1483</v>
+        <v>1585</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
       <c r="D38" s="18" t="s">
-        <v>1515</v>
+        <v>1586</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>1550</v>
+        <v>1587</v>
       </c>
       <c r="F38" s="18"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="18" t="s">
-        <v>1484</v>
+        <v>1588</v>
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
       <c r="D39" s="18" t="s">
-        <v>1516</v>
+        <v>1589</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>1551</v>
+        <v>1590</v>
       </c>
       <c r="F39" s="18"/>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="18" t="s">
-        <v>1485</v>
+        <v>1591</v>
       </c>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
       <c r="D40" s="18" t="s">
-        <v>1517</v>
+        <v>1592</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>1552</v>
+        <v>1593</v>
       </c>
       <c r="F40" s="18"/>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="18" t="s">
-        <v>1486</v>
+        <v>1594</v>
       </c>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
       <c r="D41" s="18" t="s">
-        <v>1518</v>
+        <v>1595</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>1553</v>
+        <v>1596</v>
       </c>
       <c r="F41" s="18"/>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="18" t="s">
-        <v>1487</v>
+        <v>1597</v>
       </c>
       <c r="B42" s="18"/>
       <c r="C42" s="18" t="s">
-        <v>1519</v>
+        <v>1598</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="18" t="s">
-        <v>1554</v>
+        <v>1599</v>
       </c>
       <c r="F42" s="18"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="18" t="s">
-        <v>1488</v>
+        <v>1600</v>
       </c>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
       <c r="D43" s="18" t="s">
-        <v>1520</v>
+        <v>1601</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>1555</v>
+        <v>1602</v>
       </c>
       <c r="F43" s="18"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="18" t="s">
-        <v>1489</v>
+        <v>1603</v>
       </c>
       <c r="B44" s="18"/>
       <c r="C44" s="18"/>
       <c r="D44" s="18" t="s">
-        <v>1521</v>
+        <v>1604</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>1556</v>
+        <v>1605</v>
       </c>
       <c r="F44" s="18"/>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="18" t="s">
-        <v>1313</v>
+        <v>1370</v>
       </c>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
       <c r="D45" s="18" t="s">
-        <v>1522</v>
+        <v>1606</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>1557</v>
+        <v>1607</v>
       </c>
       <c r="F45" s="18"/>
     </row>
@@ -8072,7 +8096,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -8087,7 +8111,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1453</v>
+        <v>1311</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -8097,7 +8121,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1653</v>
+        <v>1608</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8117,7 +8141,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1454</v>
+        <v>1504</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -8178,71 +8202,71 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>1643</v>
+        <v>1609</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>1648</v>
+        <v>1610</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="21" t="s">
-        <v>1654</v>
+        <v>1611</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>1644</v>
+        <v>1612</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>1649</v>
+        <v>1613</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="21" t="s">
-        <v>1655</v>
+        <v>1614</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>1645</v>
+        <v>1615</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>1650</v>
+        <v>1616</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="21" t="s">
-        <v>1656</v>
+        <v>1617</v>
       </c>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>1646</v>
+        <v>1618</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>1651</v>
+        <v>1619</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
       <c r="E13" s="21" t="s">
-        <v>1657</v>
+        <v>1620</v>
       </c>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="21" t="s">
-        <v>1647</v>
+        <v>1621</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>1652</v>
+        <v>1622</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="21" t="s">
-        <v>1658</v>
+        <v>1623</v>
       </c>
       <c r="F14" s="18"/>
     </row>
@@ -8510,7 +8534,7 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
@@ -8524,7 +8548,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1453</v>
+        <v>1311</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -8534,7 +8558,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1598</v>
+        <v>1624</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8554,7 +8578,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1454</v>
+        <v>1504</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -8615,46 +8639,46 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="20" t="s">
-        <v>1587</v>
+        <v>1625</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>1590</v>
+        <v>1626</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>1594</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="20" t="s">
-        <v>1588</v>
+        <v>1628</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>1591</v>
+        <v>1629</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>1595</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="20" t="s">
-        <v>1313</v>
+        <v>1370</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>1592</v>
+        <v>1631</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>1596</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="20" t="s">
-        <v>1589</v>
+        <v>1373</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>1593</v>
+        <v>1633</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>1597</v>
+        <v>1634</v>
       </c>
     </row>
   </sheetData>
@@ -8673,7 +8697,7 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -8688,7 +8712,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1453</v>
+        <v>1311</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -8698,7 +8722,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>1599</v>
+        <v>1635</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8718,7 +8742,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1454</v>
+        <v>1504</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -8779,57 +8803,57 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="18" t="s">
-        <v>1600</v>
+        <v>1636</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>1604</v>
+        <v>1637</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="20" t="s">
-        <v>1608</v>
+        <v>1638</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="18" t="s">
-        <v>1601</v>
+        <v>1639</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>1605</v>
+        <v>1640</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="20" t="s">
-        <v>1609</v>
+        <v>1641</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="18" t="s">
-        <v>1602</v>
+        <v>1642</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>1606</v>
+        <v>1643</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="20" t="s">
-        <v>1610</v>
+        <v>1644</v>
       </c>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="18" t="s">
-        <v>1603</v>
+        <v>1645</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>1607</v>
+        <v>1646</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
       <c r="E13" s="20" t="s">
-        <v>1611</v>
+        <v>1647</v>
       </c>
       <c r="F13" s="18"/>
     </row>
@@ -9105,7 +9129,7 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.5703125" customWidth="1"/>
@@ -9120,7 +9144,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1453</v>
+        <v>1311</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -9130,7 +9154,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1612</v>
+        <v>1648</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -9150,7 +9174,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1454</v>
+        <v>1504</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -9211,81 +9235,81 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="18" t="s">
-        <v>1613</v>
+        <v>1649</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>1617</v>
+        <v>1650</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>1618</v>
+        <v>1651</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18" t="s">
-        <v>1627</v>
+        <v>1652</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="18" t="s">
-        <v>1614</v>
+        <v>1653</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>1619</v>
+        <v>1654</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>1620</v>
+        <v>1655</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18" t="s">
-        <v>1628</v>
+        <v>1656</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="18" t="s">
-        <v>1615</v>
+        <v>1657</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>1621</v>
+        <v>1658</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>1622</v>
+        <v>1659</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18" t="s">
-        <v>1629</v>
+        <v>1660</v>
       </c>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="18" t="s">
-        <v>1616</v>
+        <v>1661</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>1623</v>
+        <v>1662</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>1624</v>
+        <v>1663</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18" t="s">
-        <v>1630</v>
+        <v>1664</v>
       </c>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="18" t="s">
-        <v>1632</v>
+        <v>1665</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>1625</v>
+        <v>1666</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>1626</v>
+        <v>1667</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18" t="s">
-        <v>1631</v>
+        <v>1668</v>
       </c>
       <c r="F14" s="18"/>
     </row>
@@ -9553,7 +9577,7 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -9567,7 +9591,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1453</v>
+        <v>1311</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -9577,7 +9601,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>1633</v>
+        <v>1669</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -9597,7 +9621,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1454</v>
+        <v>1504</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -9658,43 +9682,43 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="21" t="s">
-        <v>1634</v>
+        <v>1332</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>1637</v>
+        <v>1670</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="21" t="s">
-        <v>1640</v>
+        <v>1671</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="21" t="s">
-        <v>1635</v>
+        <v>1672</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>1638</v>
+        <v>1673</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="21" t="s">
-        <v>1641</v>
+        <v>1674</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="21" t="s">
-        <v>1636</v>
+        <v>1675</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>1639</v>
+        <v>1676</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="21" t="s">
-        <v>1642</v>
+        <v>1677</v>
       </c>
       <c r="F12" s="18"/>
     </row>
@@ -9975,7 +9999,7 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="33.28515625" customWidth="1"/>
@@ -13739,7 +13763,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -16458,7 +16482,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" style="10" customWidth="1"/>
@@ -16951,11 +16975,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8116353-BC00-4857-8D37-9470DD9A948C}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -17679,7 +17703,7 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -17835,79 +17859,88 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>1311</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>1312</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>1313</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7" s="6" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -17915,223 +17948,290 @@
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>1313</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:5" ht="30">
+      <c r="A10" s="18" t="s">
         <v>1314</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>1315</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="C10" s="18"/>
+      <c r="D10" s="19" t="s">
         <v>1316</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="17" t="s">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" ht="45">
+      <c r="A11" s="18" t="s">
         <v>1317</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B11" s="18" t="s">
         <v>1318</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="17" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="19" t="s">
         <v>1319</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" ht="30">
+      <c r="A12" s="18" t="s">
         <v>1320</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="17" t="s">
+      <c r="B12" s="18" t="s">
         <v>1321</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>1073</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="17" t="s">
+      <c r="C12" s="18"/>
+      <c r="D12" s="19" t="s">
         <v>1322</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" ht="30">
+      <c r="A13" s="18" t="s">
         <v>1323</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="17" t="s">
+      <c r="B13" s="18" t="s">
         <v>1324</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="19" t="s">
         <v>1325</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="17" t="s">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" ht="30">
+      <c r="A14" s="18" t="s">
         <v>1326</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B14" s="18" t="s">
         <v>1327</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="17" t="s">
+      <c r="C14" s="18"/>
+      <c r="D14" s="19" t="s">
         <v>1328</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" ht="45">
+      <c r="A15" s="18" t="s">
         <v>1329</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="17" t="s">
+      <c r="B15" s="18" t="s">
         <v>1330</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="C15" s="18"/>
+      <c r="D15" s="19" t="s">
         <v>1331</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="17" t="s">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="18" t="s">
         <v>1332</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B16" s="18" t="s">
         <v>1333</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="17" t="s">
+      <c r="C16" s="18"/>
+      <c r="D16" s="19" t="s">
         <v>1334</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" ht="30">
+      <c r="A17" s="18" t="s">
         <v>1335</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="17" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="18" t="s">
         <v>1336</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="D17" s="19" t="s">
         <v>1337</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="17" t="s">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" ht="45">
+      <c r="A18" s="18" t="s">
         <v>1338</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B18" s="18"/>
+      <c r="C18" s="18" t="s">
         <v>1339</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="17" t="s">
+      <c r="D18" s="19" t="s">
         <v>1340</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="60">
+      <c r="A19" s="18" t="s">
         <v>1341</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="17" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18" t="s">
         <v>1342</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="D19" s="19" t="s">
         <v>1343</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="17" t="s">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="45">
+      <c r="A20" s="18" t="s">
         <v>1344</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>1345</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="17" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="19" t="s">
         <v>1346</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" ht="30">
+      <c r="A21" s="18" t="s">
         <v>1347</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="17" t="s">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18" t="s">
         <v>1348</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="D21" s="19" t="s">
         <v>1349</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="17" t="s">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" ht="30">
+      <c r="A22" s="18" t="s">
         <v>1350</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18" t="s">
         <v>1351</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="17" t="s">
+      <c r="D22" s="19" t="s">
         <v>1352</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" ht="30">
+      <c r="A23" s="18" t="s">
         <v>1353</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>1355</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" ht="30">
+      <c r="A24" s="18" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>1358</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="18" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="19" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" ht="30">
+      <c r="A26" s="18" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="19" t="s">
+        <v>1364</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="18" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="19" t="s">
+        <v>1366</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="30">
+      <c r="A28" s="18" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="19" t="s">
+        <v>1369</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="18" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="18" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="19" t="s">
+        <v>1375</v>
+      </c>
+      <c r="E30" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -18147,10 +18247,10 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
@@ -18164,7 +18264,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1453</v>
+        <v>1311</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -18174,7 +18274,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1558</v>
+        <v>1376</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -18194,7 +18294,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1586</v>
+        <v>1377</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -18220,7 +18320,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>28</v>
+        <v>1081</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -18255,127 +18355,127 @@
     </row>
     <row r="10" spans="1:6" ht="30">
       <c r="A10" s="18" t="s">
-        <v>1560</v>
+        <v>1378</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>1568</v>
+        <v>1379</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="19" t="s">
-        <v>1577</v>
+        <v>1380</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="45">
       <c r="A11" s="18" t="s">
-        <v>1561</v>
+        <v>1381</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>1569</v>
+        <v>1382</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="19" t="s">
-        <v>1578</v>
+        <v>1383</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" ht="45">
       <c r="A12" s="18" t="s">
-        <v>1562</v>
+        <v>1384</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>1570</v>
+        <v>1385</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="19" t="s">
-        <v>1579</v>
+        <v>1386</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" ht="30">
       <c r="A13" s="18" t="s">
-        <v>1563</v>
+        <v>1387</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>1571</v>
+        <v>1388</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
       <c r="E13" s="19" t="s">
-        <v>1580</v>
+        <v>1389</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" ht="45">
       <c r="A14" s="18" t="s">
-        <v>1564</v>
+        <v>1390</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>1572</v>
+        <v>1391</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="19" t="s">
-        <v>1581</v>
+        <v>1392</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="30">
       <c r="A15" s="18" t="s">
-        <v>1565</v>
+        <v>1393</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>1573</v>
+        <v>1394</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="19" t="s">
-        <v>1582</v>
+        <v>1395</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="30">
       <c r="A16" s="18" t="s">
-        <v>1566</v>
+        <v>1396</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>1574</v>
+        <v>1397</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="19" t="s">
-        <v>1583</v>
+        <v>1398</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="45">
       <c r="A17" s="18" t="s">
-        <v>1313</v>
+        <v>1370</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>1575</v>
+        <v>1399</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="19" t="s">
-        <v>1584</v>
+        <v>1400</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="30">
       <c r="A18" s="18" t="s">
-        <v>1567</v>
+        <v>1401</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>1576</v>
+        <v>1402</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="19" t="s">
-        <v>1585</v>
+        <v>1403</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -18492,7 +18592,7 @@
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -18515,7 +18615,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1354</v>
+        <v>1404</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -18588,598 +18688,598 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>1355</v>
+        <v>1405</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1356</v>
+        <v>1406</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>1357</v>
+        <v>1407</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>1358</v>
+        <v>1408</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1356</v>
+        <v>1406</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>1359</v>
+        <v>1409</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>1360</v>
+        <v>1410</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1356</v>
+        <v>1406</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>1361</v>
+        <v>1411</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>1362</v>
+        <v>1412</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1356</v>
+        <v>1406</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>1363</v>
+        <v>1413</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>1364</v>
+        <v>1414</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1356</v>
+        <v>1406</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>1365</v>
+        <v>1415</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>1366</v>
+        <v>1416</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1356</v>
+        <v>1406</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>1367</v>
+        <v>1417</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>1368</v>
+        <v>1418</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1356</v>
+        <v>1406</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>1369</v>
+        <v>1419</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>1370</v>
+        <v>1420</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>1371</v>
+        <v>1421</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>1372</v>
+        <v>1422</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>1373</v>
+        <v>1423</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>1371</v>
+        <v>1421</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>1374</v>
+        <v>1424</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>1375</v>
+        <v>1425</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>1371</v>
+        <v>1421</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>1376</v>
+        <v>1426</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>1377</v>
+        <v>1427</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>1371</v>
+        <v>1421</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1378</v>
+        <v>1428</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>1379</v>
+        <v>1429</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1371</v>
+        <v>1421</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>1380</v>
+        <v>1430</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>1381</v>
+        <v>1431</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1382</v>
+        <v>1432</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>1383</v>
+        <v>1433</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>1384</v>
+        <v>1434</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>1382</v>
+        <v>1432</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>1385</v>
+        <v>1435</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>1386</v>
+        <v>1436</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>1382</v>
+        <v>1432</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>1387</v>
+        <v>1437</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>1388</v>
+        <v>1438</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>1382</v>
+        <v>1432</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>1389</v>
+        <v>1439</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>1390</v>
+        <v>1440</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>1382</v>
+        <v>1432</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>1391</v>
+        <v>1441</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>1392</v>
+        <v>1442</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>1393</v>
+        <v>1443</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>1394</v>
+        <v>1444</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>1395</v>
+        <v>1445</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>1393</v>
+        <v>1443</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>1396</v>
+        <v>1446</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>1397</v>
+        <v>1447</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>1393</v>
+        <v>1443</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>1398</v>
+        <v>1448</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>1399</v>
+        <v>1449</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>1393</v>
+        <v>1443</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>1401</v>
+        <v>1451</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>1393</v>
+        <v>1443</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>1402</v>
+        <v>1452</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>1403</v>
+        <v>1453</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>1393</v>
+        <v>1443</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>1404</v>
+        <v>1454</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>1405</v>
+        <v>1455</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>1393</v>
+        <v>1443</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>1406</v>
+        <v>1456</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>1407</v>
+        <v>1457</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>1393</v>
+        <v>1443</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>1408</v>
+        <v>1458</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>1409</v>
+        <v>1459</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>1393</v>
+        <v>1443</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>1410</v>
+        <v>1460</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>1411</v>
+        <v>1461</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>1393</v>
+        <v>1443</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>1412</v>
+        <v>1462</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>1413</v>
+        <v>1463</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>1393</v>
+        <v>1443</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>1414</v>
+        <v>1464</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>1415</v>
+        <v>1465</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>1416</v>
+        <v>1466</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>1417</v>
+        <v>1467</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>1418</v>
+        <v>1468</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>1416</v>
+        <v>1466</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>1419</v>
+        <v>1469</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>1420</v>
+        <v>1470</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>1416</v>
+        <v>1466</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>1421</v>
+        <v>1471</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>1422</v>
+        <v>1472</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>1416</v>
+        <v>1466</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>1423</v>
+        <v>1473</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>1424</v>
+        <v>1474</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>1416</v>
+        <v>1466</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>1425</v>
+        <v>1475</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>1426</v>
+        <v>1476</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>1416</v>
+        <v>1466</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>1427</v>
+        <v>1477</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>1428</v>
+        <v>1478</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>1416</v>
+        <v>1466</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>1429</v>
+        <v>1479</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>1430</v>
+        <v>1480</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>1416</v>
+        <v>1466</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>1431</v>
+        <v>1481</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>1432</v>
+        <v>1482</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>1433</v>
+        <v>1483</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>1434</v>
+        <v>1484</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>1435</v>
+        <v>1485</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>1433</v>
+        <v>1483</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>1436</v>
+        <v>1486</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>1437</v>
+        <v>1487</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>1433</v>
+        <v>1483</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>1438</v>
+        <v>1488</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
-        <v>1439</v>
+        <v>1489</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>1433</v>
+        <v>1483</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>1440</v>
+        <v>1490</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>1441</v>
+        <v>1491</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>1433</v>
+        <v>1483</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>1442</v>
+        <v>1492</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>1443</v>
+        <v>1493</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>1433</v>
+        <v>1483</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>1444</v>
+        <v>1494</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>1445</v>
+        <v>1495</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>1433</v>
+        <v>1483</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>1446</v>
+        <v>1496</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
-        <v>1447</v>
+        <v>1497</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>1433</v>
+        <v>1483</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>1448</v>
+        <v>1498</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>1449</v>
+        <v>1499</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>1450</v>
+        <v>1500</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>1451</v>
+        <v>1501</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
-        <v>1452</v>
+        <v>1502</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>1450</v>
+        <v>1500</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>1313</v>
+        <v>1370</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -19247,15 +19347,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19669,32 +19760,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70979E6C-A1C8-4023-9129-41BEA99BA961}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2196E6D3-62C5-4DBB-A481-E8ACEEDD134B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}"/>
 </file>
</xml_diff>

<commit_message>
[24.02.15 18:20] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="504" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7C56D4D-0218-4BE4-B173-289C4AA63644}"/>
+  <xr:revisionPtr revIDLastSave="506" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F3039F5-C7BB-4CFF-BDF0-736E53BDDFC7}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="705" windowWidth="25860" windowHeight="14580" firstSheet="13" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="705" windowWidth="25860" windowHeight="14580" firstSheet="6" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -3824,30 +3824,8 @@
     <t>Brûlure grave</t>
   </si>
   <si>
-    <r>
-      <t>Brûlure grave si localisation cervico-faciale et supérieure au 1er degré
-Brûlure de 3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> degré : La peau peut être cartonnée, blanche ou noire, insensible à la douleur</t>
-    </r>
+    <t>Brûlure grave si localisation cervico-faciale et supérieure au 1er degré
+Brûlure de 3e degré : La peau peut être cartonnée, blanche ou noire, insensible à la douleur</t>
   </si>
   <si>
     <t>M02.05</t>
@@ -3911,29 +3889,7 @@
     <t>Autre problème obstétrique non hémorragique</t>
   </si>
   <si>
-    <r>
-      <t>Yc. 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>er</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> trimestre de grossesse</t>
-    </r>
+    <t>Yc. 1er trimestre de grossesse</t>
   </si>
   <si>
     <t>M03.03</t>
@@ -5384,7 +5340,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5465,6 +5421,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -5515,7 +5477,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5563,6 +5525,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
@@ -16975,8 +16940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8116353-BC00-4857-8D37-9470DD9A948C}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -17161,7 +17126,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5" ht="70.5">
+    <row r="18" spans="1:5" ht="50.25">
       <c r="A18" s="2" t="s">
         <v>1190</v>
       </c>
@@ -17169,12 +17134,12 @@
       <c r="C18" s="2" t="s">
         <v>1191</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="23" t="s">
         <v>1192</v>
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" ht="77.25">
+    <row r="19" spans="1:5" ht="67.5">
       <c r="A19" s="2" t="s">
         <v>1193</v>
       </c>
@@ -17274,7 +17239,7 @@
       <c r="C27" s="2" t="s">
         <v>1212</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="23" t="s">
         <v>1213</v>
       </c>
       <c r="E27" s="12"/>
@@ -17861,7 +17826,7 @@
   </sheetPr>
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -19295,55 +19260,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19761,16 +19683,59 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19778,5 +19743,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}"/>
 </file>
</xml_diff>

<commit_message>
[24.02.28 11:46] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27421"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="506" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F3039F5-C7BB-4CFF-BDF0-736E53BDDFC7}"/>
+  <xr:revisionPtr revIDLastSave="507" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCD99FA6-95ED-41D9-AFB7-211DF93457BC}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="705" windowWidth="25860" windowHeight="14580" firstSheet="6" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="705" windowWidth="25860" windowHeight="14580" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -3961,26 +3961,7 @@
     <t>M03.08</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Signes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> d’AVC</t>
-    </r>
+    <t>Signes d’AVC</t>
   </si>
   <si>
     <t>AVC : accident vasculaire-cérébral</t>
@@ -5340,7 +5321,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5427,6 +5408,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -5477,7 +5464,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5528,6 +5515,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
@@ -9090,8 +9078,8 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -13724,8 +13712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3991FE2B-C9FE-43D1-B302-70CA3C5EF889}">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -16940,8 +16928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8116353-BC00-4857-8D37-9470DD9A948C}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -17301,12 +17289,12 @@
       </c>
       <c r="E32" s="12"/>
     </row>
-    <row r="33" spans="1:5" ht="26.25">
+    <row r="33" spans="1:5" ht="27">
       <c r="A33" s="2" t="s">
         <v>1225</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="24" t="s">
         <v>1226</v>
       </c>
       <c r="D33" s="12" t="s">
@@ -19269,6 +19257,58 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19682,66 +19722,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70979E6C-A1C8-4023-9129-41BEA99BA961}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70979E6C-A1C8-4023-9129-41BEA99BA961}"/>
 </file>
</xml_diff>

<commit_message>
[24.02.29 09:44] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27424"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="507" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCD99FA6-95ED-41D9-AFB7-211DF93457BC}"/>
+  <xr:revisionPtr revIDLastSave="521" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CDF8D87-92DB-4994-92C0-908F2E7E1DF1}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="705" windowWidth="25860" windowHeight="14580" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="705" windowWidth="25860" windowHeight="14580" firstSheet="13" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -8484,7 +8484,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -9078,7 +9078,7 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -9946,10 +9946,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24418BCA-6BA9-46F7-8F30-546B2F7203DE}">
-  <dimension ref="A1:F308"/>
+  <dimension ref="A1:F317"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -10096,10 +10096,11 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" ht="26.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" ht="27">
+      <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="C14" s="2"/>
       <c r="D14" t="s">
         <v>43</v>
       </c>
@@ -10162,10 +10163,11 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6" ht="27">
+      <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="C19" s="2"/>
       <c r="D19" t="s">
         <v>57</v>
       </c>
@@ -10231,10 +10233,10 @@
       <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E24" s="12"/>
@@ -10297,10 +10299,10 @@
       <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>86</v>
       </c>
       <c r="E29" s="12"/>
@@ -10359,9 +10361,10 @@
       <c r="F33" s="12"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>97</v>
       </c>
+      <c r="C34" s="2"/>
       <c r="D34" t="s">
         <v>98</v>
       </c>
@@ -10424,10 +10427,11 @@
       </c>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="1:6" ht="39">
-      <c r="A39" t="s">
+    <row r="39" spans="1:6" ht="40.5">
+      <c r="A39" s="2" t="s">
         <v>111</v>
       </c>
+      <c r="C39" s="2"/>
       <c r="D39" t="s">
         <v>112</v>
       </c>
@@ -10491,10 +10495,10 @@
       <c r="F43" s="12"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E44" s="12"/>
@@ -10551,9 +10555,10 @@
       <c r="F48" s="12"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="C49" s="2"/>
       <c r="D49" t="s">
         <v>137</v>
       </c>
@@ -10612,10 +10617,11 @@
       </c>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:6" ht="64.5">
-      <c r="A54" t="s">
+    <row r="54" spans="1:6" ht="67.5">
+      <c r="A54" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="C54" s="2"/>
       <c r="D54" t="s">
         <v>149</v>
       </c>
@@ -10673,9 +10679,10 @@
       <c r="F58" s="12"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" t="s">
+      <c r="A59" s="2" t="s">
         <v>159</v>
       </c>
+      <c r="C59" s="2"/>
       <c r="D59" t="s">
         <v>160</v>
       </c>
@@ -10731,10 +10738,11 @@
       <c r="F63" s="12"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" t="s">
+      <c r="A64" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D64" t="s">
+      <c r="C64" s="2"/>
+      <c r="D64" s="2" t="s">
         <v>170</v>
       </c>
       <c r="E64" s="12"/>
@@ -10789,10 +10797,10 @@
       <c r="F68" s="12"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" t="s">
+      <c r="A69" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="2" t="s">
         <v>180</v>
       </c>
       <c r="E69" s="12"/>
@@ -10853,10 +10861,10 @@
       <c r="F73" s="12"/>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" t="s">
+      <c r="A74" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="2" t="s">
         <v>193</v>
       </c>
       <c r="E74" s="12"/>
@@ -10911,10 +10919,11 @@
       <c r="F78" s="12"/>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" t="s">
+      <c r="A79" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D79" t="s">
+      <c r="C79" s="2"/>
+      <c r="D79" s="2" t="s">
         <v>203</v>
       </c>
       <c r="E79" s="12"/>
@@ -10969,10 +10978,11 @@
       <c r="F83" s="12"/>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" t="s">
+      <c r="A84" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D84" t="s">
+      <c r="C84" s="2"/>
+      <c r="D84" s="2" t="s">
         <v>213</v>
       </c>
       <c r="E84" s="12"/>
@@ -11030,11 +11040,12 @@
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
     </row>
-    <row r="89" spans="1:6" ht="51.75">
-      <c r="A89" t="s">
+    <row r="89" spans="1:6" ht="53.25">
+      <c r="A89" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D89" t="s">
+      <c r="C89" s="2"/>
+      <c r="D89" s="2" t="s">
         <v>223</v>
       </c>
       <c r="E89" s="12" t="s">
@@ -11097,10 +11108,11 @@
       <c r="F93" s="12"/>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" t="s">
+      <c r="A94" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D94" t="s">
+      <c r="C94" s="2"/>
+      <c r="D94" s="2" t="s">
         <v>234</v>
       </c>
       <c r="E94" s="12" t="s">
@@ -11157,12 +11169,13 @@
       <c r="F98" s="12"/>
     </row>
     <row r="99" spans="1:6">
-      <c r="A99" t="s">
+      <c r="A99" s="2" t="s">
         <v>244</v>
       </c>
       <c r="B99" t="s">
         <v>245</v>
       </c>
+      <c r="C99" s="2"/>
       <c r="E99" s="12"/>
       <c r="F99" s="12"/>
     </row>
@@ -11217,10 +11230,11 @@
       <c r="F103" s="12"/>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" t="s">
+      <c r="A104" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D104" t="s">
+      <c r="C104" s="2"/>
+      <c r="D104" s="2" t="s">
         <v>256</v>
       </c>
       <c r="E104" s="12"/>
@@ -11279,10 +11293,11 @@
       <c r="F108" s="12"/>
     </row>
     <row r="109" spans="1:6">
-      <c r="A109" t="s">
+      <c r="A109" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D109" t="s">
+      <c r="C109" s="2"/>
+      <c r="D109" s="2" t="s">
         <v>268</v>
       </c>
       <c r="E109" s="12"/>
@@ -11341,10 +11356,11 @@
       <c r="F113" s="12"/>
     </row>
     <row r="114" spans="1:6">
-      <c r="A114" t="s">
+      <c r="A114" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D114" t="s">
+      <c r="C114" s="2"/>
+      <c r="D114" s="2" t="s">
         <v>280</v>
       </c>
       <c r="E114" s="12"/>
@@ -11400,11 +11416,12 @@
         <v>289</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="26.25">
-      <c r="A119" t="s">
+    <row r="119" spans="1:6">
+      <c r="A119" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="D119" t="s">
+      <c r="C119" s="2"/>
+      <c r="D119" s="2" t="s">
         <v>291</v>
       </c>
       <c r="E119" s="12"/>
@@ -11465,10 +11482,11 @@
       <c r="F123" s="12"/>
     </row>
     <row r="124" spans="1:6">
-      <c r="A124" t="s">
+      <c r="A124" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D124" t="s">
+      <c r="C124" s="2"/>
+      <c r="D124" s="2" t="s">
         <v>304</v>
       </c>
       <c r="E124" s="12"/>
@@ -11525,10 +11543,10 @@
       <c r="F128" s="12"/>
     </row>
     <row r="129" spans="1:6">
-      <c r="A129" t="s">
+      <c r="A129" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="2" t="s">
         <v>315</v>
       </c>
       <c r="E129" s="12"/>
@@ -11585,10 +11603,10 @@
       <c r="F133" s="12"/>
     </row>
     <row r="134" spans="1:6">
-      <c r="A134" t="s">
+      <c r="A134" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="2" t="s">
         <v>326</v>
       </c>
       <c r="E134" s="12"/>
@@ -11644,13 +11662,14 @@
       <c r="E138" s="12"/>
       <c r="F138" s="12"/>
     </row>
-    <row r="139" spans="1:6" ht="26.25">
-      <c r="A139" t="s">
+    <row r="139" spans="1:6" ht="27">
+      <c r="A139" s="2" t="s">
         <v>336</v>
       </c>
       <c r="B139" t="s">
         <v>337</v>
       </c>
+      <c r="C139" s="2"/>
       <c r="E139" s="12" t="s">
         <v>338</v>
       </c>
@@ -11710,11 +11729,12 @@
       </c>
       <c r="F143" s="12"/>
     </row>
-    <row r="144" spans="1:6" ht="26.25">
-      <c r="A144" t="s">
+    <row r="144" spans="1:6" ht="27">
+      <c r="A144" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="D144" t="s">
+      <c r="C144" s="2"/>
+      <c r="D144" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E144" s="12" t="s">
@@ -11780,11 +11800,12 @@
       </c>
       <c r="F148" s="12"/>
     </row>
-    <row r="149" spans="1:6" ht="26.25">
-      <c r="A149" t="s">
+    <row r="149" spans="1:6" ht="27">
+      <c r="A149" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="D149" t="s">
+      <c r="C149" s="2"/>
+      <c r="D149" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E149" s="12" t="s">
@@ -11845,10 +11866,11 @@
       <c r="F153" s="12"/>
     </row>
     <row r="154" spans="1:6">
-      <c r="A154" t="s">
+      <c r="A154" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="D154" t="s">
+      <c r="C154" s="2"/>
+      <c r="D154" s="2" t="s">
         <v>358</v>
       </c>
       <c r="E154" s="12"/>
@@ -11903,12 +11925,13 @@
       <c r="F158" s="12"/>
     </row>
     <row r="159" spans="1:6">
-      <c r="A159" t="s">
+      <c r="A159" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="2" t="s">
         <v>368</v>
       </c>
+      <c r="D159" s="2"/>
       <c r="E159" s="12"/>
       <c r="F159" s="12"/>
     </row>
@@ -11964,11 +11987,12 @@
       </c>
       <c r="F163" s="12"/>
     </row>
-    <row r="164" spans="1:6" ht="39">
-      <c r="A164" t="s">
+    <row r="164" spans="1:6" ht="40.5">
+      <c r="A164" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="D164" t="s">
+      <c r="C164" s="2"/>
+      <c r="D164" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E164" s="12" t="s">
@@ -12029,12 +12053,13 @@
       <c r="F168" s="12"/>
     </row>
     <row r="169" spans="1:6">
-      <c r="A169" t="s">
+      <c r="A169" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C169" s="2" t="s">
         <v>392</v>
       </c>
+      <c r="D169" s="2"/>
       <c r="E169" s="12"/>
       <c r="F169" s="12"/>
     </row>
@@ -12087,12 +12112,14 @@
       <c r="F173" s="12"/>
     </row>
     <row r="174" spans="1:6">
-      <c r="A174" t="s">
+      <c r="A174" s="2" t="s">
         <v>401</v>
       </c>
       <c r="B174" t="s">
         <v>402</v>
       </c>
+      <c r="C174" s="2"/>
+      <c r="D174" s="2"/>
       <c r="E174" s="12"/>
       <c r="F174" s="12"/>
     </row>
@@ -12147,10 +12174,11 @@
       <c r="F178" s="12"/>
     </row>
     <row r="179" spans="1:6">
-      <c r="A179" t="s">
+      <c r="A179" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D179" t="s">
+      <c r="C179" s="2"/>
+      <c r="D179" s="2" t="s">
         <v>413</v>
       </c>
       <c r="E179" s="12"/>
@@ -12205,12 +12233,13 @@
       <c r="F183" s="12"/>
     </row>
     <row r="184" spans="1:6">
-      <c r="A184" t="s">
+      <c r="A184" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C184" s="2" t="s">
         <v>423</v>
       </c>
+      <c r="D184" s="2"/>
       <c r="E184" s="12"/>
       <c r="F184" s="12"/>
     </row>
@@ -12265,10 +12294,11 @@
       <c r="F188" s="12"/>
     </row>
     <row r="189" spans="1:6">
-      <c r="A189" t="s">
+      <c r="A189" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="D189" t="s">
+      <c r="C189" s="2"/>
+      <c r="D189" s="2" t="s">
         <v>434</v>
       </c>
       <c r="E189" s="12" t="s">
@@ -12325,10 +12355,11 @@
       <c r="F193" s="12"/>
     </row>
     <row r="194" spans="1:6">
-      <c r="A194" t="s">
+      <c r="A194" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="D194" t="s">
+      <c r="C194" s="2"/>
+      <c r="D194" s="2" t="s">
         <v>445</v>
       </c>
       <c r="E194" s="12"/>
@@ -12389,10 +12420,11 @@
       <c r="F198" s="12"/>
     </row>
     <row r="199" spans="1:6">
-      <c r="A199" t="s">
+      <c r="A199" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="D199" t="s">
+      <c r="C199" s="2"/>
+      <c r="D199" s="2" t="s">
         <v>458</v>
       </c>
       <c r="E199" s="12"/>
@@ -12449,10 +12481,11 @@
       <c r="F203" s="12"/>
     </row>
     <row r="204" spans="1:6">
-      <c r="A204" t="s">
+      <c r="A204" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="D204" t="s">
+      <c r="C204" s="2"/>
+      <c r="D204" s="2" t="s">
         <v>469</v>
       </c>
       <c r="E204" s="12"/>
@@ -12513,12 +12546,13 @@
       </c>
     </row>
     <row r="209" spans="1:6">
-      <c r="A209" t="s">
+      <c r="A209" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C209" s="2" t="s">
         <v>482</v>
       </c>
+      <c r="D209" s="2"/>
       <c r="E209" s="12"/>
       <c r="F209" s="12"/>
     </row>
@@ -12571,12 +12605,13 @@
       <c r="F213" s="12"/>
     </row>
     <row r="214" spans="1:6">
-      <c r="A214" t="s">
+      <c r="A214" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C214" s="2" t="s">
         <v>492</v>
       </c>
+      <c r="D214" s="2"/>
       <c r="E214" s="12"/>
       <c r="F214" s="12"/>
     </row>
@@ -12631,10 +12666,11 @@
       <c r="F218" s="12"/>
     </row>
     <row r="219" spans="1:6">
-      <c r="A219" t="s">
+      <c r="A219" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="D219" t="s">
+      <c r="C219" s="2"/>
+      <c r="D219" s="2" t="s">
         <v>503</v>
       </c>
       <c r="E219" s="12"/>
@@ -12689,10 +12725,11 @@
       <c r="F223" s="12"/>
     </row>
     <row r="224" spans="1:6">
-      <c r="A224" t="s">
+      <c r="A224" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="D224" t="s">
+      <c r="C224" s="2"/>
+      <c r="D224" s="2" t="s">
         <v>513</v>
       </c>
       <c r="E224" s="12"/>
@@ -12749,10 +12786,11 @@
       <c r="F228" s="12"/>
     </row>
     <row r="229" spans="1:6">
-      <c r="A229" t="s">
+      <c r="A229" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="D229" t="s">
+      <c r="C229" s="2"/>
+      <c r="D229" s="2" t="s">
         <v>524</v>
       </c>
       <c r="E229" s="12"/>
@@ -12807,12 +12845,13 @@
       <c r="F233" s="12"/>
     </row>
     <row r="234" spans="1:6">
-      <c r="A234" t="s">
+      <c r="A234" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="C234" t="s">
+      <c r="C234" s="2" t="s">
         <v>534</v>
       </c>
+      <c r="D234" s="2"/>
       <c r="E234" s="12"/>
       <c r="F234" s="12"/>
     </row>
@@ -12867,10 +12906,11 @@
       <c r="F238" s="12"/>
     </row>
     <row r="239" spans="1:6">
-      <c r="A239" t="s">
+      <c r="A239" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="D239" t="s">
+      <c r="C239" s="2"/>
+      <c r="D239" s="2" t="s">
         <v>545</v>
       </c>
       <c r="E239" s="12"/>
@@ -12927,12 +12967,13 @@
       <c r="F243" s="12"/>
     </row>
     <row r="244" spans="1:6">
-      <c r="A244" t="s">
+      <c r="A244" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="C244" t="s">
+      <c r="C244" s="2" t="s">
         <v>556</v>
       </c>
+      <c r="D244" s="2"/>
       <c r="E244" s="12"/>
       <c r="F244" s="12"/>
     </row>
@@ -12985,12 +13026,13 @@
       <c r="F248" s="12"/>
     </row>
     <row r="249" spans="1:6">
-      <c r="A249" t="s">
+      <c r="A249" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="C249" t="s">
+      <c r="C249" s="2" t="s">
         <v>566</v>
       </c>
+      <c r="D249" s="2"/>
       <c r="E249" s="12"/>
       <c r="F249" s="12" t="s">
         <v>567</v>
@@ -13045,12 +13087,13 @@
       <c r="F253" s="12"/>
     </row>
     <row r="254" spans="1:6">
-      <c r="A254" t="s">
+      <c r="A254" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="C254" t="s">
+      <c r="C254" s="2" t="s">
         <v>577</v>
       </c>
+      <c r="D254" s="2"/>
       <c r="E254" s="12"/>
       <c r="F254" s="12"/>
     </row>
@@ -13103,10 +13146,11 @@
       <c r="F258" s="12"/>
     </row>
     <row r="259" spans="1:6">
-      <c r="A259" t="s">
+      <c r="A259" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="D259" t="s">
+      <c r="C259" s="2"/>
+      <c r="D259" s="2" t="s">
         <v>587</v>
       </c>
       <c r="E259" s="12"/>
@@ -13161,10 +13205,11 @@
       <c r="F263" s="12"/>
     </row>
     <row r="264" spans="1:6">
-      <c r="A264" t="s">
+      <c r="A264" s="2" t="s">
         <v>596</v>
       </c>
-      <c r="D264" t="s">
+      <c r="C264" s="2"/>
+      <c r="D264" s="2" t="s">
         <v>597</v>
       </c>
       <c r="E264" s="12"/>
@@ -13219,12 +13264,13 @@
       <c r="F268" s="12"/>
     </row>
     <row r="269" spans="1:6">
-      <c r="A269" t="s">
+      <c r="A269" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="C269" t="s">
+      <c r="C269" s="2" t="s">
         <v>607</v>
       </c>
+      <c r="D269" s="2"/>
       <c r="E269" s="12"/>
       <c r="F269" s="12"/>
     </row>
@@ -13277,10 +13323,11 @@
       <c r="F273" s="12"/>
     </row>
     <row r="274" spans="1:6">
-      <c r="A274" t="s">
+      <c r="A274" s="2" t="s">
         <v>616</v>
       </c>
-      <c r="D274" t="s">
+      <c r="C274" s="2"/>
+      <c r="D274" s="2" t="s">
         <v>617</v>
       </c>
       <c r="E274" s="12" t="s">
@@ -13341,10 +13388,11 @@
       <c r="F278" s="12"/>
     </row>
     <row r="279" spans="1:6">
-      <c r="A279" t="s">
+      <c r="A279" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="D279" t="s">
+      <c r="C279" s="2"/>
+      <c r="D279" s="2" t="s">
         <v>630</v>
       </c>
       <c r="E279" s="12"/>
@@ -13402,11 +13450,12 @@
       </c>
       <c r="F283" s="12"/>
     </row>
-    <row r="284" spans="1:6" ht="26.25">
-      <c r="A284" t="s">
+    <row r="284" spans="1:6" ht="27">
+      <c r="A284" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="D284" t="s">
+      <c r="C284" s="2"/>
+      <c r="D284" s="2" t="s">
         <v>642</v>
       </c>
       <c r="E284" s="12" t="s">
@@ -13467,10 +13516,11 @@
       <c r="F288" s="12"/>
     </row>
     <row r="289" spans="1:6">
-      <c r="A289" t="s">
+      <c r="A289" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="D289" t="s">
+      <c r="C289" s="2"/>
+      <c r="D289" s="2" t="s">
         <v>655</v>
       </c>
       <c r="E289" s="12"/>
@@ -13525,12 +13575,13 @@
       <c r="F293" s="12"/>
     </row>
     <row r="294" spans="1:6">
-      <c r="A294" t="s">
+      <c r="A294" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="C294" t="s">
+      <c r="C294" s="2" t="s">
         <v>665</v>
       </c>
+      <c r="D294" s="2"/>
       <c r="E294" s="12"/>
       <c r="F294" s="12"/>
     </row>
@@ -13585,10 +13636,11 @@
       <c r="F298" s="12"/>
     </row>
     <row r="299" spans="1:6">
-      <c r="A299" t="s">
+      <c r="A299" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="D299" t="s">
+      <c r="C299" s="2"/>
+      <c r="D299" s="2" t="s">
         <v>676</v>
       </c>
       <c r="E299" s="12"/>
@@ -13643,12 +13695,13 @@
       <c r="F303" s="12"/>
     </row>
     <row r="304" spans="1:6">
-      <c r="A304" t="s">
+      <c r="A304" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="C304" t="s">
+      <c r="C304" s="2" t="s">
         <v>686</v>
       </c>
+      <c r="D304" s="2"/>
       <c r="E304" s="12"/>
       <c r="F304" s="12"/>
     </row>
@@ -13699,6 +13752,33 @@
       <c r="D308" s="2"/>
       <c r="E308" s="12"/>
       <c r="F308" s="12"/>
+    </row>
+    <row r="309" spans="1:6">
+      <c r="C309" s="2"/>
+    </row>
+    <row r="310" spans="1:6">
+      <c r="C310" s="2"/>
+    </row>
+    <row r="311" spans="1:6">
+      <c r="C311" s="2"/>
+    </row>
+    <row r="312" spans="1:6">
+      <c r="C312" s="2"/>
+    </row>
+    <row r="313" spans="1:6">
+      <c r="C313" s="2"/>
+    </row>
+    <row r="314" spans="1:6">
+      <c r="C314" s="2"/>
+    </row>
+    <row r="315" spans="1:6">
+      <c r="C315" s="2"/>
+    </row>
+    <row r="316" spans="1:6">
+      <c r="C316" s="2"/>
+    </row>
+    <row r="317" spans="1:6">
+      <c r="C317" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13712,8 +13792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3991FE2B-C9FE-43D1-B302-70CA3C5EF889}">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -16929,7 +17009,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -17815,7 +17895,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -19248,15 +19328,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -19306,6 +19377,15 @@
     </l0a6b4600f484920bbceae0813174244>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19723,11 +19803,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
[24.03.11 09:43] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27424"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="521" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CDF8D87-92DB-4994-92C0-908F2E7E1DF1}"/>
+  <xr:revisionPtr revIDLastSave="525" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEB3D976-59F3-47AE-A60A-F8489393F03A}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="705" windowWidth="25860" windowHeight="14580" firstSheet="13" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8025" yWindow="0" windowWidth="20820" windowHeight="14130" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -3922,42 +3922,6 @@
     <t>Problème neurologique hors AVC, épilepsie</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Dont </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>convulsions persistantes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AVC : accident vasculaire-cérébral</t>
-    </r>
-  </si>
-  <si>
     <t>M03.08</t>
   </si>
   <si>
@@ -5315,13 +5279,17 @@
   </si>
   <si>
     <t>L'équipage du vecteur ne comporte que des secouristes professionnnels ni médecin, ni infimier</t>
+  </si>
+  <si>
+    <t>Dont convulsions persistantes
+AVC : accident vasculaire-cérébral</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5406,12 +5374,7 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -5464,7 +5427,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5515,7 +5478,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
@@ -7240,7 +7202,7 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -7425,7 +7387,7 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -7440,7 +7402,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -7450,7 +7412,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -7470,7 +7432,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -7531,505 +7493,505 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="18" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="18" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="18" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="18" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18" t="s">
+        <v>1510</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>1511</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>1512</v>
       </c>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="18" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18" t="s">
+        <v>1513</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>1514</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>1515</v>
       </c>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="18" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18" t="s">
+        <v>1516</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>1517</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>1518</v>
       </c>
       <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="18" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="s">
+        <v>1519</v>
+      </c>
+      <c r="E15" s="18" t="s">
         <v>1520</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>1521</v>
       </c>
       <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="18" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18" t="s">
+        <v>1522</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>1523</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>1524</v>
       </c>
       <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="18" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
       <c r="D17" s="18" t="s">
+        <v>1525</v>
+      </c>
+      <c r="E17" s="18" t="s">
         <v>1526</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>1527</v>
       </c>
       <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="18" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18" t="s">
+        <v>1528</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>1529</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>1530</v>
       </c>
       <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="18" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18" t="s">
+        <v>1531</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>1532</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>1533</v>
       </c>
       <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="18" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="D20" s="18" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>1535</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>1536</v>
       </c>
       <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="18" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
       <c r="D21" s="18" t="s">
+        <v>1537</v>
+      </c>
+      <c r="E21" s="18" t="s">
         <v>1538</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>1539</v>
       </c>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="18" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="18" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E23" s="18" t="s">
         <v>1544</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>1545</v>
       </c>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="18" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
       <c r="D24" s="18" t="s">
+        <v>1546</v>
+      </c>
+      <c r="E24" s="18" t="s">
         <v>1547</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>1548</v>
       </c>
       <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="18" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18" t="s">
+        <v>1549</v>
+      </c>
+      <c r="E25" s="18" t="s">
         <v>1550</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>1551</v>
       </c>
       <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="18" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="18" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="18" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="18" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18" t="s">
+        <v>1556</v>
+      </c>
+      <c r="E28" s="18" t="s">
         <v>1557</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>1558</v>
       </c>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="18" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18" t="s">
+        <v>1559</v>
+      </c>
+      <c r="E29" s="18" t="s">
         <v>1560</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>1561</v>
       </c>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="18" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
       <c r="D30" s="18" t="s">
+        <v>1562</v>
+      </c>
+      <c r="E30" s="18" t="s">
         <v>1563</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>1564</v>
       </c>
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="18" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
       <c r="D31" s="18" t="s">
+        <v>1565</v>
+      </c>
+      <c r="E31" s="18" t="s">
         <v>1566</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>1567</v>
       </c>
       <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="18" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
       <c r="D32" s="18" t="s">
+        <v>1568</v>
+      </c>
+      <c r="E32" s="18" t="s">
         <v>1569</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>1570</v>
       </c>
       <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="18" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18" t="s">
+        <v>1571</v>
+      </c>
+      <c r="E33" s="18" t="s">
         <v>1572</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>1573</v>
       </c>
       <c r="F33" s="18"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="18" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18" t="s">
+        <v>1574</v>
+      </c>
+      <c r="E34" s="18" t="s">
         <v>1575</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>1576</v>
       </c>
       <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="18" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
       <c r="E35" s="18" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="F35" s="18"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="18" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="18" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
       <c r="D37" s="18" t="s">
+        <v>1582</v>
+      </c>
+      <c r="E37" s="18" t="s">
         <v>1583</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>1584</v>
       </c>
       <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="18" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
       <c r="D38" s="18" t="s">
+        <v>1585</v>
+      </c>
+      <c r="E38" s="18" t="s">
         <v>1586</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>1587</v>
       </c>
       <c r="F38" s="18"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="18" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
       <c r="D39" s="18" t="s">
+        <v>1588</v>
+      </c>
+      <c r="E39" s="18" t="s">
         <v>1589</v>
-      </c>
-      <c r="E39" s="18" t="s">
-        <v>1590</v>
       </c>
       <c r="F39" s="18"/>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="18" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
       <c r="D40" s="18" t="s">
+        <v>1591</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>1592</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>1593</v>
       </c>
       <c r="F40" s="18"/>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="18" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
       <c r="D41" s="18" t="s">
+        <v>1594</v>
+      </c>
+      <c r="E41" s="18" t="s">
         <v>1595</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>1596</v>
       </c>
       <c r="F41" s="18"/>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="18" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="B42" s="18"/>
       <c r="C42" s="18" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="18" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="F42" s="18"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="18" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
       <c r="D43" s="18" t="s">
+        <v>1600</v>
+      </c>
+      <c r="E43" s="18" t="s">
         <v>1601</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>1602</v>
       </c>
       <c r="F43" s="18"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="18" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="B44" s="18"/>
       <c r="C44" s="18"/>
       <c r="D44" s="18" t="s">
+        <v>1603</v>
+      </c>
+      <c r="E44" s="18" t="s">
         <v>1604</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>1605</v>
       </c>
       <c r="F44" s="18"/>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="18" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
       <c r="D45" s="18" t="s">
+        <v>1605</v>
+      </c>
+      <c r="E45" s="18" t="s">
         <v>1606</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>1607</v>
       </c>
       <c r="F45" s="18"/>
     </row>
@@ -8049,7 +8011,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -8064,7 +8026,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -8074,7 +8036,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8094,7 +8056,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -8155,71 +8117,71 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>1609</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>1610</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="21" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>1611</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>1612</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>1613</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="21" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>1615</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>1616</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="21" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>1618</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>1619</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
       <c r="E13" s="21" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="21" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>1621</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>1622</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="21" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="F14" s="18"/>
     </row>
@@ -8487,7 +8449,7 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
@@ -8501,7 +8463,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -8511,7 +8473,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8531,7 +8493,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -8592,46 +8554,46 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="20" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>1625</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="E10" s="20" t="s">
         <v>1626</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>1627</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="20" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>1628</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="E11" s="20" t="s">
         <v>1629</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>1630</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="20" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="B12" s="20" t="s">
+        <v>1630</v>
+      </c>
+      <c r="E12" s="20" t="s">
         <v>1631</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>1632</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="20" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E13" s="20" t="s">
         <v>1633</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>1634</v>
       </c>
     </row>
   </sheetData>
@@ -8650,7 +8612,7 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -8665,7 +8627,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -8675,7 +8637,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8695,7 +8657,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -8756,57 +8718,57 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="18" t="s">
+        <v>1635</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>1636</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>1637</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="20" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="18" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>1639</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>1640</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="20" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="18" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>1642</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>1643</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="20" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="18" t="s">
+        <v>1644</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>1645</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>1646</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
       <c r="E13" s="20" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="F13" s="18"/>
     </row>
@@ -9082,7 +9044,7 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.5703125" customWidth="1"/>
@@ -9097,7 +9059,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -9107,7 +9069,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -9127,7 +9089,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -9188,81 +9150,81 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="18" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>1649</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="C10" s="18" t="s">
         <v>1650</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>1651</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="18" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>1653</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="C11" s="18" t="s">
         <v>1654</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>1655</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="18" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>1657</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="C12" s="18" t="s">
         <v>1658</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>1659</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="18" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>1661</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="C13" s="18" t="s">
         <v>1662</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>1663</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="18" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>1665</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="C14" s="18" t="s">
         <v>1666</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>1667</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="F14" s="18"/>
     </row>
@@ -9530,7 +9492,7 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -9544,7 +9506,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -9554,7 +9516,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -9574,7 +9536,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -9635,43 +9597,43 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="21" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="21" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="21" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>1672</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>1673</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="21" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="21" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>1675</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>1676</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="21" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="F12" s="18"/>
     </row>
@@ -9948,11 +9910,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24418BCA-6BA9-46F7-8F30-546B2F7203DE}">
   <dimension ref="A1:F317"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="33.28515625" customWidth="1"/>
@@ -10096,7 +10058,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" ht="27">
+    <row r="14" spans="1:6" ht="26.25">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -10163,7 +10125,7 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="27">
+    <row r="19" spans="1:6" ht="26.25">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -10427,7 +10389,7 @@
       </c>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="1:6" ht="40.5">
+    <row r="39" spans="1:6" ht="39">
       <c r="A39" s="2" t="s">
         <v>111</v>
       </c>
@@ -10617,7 +10579,7 @@
       </c>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:6" ht="67.5">
+    <row r="54" spans="1:6" ht="64.5">
       <c r="A54" s="2" t="s">
         <v>148</v>
       </c>
@@ -11040,7 +11002,7 @@
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
     </row>
-    <row r="89" spans="1:6" ht="53.25">
+    <row r="89" spans="1:6" ht="51.75">
       <c r="A89" s="2" t="s">
         <v>212</v>
       </c>
@@ -11416,7 +11378,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" ht="26.25">
       <c r="A119" s="2" t="s">
         <v>290</v>
       </c>
@@ -11662,7 +11624,7 @@
       <c r="E138" s="12"/>
       <c r="F138" s="12"/>
     </row>
-    <row r="139" spans="1:6" ht="27">
+    <row r="139" spans="1:6" ht="26.25">
       <c r="A139" s="2" t="s">
         <v>336</v>
       </c>
@@ -11729,7 +11691,7 @@
       </c>
       <c r="F143" s="12"/>
     </row>
-    <row r="144" spans="1:6" ht="27">
+    <row r="144" spans="1:6" ht="26.25">
       <c r="A144" s="2" t="s">
         <v>344</v>
       </c>
@@ -11800,7 +11762,7 @@
       </c>
       <c r="F148" s="12"/>
     </row>
-    <row r="149" spans="1:6" ht="27">
+    <row r="149" spans="1:6" ht="26.25">
       <c r="A149" s="2" t="s">
         <v>350</v>
       </c>
@@ -11987,7 +11949,7 @@
       </c>
       <c r="F163" s="12"/>
     </row>
-    <row r="164" spans="1:6" ht="40.5">
+    <row r="164" spans="1:6" ht="39">
       <c r="A164" s="2" t="s">
         <v>379</v>
       </c>
@@ -13450,7 +13412,7 @@
       </c>
       <c r="F283" s="12"/>
     </row>
-    <row r="284" spans="1:6" ht="27">
+    <row r="284" spans="1:6" ht="26.25">
       <c r="A284" s="2" t="s">
         <v>641</v>
       </c>
@@ -13792,11 +13754,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3991FE2B-C9FE-43D1-B302-70CA3C5EF889}">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -16515,7 +16477,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" style="10" customWidth="1"/>
@@ -17008,11 +16970,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8116353-BC00-4857-8D37-9470DD9A948C}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -17194,7 +17156,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5" ht="50.25">
+    <row r="18" spans="1:5" ht="60.75">
       <c r="A18" s="2" t="s">
         <v>1190</v>
       </c>
@@ -17207,7 +17169,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" ht="67.5">
+    <row r="19" spans="1:5" ht="77.25">
       <c r="A19" s="2" t="s">
         <v>1193</v>
       </c>
@@ -17356,7 +17318,7 @@
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:5" ht="30">
+    <row r="32" spans="1:5" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>1222</v>
       </c>
@@ -17365,137 +17327,137 @@
         <v>1223</v>
       </c>
       <c r="D32" s="12" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E32" s="12"/>
+    </row>
+    <row r="33" spans="1:5" ht="26.25">
+      <c r="A33" s="2" t="s">
         <v>1224</v>
       </c>
-      <c r="E32" s="12"/>
-    </row>
-    <row r="33" spans="1:5" ht="27">
-      <c r="A33" s="2" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
         <v>1225</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="24" t="s">
+      <c r="D33" s="2" t="s">
         <v>1226</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="E33" s="12" t="s">
         <v>1227</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>1228</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>1230</v>
-      </c>
-      <c r="D34" s="12"/>
+        <v>1229</v>
+      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="12"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>1232</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>1233</v>
       </c>
       <c r="E35" s="12"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="12"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2" t="s">
         <v>1235</v>
-      </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-    </row>
-    <row r="37" spans="1:5" ht="26.25">
-      <c r="A37" s="2" t="s">
-        <v>1236</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>1237</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="E37" s="12"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
         <v>1238</v>
-      </c>
-      <c r="E37" s="12"/>
-    </row>
-    <row r="38" spans="1:5" ht="26.25">
-      <c r="A38" s="2" t="s">
-        <v>1239</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>1240</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>1241</v>
       </c>
       <c r="E38" s="12"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
     </row>
     <row r="40" spans="1:5" ht="51.75">
       <c r="A40" s="2" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="12" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D41" s="12" t="s">
         <v>1248</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>1249</v>
       </c>
       <c r="E41" s="12"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
     </row>
     <row r="43" spans="1:5" ht="26.25">
       <c r="A43" s="2" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
@@ -17508,58 +17470,58 @@
     </row>
     <row r="44" spans="1:5" ht="39">
       <c r="A44" s="2" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D44" s="12" t="s">
         <v>1254</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>1255</v>
       </c>
       <c r="E44" s="12"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D46" s="12" t="s">
         <v>1259</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>1260</v>
       </c>
       <c r="E46" s="12"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>1263</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>1264</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="12"/>
@@ -17567,58 +17529,58 @@
     </row>
     <row r="49" spans="1:5" ht="26.25">
       <c r="A49" s="2" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D49" s="12" t="s">
         <v>1266</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>1267</v>
       </c>
       <c r="E49" s="12"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
     </row>
     <row r="52" spans="1:5" ht="26.25">
       <c r="A52" s="2" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="D52" s="12"/>
       <c r="E52" s="12" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>1275</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>1276</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="12"/>
@@ -17626,34 +17588,34 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D55" s="12" t="s">
         <v>1280</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>1281</v>
       </c>
       <c r="E55" s="12"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>1282</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>1283</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="12"/>
@@ -17661,63 +17623,63 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="2" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D59" s="12" t="s">
         <v>1289</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>1290</v>
       </c>
       <c r="E59" s="12"/>
     </row>
     <row r="60" spans="1:5" ht="51.75">
       <c r="A60" s="2" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D60" s="12" t="s">
         <v>1292</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>1293</v>
       </c>
       <c r="E60" s="12"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="2" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>1294</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>1295</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="12"/>
       <c r="E61" s="12" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
   </sheetData>
@@ -17736,7 +17698,7 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -17757,7 +17719,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -17820,61 +17782,61 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>1302</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>1303</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>1304</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>1305</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>1306</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>1307</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>1308</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>1309</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>1310</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -17895,10 +17857,10 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
@@ -17912,7 +17874,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C1" s="3"/>
     </row>
@@ -17921,7 +17883,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -17939,7 +17901,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -17992,274 +17954,274 @@
     </row>
     <row r="10" spans="1:5" ht="30">
       <c r="A10" s="18" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>1314</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>1315</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="19" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="45">
       <c r="A11" s="18" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>1317</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>1318</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="19" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="30">
       <c r="A12" s="18" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>1320</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>1321</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="19" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="30">
       <c r="A13" s="18" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>1323</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>1324</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="19" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="30">
       <c r="A14" s="18" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>1326</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>1327</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="19" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="45">
       <c r="A15" s="18" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>1329</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>1330</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="19" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="30">
       <c r="A16" s="18" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>1332</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>1333</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="19" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="30">
       <c r="A17" s="18" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18" t="s">
+        <v>1335</v>
+      </c>
+      <c r="D17" s="19" t="s">
         <v>1336</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>1337</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" ht="45">
       <c r="A18" s="18" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="18" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>1339</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>1340</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="60">
       <c r="A19" s="18" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="18" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>1342</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>1343</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="45">
       <c r="A20" s="18" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>1344</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>1345</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="19" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="30">
       <c r="A21" s="18" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="18" t="s">
+        <v>1347</v>
+      </c>
+      <c r="D21" s="19" t="s">
         <v>1348</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>1349</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="30">
       <c r="A22" s="18" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D22" s="19" t="s">
         <v>1351</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>1352</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" ht="30">
       <c r="A23" s="18" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="18" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D23" s="19" t="s">
         <v>1354</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>1355</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" ht="30">
       <c r="A24" s="18" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D24" s="19" t="s">
         <v>1357</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>1358</v>
       </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="30">
       <c r="A25" s="18" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>1359</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>1360</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="19" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" ht="30">
       <c r="A26" s="18" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>1362</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>1363</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="19" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="19" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="30">
       <c r="A28" s="18" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>1367</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>1368</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="19" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="18" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B29" s="18" t="s">
         <v>1370</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>1371</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="19" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B30" s="18" t="s">
         <v>1373</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>1374</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="19" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="E30" s="2"/>
     </row>
@@ -18283,7 +18245,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
@@ -18297,7 +18259,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -18307,7 +18269,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -18327,7 +18289,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -18388,127 +18350,127 @@
     </row>
     <row r="10" spans="1:6" ht="30">
       <c r="A10" s="18" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>1378</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>1379</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="19" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="45">
       <c r="A11" s="18" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>1381</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>1382</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="19" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" ht="45">
       <c r="A12" s="18" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>1384</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>1385</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="19" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" ht="30">
       <c r="A13" s="18" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>1387</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>1388</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
       <c r="E13" s="19" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" ht="45">
       <c r="A14" s="18" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>1390</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>1391</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="19" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="30">
       <c r="A15" s="18" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>1393</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>1394</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="19" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="30">
       <c r="A16" s="18" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>1396</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>1397</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="19" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="45">
       <c r="A17" s="18" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="19" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="30">
       <c r="A18" s="18" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>1401</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>1402</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="19" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -18621,11 +18583,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3700FB-CD0A-4D38-965B-161A1B9D93F3}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -18648,7 +18610,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -18721,598 +18683,598 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>1405</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>1406</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>1407</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>1408</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>1409</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>1410</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>1411</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>1412</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>1413</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>1414</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>1415</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>1416</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>1417</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>1418</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>1419</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>1420</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>1421</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>1422</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>1423</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>1421</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>1424</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>1425</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>1421</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>1426</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>1427</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>1421</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>1428</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>1429</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1421</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>1430</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>1431</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>1432</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>1433</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>1434</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>1432</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>1435</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>1436</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>1432</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>1437</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>1438</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>1432</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>1439</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>1440</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>1432</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>1441</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>1442</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>1443</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>1444</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>1445</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>1443</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>1446</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>1447</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>1443</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>1448</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>1449</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>1443</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>1450</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>1451</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>1443</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>1452</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>1453</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>1443</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>1454</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>1455</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>1443</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>1456</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>1457</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>1443</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>1458</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
+        <v>1458</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>1459</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>1443</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>1460</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>1461</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>1443</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>1462</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>1463</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>1443</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>1464</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>1465</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>1466</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>1467</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>1468</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>1469</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
+        <v>1469</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>1470</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>1471</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>1472</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>1473</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>1474</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>1475</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>1476</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>1477</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>1478</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>1479</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>1480</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>1481</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>1482</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>1483</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>1484</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>1485</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>1483</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>1486</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>1487</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>1483</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>1488</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>1489</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>1483</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>1490</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>1491</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>1483</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>1492</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>1493</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>1483</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>1494</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>1495</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>1483</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>1496</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>1497</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>1483</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>1498</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>1499</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>1500</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>1501</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -19328,58 +19290,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -19388,7 +19298,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19802,14 +19712,100 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70979E6C-A1C8-4023-9129-41BEA99BA961}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70979E6C-A1C8-4023-9129-41BEA99BA961}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.03.25 11:34] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="528" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0895C31B-DAAD-45B5-A914-7551A6D34ABB}"/>
+  <xr:revisionPtr revIDLastSave="557" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C34E23FC-B63B-4C12-BFBA-A09E0F8D99D8}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="25305" windowHeight="13920" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="615" yWindow="765" windowWidth="28860" windowHeight="13665" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -28,6 +28,9 @@
     <sheet name="Niveau de soin" sheetId="29" r:id="rId13"/>
     <sheet name="Type de décision" sheetId="30" r:id="rId14"/>
     <sheet name="Niveau de médicalisation" sheetId="31" r:id="rId15"/>
+    <sheet name="Etat du dossier" sheetId="34" r:id="rId16"/>
+    <sheet name="Orientation" sheetId="35" r:id="rId17"/>
+    <sheet name="Type de ressource-transport" sheetId="36" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -50,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2034" uniqueCount="1678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="1722">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -5284,12 +5287,204 @@
   <si>
     <t>L'équipage du vecteur ne comporte que des secouristes professionnnels ni médecin, ni infimier</t>
   </si>
+  <si>
+    <t>SI SAMU</t>
+  </si>
+  <si>
+    <t>TYPE_MOYEN</t>
+  </si>
+  <si>
+    <t>SMUR</t>
+  </si>
+  <si>
+    <t>Smur</t>
+  </si>
+  <si>
+    <t>HOSPIT</t>
+  </si>
+  <si>
+    <t>Hospitaliers (hors Smur)</t>
+  </si>
+  <si>
+    <t>LIB</t>
+  </si>
+  <si>
+    <t>Professionnels Libéraux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSU </t>
+  </si>
+  <si>
+    <t>Ambulanciers privés (Transporteurs Sanitaires Urgent)</t>
+  </si>
+  <si>
+    <t>SIS</t>
+  </si>
+  <si>
+    <t>Pompiers</t>
+  </si>
+  <si>
+    <t>SECI</t>
+  </si>
+  <si>
+    <t>FDO</t>
+  </si>
+  <si>
+    <t>Force de l'Ordre et douanes</t>
+  </si>
+  <si>
+    <t>ADM</t>
+  </si>
+  <si>
+    <t>Institutions administratives et sociales</t>
+  </si>
+  <si>
+    <t>DAE</t>
+  </si>
+  <si>
+    <t>Défibrillateurs Automatisés Externes</t>
+  </si>
+  <si>
+    <t>Autres ressources</t>
+  </si>
+  <si>
+    <t>Sécurité civile, secouriste</t>
+  </si>
+  <si>
+    <t>Ensemble des ressources fixes et mobiles relevant de la responsabilité des Smur (UMH, HéliSmur…)</t>
+  </si>
+  <si>
+    <r>
+      <t>Ensemble des ressources fixes ou mobiles relevant du secteur hospitalier,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> public ou privé </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(établissement de soins, vecteurs sanitaires hospitaliers hors Smur…)</t>
+    </r>
+  </si>
+  <si>
+    <t>Ensemble des ressources fixes ou mobiles relevant de la prise en charge libérale (médecins libéraux, paramédicaux libéraux, pharmacies, MMG, SOS Médecin…)</t>
+  </si>
+  <si>
+    <t>Ensemble des ressources fixes et mobiles relevant des ambulances privées (ASSU, Ambulanciers…)</t>
+  </si>
+  <si>
+    <t>Ensemble des ressources fixes ou mobiles relevant des forces d’intervention Pompiers (VSAV, ISP, VLI, médecin SP…)</t>
+  </si>
+  <si>
+    <t>Ensemble des ressources fixes ou mobiles relevant des organisations de secourisme</t>
+  </si>
+  <si>
+    <t>Ensemble des ressources fixes ou mobiles relevant des forces de l’ordre (police nationale, municipale, gendarmerie nationaux et douanes)</t>
+  </si>
+  <si>
+    <t>Ensemble des ressources fixes ou mobiles relevant des administrations ou services sociaux (ARS, Institut National de Veille Sanitaire…)</t>
+  </si>
+  <si>
+    <t>Ensemble des défibrillateurs automatisés externes présents sur le territoire</t>
+  </si>
+  <si>
+    <t>Ensemble des ressources fixes ou mobiles ne relevant d’aucune catégorie précédemment définie</t>
+  </si>
+  <si>
+    <t>TYPE_DEC_ORIENT</t>
+  </si>
+  <si>
+    <t>LSP</t>
+  </si>
+  <si>
+    <t>REFUS</t>
+  </si>
+  <si>
+    <t>RAD</t>
+  </si>
+  <si>
+    <t>ORIENTE</t>
+  </si>
+  <si>
+    <t>Laissé sur place</t>
+  </si>
+  <si>
+    <t>Refus</t>
+  </si>
+  <si>
+    <r>
+      <t>Retour à domicile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ou autre lieu privé</t>
+    </r>
+  </si>
+  <si>
+    <t>Orientation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La situation du patient ne nécessite pas d'orientation vers un établissement de santé. Le patient est laissé sur place, sur les lieux d'intervention. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le patient refuse l'orientation proposée. Une autre modalité d'orientation doit lui être proposée. </t>
+  </si>
+  <si>
+    <r>
+      <t>La situation du patient ne nécessite pas d'orientation vers un établissement de santé. Le patient peut rentrer à domicile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ou tout autre lieu privé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> . Il peut être transporté par le vecteur d'intervention ou y rentrer par ses propres moyens. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le patient est orienté vers un établissement de santé </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ou un cabinet libéral</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5377,6 +5572,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -5398,7 +5614,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -5421,13 +5637,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5480,6 +5727,34 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7205,7 +7480,7 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -7387,10 +7662,10 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -8011,10 +8286,10 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -8452,7 +8727,7 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
@@ -8615,7 +8890,7 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -9047,7 +9322,7 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.5703125" customWidth="1"/>
@@ -9495,7 +9770,7 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -9694,6 +9969,1131 @@
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D57502-0378-4DA0-A304-75165DAB1E92}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="32"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="27"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="27"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="27"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="27"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="27"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="27"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="27"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="27"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="27"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="31"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="31"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="28"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="31"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="28"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="31"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="28"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="31"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="28"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="27"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="27"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="27"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="27"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="27"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="27"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84808B80-6F52-46A5-8814-B228DDBE2F0A}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:F45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="25.5">
+      <c r="A10" s="37" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="38" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="37" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="38" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" spans="1:6" ht="38.25">
+      <c r="A12" s="20" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="38" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="20" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="38" t="s">
+        <v>1721</v>
+      </c>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9407A0FF-6A83-4239-B794-9A5636395AD1}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:F45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="21" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>1681</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="21" t="s">
+        <v>1699</v>
+      </c>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="21" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>1683</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="21" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="21" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>1685</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="21" t="s">
+        <v>1701</v>
+      </c>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="21" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="21" t="s">
+        <v>1702</v>
+      </c>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="36" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="21" t="s">
+        <v>1703</v>
+      </c>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="36" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>1698</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="36" t="s">
+        <v>1704</v>
+      </c>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="21" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>1692</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="21" t="s">
+        <v>1705</v>
+      </c>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="21" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>1694</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="21" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="21" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>1696</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="21" t="s">
+        <v>1707</v>
+      </c>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="21" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>1697</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="21" t="s">
+        <v>1708</v>
+      </c>
       <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6">
@@ -9917,7 +11317,7 @@
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="33.28515625" customWidth="1"/>
@@ -13761,7 +15161,7 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -16480,7 +17880,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" style="10" customWidth="1"/>
@@ -16973,11 +18373,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8116353-BC00-4857-8D37-9470DD9A948C}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -17159,7 +18559,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5" ht="60.75">
+    <row r="18" spans="1:5" ht="48.75">
       <c r="A18" s="2" t="s">
         <v>1190</v>
       </c>
@@ -17172,7 +18572,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" ht="77.25">
+    <row r="19" spans="1:5" ht="64.5">
       <c r="A19" s="2" t="s">
         <v>1193</v>
       </c>
@@ -17659,7 +19059,7 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" ht="51.75">
+    <row r="60" spans="1:5" ht="39">
       <c r="A60" s="2" t="s">
         <v>1291</v>
       </c>
@@ -17701,7 +19101,7 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -17863,7 +19263,7 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
@@ -18248,7 +19648,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
@@ -18590,7 +19990,7 @@
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -19293,6 +20693,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19706,7 +21115,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -19758,23 +21167,48 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70979E6C-A1C8-4023-9129-41BEA99BA961}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70979E6C-A1C8-4023-9129-41BEA99BA961}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: removing old nomenclatures/in/ files, supporting "skipping nomenclature sheets", failing on not found nomenclature for MDD
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="557" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C34E23FC-B63B-4C12-BFBA-A09E0F8D99D8}"/>
+  <xr:revisionPtr revIDLastSave="570" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EF398EC-96EF-D14C-AEB3-F307AE88B876}"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="765" windowWidth="28860" windowHeight="13665" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" firstSheet="8" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -28,9 +28,10 @@
     <sheet name="Niveau de soin" sheetId="29" r:id="rId13"/>
     <sheet name="Type de décision" sheetId="30" r:id="rId14"/>
     <sheet name="Niveau de médicalisation" sheetId="31" r:id="rId15"/>
-    <sheet name="Etat du dossier" sheetId="34" r:id="rId16"/>
+    <sheet name="# Etat du dossier" sheetId="34" r:id="rId16"/>
     <sheet name="Orientation" sheetId="35" r:id="rId17"/>
-    <sheet name="Type de ressource-transport" sheetId="36" r:id="rId18"/>
+    <sheet name="Type de ressource" sheetId="36" r:id="rId18"/>
+    <sheet name="# Type de vecteurs" sheetId="37" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="1722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="1723">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -5478,6 +5479,9 @@
       </rPr>
       <t>ou un cabinet libéral</t>
     </r>
+  </si>
+  <si>
+    <t>A garder pour échanger : EMSI  (dans OPG) - dans le sens type de moyen/ressource, plus large que le type de vecteur/véhicule</t>
   </si>
 </sst>
 </file>
@@ -5674,7 +5678,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5756,9 +5760,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
+    <cellStyle name="60% - Accent5" xfId="1" builtinId="48"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
@@ -7085,6 +7090,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A9:D27" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}"/>
@@ -7480,12 +7489,12 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -7665,14 +7674,14 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91.7109375" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.6640625" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -8289,14 +8298,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -8727,13 +8736,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" customWidth="1"/>
-    <col min="6" max="6" width="61.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" customWidth="1"/>
+    <col min="6" max="6" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -8890,14 +8899,14 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -9322,14 +9331,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -9770,13 +9779,13 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10191,17 +10200,17 @@
   </sheetPr>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.140625" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="68.1640625" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10440,13 +10449,13 @@
       <selection activeCell="E10" sqref="E10:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10539,7 +10548,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="25.5">
+    <row r="10" spans="1:6" ht="28">
       <c r="A10" s="37" t="s">
         <v>1710</v>
       </c>
@@ -10567,7 +10576,7 @@
       </c>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:6" ht="38.25">
+    <row r="12" spans="1:6" ht="42">
       <c r="A12" s="20" t="s">
         <v>1712</v>
       </c>
@@ -10863,17 +10872,17 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10942,7 +10951,9 @@
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="39" t="s">
+        <v>1722</v>
+      </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
@@ -11305,6 +11316,23 @@
       <c r="F45" s="18"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EE5AD-9985-4D20-8EAC-8B61AD8038D6}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11313,18 +11341,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24418BCA-6BA9-46F7-8F30-546B2F7203DE}">
   <dimension ref="A1:F317"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="38.5703125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.83203125" customWidth="1"/>
+    <col min="5" max="5" width="47.83203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="38.5" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -11407,7 +11435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="64.5">
+    <row r="10" spans="1:6" ht="60">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -11433,7 +11461,7 @@
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="26.25">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -11447,7 +11475,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" ht="26.25">
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -11461,7 +11489,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" ht="26.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -11474,7 +11502,7 @@
       </c>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" ht="26.25">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -11502,7 +11530,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" ht="26.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -11528,7 +11556,7 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -11543,7 +11571,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="26.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -11569,7 +11597,7 @@
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" ht="39">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -11583,7 +11611,7 @@
       </c>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" ht="39">
+    <row r="23" spans="1:6" ht="30">
       <c r="A23" s="2" t="s">
         <v>68</v>
       </c>
@@ -11607,7 +11635,7 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:6" ht="26.25">
+    <row r="25" spans="1:6" ht="30">
       <c r="A25" s="2" t="s">
         <v>73</v>
       </c>
@@ -11621,7 +11649,7 @@
       </c>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:6" ht="26.25">
+    <row r="26" spans="1:6" ht="30">
       <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
@@ -11635,7 +11663,7 @@
       </c>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:6" ht="26.25">
+    <row r="27" spans="1:6" ht="30">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -11649,7 +11677,7 @@
       </c>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:6" ht="26.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
         <v>82</v>
       </c>
@@ -11685,7 +11713,7 @@
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="1:6" ht="51.75">
+    <row r="31" spans="1:6" ht="60">
       <c r="A31" s="2" t="s">
         <v>89</v>
       </c>
@@ -11699,7 +11727,7 @@
       </c>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:6" ht="26.25">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="2" t="s">
         <v>92</v>
       </c>
@@ -11738,7 +11766,7 @@
       </c>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" ht="26.25">
+    <row r="35" spans="1:6" ht="30">
       <c r="A35" s="2" t="s">
         <v>100</v>
       </c>
@@ -11764,7 +11792,7 @@
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:6" ht="102.75">
+    <row r="37" spans="1:6" ht="120">
       <c r="A37" s="2" t="s">
         <v>105</v>
       </c>
@@ -11778,7 +11806,7 @@
       </c>
       <c r="F37" s="12"/>
     </row>
-    <row r="38" spans="1:6" ht="26.25">
+    <row r="38" spans="1:6" ht="30">
       <c r="A38" s="2" t="s">
         <v>108</v>
       </c>
@@ -11792,7 +11820,7 @@
       </c>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="1:6" ht="39">
+    <row r="39" spans="1:6" ht="30">
       <c r="A39" s="2" t="s">
         <v>111</v>
       </c>
@@ -11817,7 +11845,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
     </row>
-    <row r="41" spans="1:6" ht="39">
+    <row r="41" spans="1:6" ht="30">
       <c r="A41" s="2" t="s">
         <v>116</v>
       </c>
@@ -11831,7 +11859,7 @@
       </c>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:6" ht="26.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>119</v>
       </c>
@@ -11845,7 +11873,7 @@
       </c>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:6" ht="39">
+    <row r="43" spans="1:6" ht="30">
       <c r="A43" s="2" t="s">
         <v>122</v>
       </c>
@@ -11869,7 +11897,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
     </row>
-    <row r="45" spans="1:6" ht="39">
+    <row r="45" spans="1:6" ht="45">
       <c r="A45" s="2" t="s">
         <v>127</v>
       </c>
@@ -11968,7 +11996,7 @@
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="1:6" ht="26.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
         <v>145</v>
       </c>
@@ -11982,7 +12010,7 @@
       </c>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:6" ht="64.5">
+    <row r="54" spans="1:6" ht="60">
       <c r="A54" s="2" t="s">
         <v>148</v>
       </c>
@@ -12353,7 +12381,7 @@
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
     </row>
-    <row r="85" spans="1:6" ht="39">
+    <row r="85" spans="1:6" ht="45">
       <c r="A85" s="2" t="s">
         <v>214</v>
       </c>
@@ -12379,7 +12407,7 @@
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
     </row>
-    <row r="87" spans="1:6" ht="128.25">
+    <row r="87" spans="1:6" ht="135">
       <c r="A87" s="2" t="s">
         <v>219</v>
       </c>
@@ -12405,7 +12433,7 @@
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
     </row>
-    <row r="89" spans="1:6" ht="51.75">
+    <row r="89" spans="1:6" ht="60">
       <c r="A89" s="2" t="s">
         <v>212</v>
       </c>
@@ -12418,7 +12446,7 @@
       </c>
       <c r="F89" s="12"/>
     </row>
-    <row r="90" spans="1:6" ht="26.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="2" t="s">
         <v>214</v>
       </c>
@@ -12458,7 +12486,7 @@
       <c r="E92" s="12"/>
       <c r="F92" s="12"/>
     </row>
-    <row r="93" spans="1:6" ht="26.25">
+    <row r="93" spans="1:6" ht="30">
       <c r="A93" s="2" t="s">
         <v>230</v>
       </c>
@@ -12629,7 +12657,7 @@
       <c r="E106" s="12"/>
       <c r="F106" s="12"/>
     </row>
-    <row r="107" spans="1:6" ht="26.25">
+    <row r="107" spans="1:6" ht="30">
       <c r="A107" s="2" t="s">
         <v>261</v>
       </c>
@@ -12643,7 +12671,7 @@
       </c>
       <c r="F107" s="12"/>
     </row>
-    <row r="108" spans="1:6" ht="26.25">
+    <row r="108" spans="1:6">
       <c r="A108" s="2" t="s">
         <v>264</v>
       </c>
@@ -12767,7 +12795,7 @@
       <c r="E117" s="12"/>
       <c r="F117" s="12"/>
     </row>
-    <row r="118" spans="1:6" ht="26.25">
+    <row r="118" spans="1:6" ht="30">
       <c r="A118" s="2" t="s">
         <v>287</v>
       </c>
@@ -12781,7 +12809,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="26.25">
+    <row r="119" spans="1:6">
       <c r="A119" s="2" t="s">
         <v>290</v>
       </c>
@@ -12794,7 +12822,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="39">
+    <row r="120" spans="1:6" ht="45">
       <c r="A120" s="2" t="s">
         <v>293</v>
       </c>
@@ -12832,7 +12860,7 @@
       <c r="E122" s="12"/>
       <c r="F122" s="12"/>
     </row>
-    <row r="123" spans="1:6" ht="39">
+    <row r="123" spans="1:6" ht="45">
       <c r="A123" s="2" t="s">
         <v>300</v>
       </c>
@@ -12893,7 +12921,7 @@
       <c r="E127" s="12"/>
       <c r="F127" s="12"/>
     </row>
-    <row r="128" spans="1:6" ht="39">
+    <row r="128" spans="1:6" ht="45">
       <c r="A128" s="2" t="s">
         <v>311</v>
       </c>
@@ -13027,7 +13055,7 @@
       <c r="E138" s="12"/>
       <c r="F138" s="12"/>
     </row>
-    <row r="139" spans="1:6" ht="26.25">
+    <row r="139" spans="1:6" ht="30">
       <c r="A139" s="2" t="s">
         <v>336</v>
       </c>
@@ -13052,7 +13080,7 @@
       <c r="E140" s="12"/>
       <c r="F140" s="12"/>
     </row>
-    <row r="141" spans="1:6" ht="26.25">
+    <row r="141" spans="1:6" ht="30">
       <c r="A141" s="2" t="s">
         <v>341</v>
       </c>
@@ -13066,7 +13094,7 @@
       </c>
       <c r="F141" s="12"/>
     </row>
-    <row r="142" spans="1:6" ht="26.25">
+    <row r="142" spans="1:6" ht="30">
       <c r="A142" s="2" t="s">
         <v>342</v>
       </c>
@@ -13080,7 +13108,7 @@
       </c>
       <c r="F142" s="12"/>
     </row>
-    <row r="143" spans="1:6" ht="26.25">
+    <row r="143" spans="1:6">
       <c r="A143" s="2" t="s">
         <v>343</v>
       </c>
@@ -13094,7 +13122,7 @@
       </c>
       <c r="F143" s="12"/>
     </row>
-    <row r="144" spans="1:6" ht="26.25">
+    <row r="144" spans="1:6" ht="30">
       <c r="A144" s="2" t="s">
         <v>344</v>
       </c>
@@ -13123,7 +13151,7 @@
       </c>
       <c r="F145" s="12"/>
     </row>
-    <row r="146" spans="1:6" ht="26.25">
+    <row r="146" spans="1:6">
       <c r="A146" s="2" t="s">
         <v>347</v>
       </c>
@@ -13137,7 +13165,7 @@
       </c>
       <c r="F146" s="12"/>
     </row>
-    <row r="147" spans="1:6" ht="39">
+    <row r="147" spans="1:6" ht="30">
       <c r="A147" s="2" t="s">
         <v>348</v>
       </c>
@@ -13151,7 +13179,7 @@
       </c>
       <c r="F147" s="12"/>
     </row>
-    <row r="148" spans="1:6" ht="39">
+    <row r="148" spans="1:6" ht="30">
       <c r="A148" s="2" t="s">
         <v>349</v>
       </c>
@@ -13165,7 +13193,7 @@
       </c>
       <c r="F148" s="12"/>
     </row>
-    <row r="149" spans="1:6" ht="26.25">
+    <row r="149" spans="1:6" ht="30">
       <c r="A149" s="2" t="s">
         <v>350</v>
       </c>
@@ -13178,7 +13206,7 @@
       </c>
       <c r="F149" s="12"/>
     </row>
-    <row r="150" spans="1:6" ht="26.25">
+    <row r="150" spans="1:6" ht="30">
       <c r="A150" s="2" t="s">
         <v>351</v>
       </c>
@@ -13192,7 +13220,7 @@
       </c>
       <c r="F150" s="12"/>
     </row>
-    <row r="151" spans="1:6" ht="26.25">
+    <row r="151" spans="1:6" ht="30">
       <c r="A151" s="2" t="s">
         <v>352</v>
       </c>
@@ -13324,7 +13352,7 @@
       <c r="E161" s="12"/>
       <c r="F161" s="12"/>
     </row>
-    <row r="162" spans="1:6" ht="39">
+    <row r="162" spans="1:6" ht="30">
       <c r="A162" s="2" t="s">
         <v>373</v>
       </c>
@@ -13338,7 +13366,7 @@
       </c>
       <c r="F162" s="12"/>
     </row>
-    <row r="163" spans="1:6" ht="39">
+    <row r="163" spans="1:6" ht="45">
       <c r="A163" s="2" t="s">
         <v>376</v>
       </c>
@@ -13352,7 +13380,7 @@
       </c>
       <c r="F163" s="12"/>
     </row>
-    <row r="164" spans="1:6" ht="39">
+    <row r="164" spans="1:6" ht="45">
       <c r="A164" s="2" t="s">
         <v>379</v>
       </c>
@@ -13403,7 +13431,7 @@
       <c r="E167" s="12"/>
       <c r="F167" s="12"/>
     </row>
-    <row r="168" spans="1:6" ht="26.25">
+    <row r="168" spans="1:6" ht="30">
       <c r="A168" s="2" t="s">
         <v>389</v>
       </c>
@@ -13620,7 +13648,7 @@
       <c r="E185" s="12"/>
       <c r="F185" s="12"/>
     </row>
-    <row r="186" spans="1:6" ht="26.25">
+    <row r="186" spans="1:6" ht="30">
       <c r="A186" s="2" t="s">
         <v>426</v>
       </c>
@@ -13756,7 +13784,7 @@
       </c>
       <c r="F196" s="12"/>
     </row>
-    <row r="197" spans="1:6" ht="26.25">
+    <row r="197" spans="1:6">
       <c r="A197" s="2" t="s">
         <v>451</v>
       </c>
@@ -13856,7 +13884,7 @@
       <c r="E204" s="12"/>
       <c r="F204" s="12"/>
     </row>
-    <row r="205" spans="1:6" ht="26.25">
+    <row r="205" spans="1:6" ht="30">
       <c r="A205" s="2" t="s">
         <v>470</v>
       </c>
@@ -13882,7 +13910,7 @@
       <c r="E206" s="12"/>
       <c r="F206" s="12"/>
     </row>
-    <row r="207" spans="1:6" ht="26.25">
+    <row r="207" spans="1:6" ht="30">
       <c r="A207" s="2" t="s">
         <v>475</v>
       </c>
@@ -13980,7 +14008,7 @@
       <c r="E214" s="12"/>
       <c r="F214" s="12"/>
     </row>
-    <row r="215" spans="1:6" ht="26.25">
+    <row r="215" spans="1:6" ht="30">
       <c r="A215" s="2" t="s">
         <v>493</v>
       </c>
@@ -14801,7 +14829,7 @@
       <c r="E282" s="12"/>
       <c r="F282" s="12"/>
     </row>
-    <row r="283" spans="1:6" ht="26.25">
+    <row r="283" spans="1:6" ht="30">
       <c r="A283" s="2" t="s">
         <v>638</v>
       </c>
@@ -14815,7 +14843,7 @@
       </c>
       <c r="F283" s="12"/>
     </row>
-    <row r="284" spans="1:6" ht="26.25">
+    <row r="284" spans="1:6" ht="30">
       <c r="A284" s="2" t="s">
         <v>641</v>
       </c>
@@ -15161,14 +15189,14 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -17880,12 +17908,12 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" style="10" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="10" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -17896,7 +17924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24.75">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -17962,7 +17990,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="39">
+    <row r="10" spans="1:4" ht="45">
       <c r="A10" s="2" t="s">
         <v>1082</v>
       </c>
@@ -17984,7 +18012,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="26.25">
+    <row r="12" spans="1:4" ht="30">
       <c r="A12" s="2" t="s">
         <v>1087</v>
       </c>
@@ -17994,7 +18022,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="39">
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="2" t="s">
         <v>1089</v>
       </c>
@@ -18004,7 +18032,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="26.25">
+    <row r="14" spans="1:4" ht="30">
       <c r="A14" s="2" t="s">
         <v>1091</v>
       </c>
@@ -18014,7 +18042,7 @@
       <c r="C14" s="12"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="26.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>1093</v>
       </c>
@@ -18024,7 +18052,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="26.25">
+    <row r="16" spans="1:4" ht="30">
       <c r="A16" s="2" t="s">
         <v>1095</v>
       </c>
@@ -18036,7 +18064,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="39">
+    <row r="17" spans="1:4" ht="45">
       <c r="A17" s="2" t="s">
         <v>1098</v>
       </c>
@@ -18048,7 +18076,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="39">
+    <row r="18" spans="1:4" ht="30">
       <c r="A18" s="2" t="s">
         <v>1101</v>
       </c>
@@ -18058,7 +18086,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="39">
+    <row r="19" spans="1:4" ht="45">
       <c r="A19" s="2" t="s">
         <v>1103</v>
       </c>
@@ -18068,7 +18096,7 @@
       <c r="C19" s="12"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="26.25">
+    <row r="20" spans="1:4" ht="30">
       <c r="A20" s="2" t="s">
         <v>1105</v>
       </c>
@@ -18078,7 +18106,7 @@
       <c r="C20" s="12"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" ht="26.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>1107</v>
       </c>
@@ -18088,7 +18116,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="26.25">
+    <row r="22" spans="1:4" ht="30">
       <c r="A22" s="2" t="s">
         <v>1109</v>
       </c>
@@ -18118,7 +18146,7 @@
       <c r="C24" s="12"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" ht="26.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>1115</v>
       </c>
@@ -18148,7 +18176,7 @@
       <c r="C27" s="12"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="26.25">
+    <row r="28" spans="1:4" ht="30">
       <c r="A28" s="2" t="s">
         <v>1120</v>
       </c>
@@ -18160,7 +18188,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="26.25">
+    <row r="29" spans="1:4" ht="30">
       <c r="A29" s="2" t="s">
         <v>1123</v>
       </c>
@@ -18172,7 +18200,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="26.25">
+    <row r="30" spans="1:4" ht="30">
       <c r="A30" s="2" t="s">
         <v>1126</v>
       </c>
@@ -18194,7 +18222,7 @@
       <c r="C31" s="12"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="26.25">
+    <row r="32" spans="1:4" ht="30">
       <c r="A32" s="2" t="s">
         <v>1131</v>
       </c>
@@ -18206,7 +18234,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="39">
+    <row r="33" spans="1:4" ht="30">
       <c r="A33" s="2" t="s">
         <v>1134</v>
       </c>
@@ -18218,7 +18246,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" ht="26.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>1137</v>
       </c>
@@ -18230,7 +18258,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="128.25">
+    <row r="35" spans="1:4" ht="135">
       <c r="A35" s="2" t="s">
         <v>1140</v>
       </c>
@@ -18242,7 +18270,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="128.25">
+    <row r="36" spans="1:4" ht="135">
       <c r="A36" s="2" t="s">
         <v>1143</v>
       </c>
@@ -18326,7 +18354,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="26.25">
+    <row r="44" spans="1:4" ht="30">
       <c r="A44" s="2" t="s">
         <v>1160</v>
       </c>
@@ -18338,7 +18366,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="26.25">
+    <row r="45" spans="1:4" ht="30">
       <c r="A45" s="2" t="s">
         <v>1163</v>
       </c>
@@ -18348,7 +18376,7 @@
       <c r="C45" s="12"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" ht="77.25">
+    <row r="46" spans="1:4" ht="75">
       <c r="A46" s="2" t="s">
         <v>1165</v>
       </c>
@@ -18377,13 +18405,13 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="39.5" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.1640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18498,7 +18526,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5" ht="26.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>1177</v>
       </c>
@@ -18522,7 +18550,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" ht="26.25">
+    <row r="15" spans="1:5" ht="30">
       <c r="A15" s="2" t="s">
         <v>1182</v>
       </c>
@@ -18535,7 +18563,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" ht="26.25">
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="2" t="s">
         <v>1185</v>
       </c>
@@ -18559,7 +18587,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5" ht="48.75">
+    <row r="18" spans="1:5" ht="40">
       <c r="A18" s="2" t="s">
         <v>1190</v>
       </c>
@@ -18572,7 +18600,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" ht="64.5">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="2" t="s">
         <v>1193</v>
       </c>
@@ -18721,7 +18749,7 @@
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:5" ht="26.25">
+    <row r="32" spans="1:5" ht="30">
       <c r="A32" s="2" t="s">
         <v>1222</v>
       </c>
@@ -18734,7 +18762,7 @@
       </c>
       <c r="E32" s="12"/>
     </row>
-    <row r="33" spans="1:5" ht="26.25">
+    <row r="33" spans="1:5" ht="30">
       <c r="A33" s="2" t="s">
         <v>1225</v>
       </c>
@@ -18821,7 +18849,7 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
     </row>
-    <row r="40" spans="1:5" ht="51.75">
+    <row r="40" spans="1:5" ht="45">
       <c r="A40" s="2" t="s">
         <v>1244</v>
       </c>
@@ -18858,7 +18886,7 @@
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5" ht="26.25">
+    <row r="43" spans="1:5" ht="30">
       <c r="A43" s="2" t="s">
         <v>1252</v>
       </c>
@@ -18871,7 +18899,7 @@
       </c>
       <c r="E43" s="12"/>
     </row>
-    <row r="44" spans="1:5" ht="39">
+    <row r="44" spans="1:5" ht="30">
       <c r="A44" s="2" t="s">
         <v>1253</v>
       </c>
@@ -18930,7 +18958,7 @@
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
     </row>
-    <row r="49" spans="1:5" ht="26.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="2" t="s">
         <v>1265</v>
       </c>
@@ -18965,7 +18993,7 @@
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
     </row>
-    <row r="52" spans="1:5" ht="26.25">
+    <row r="52" spans="1:5" ht="30">
       <c r="A52" s="2" t="s">
         <v>1272</v>
       </c>
@@ -19059,7 +19087,7 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" ht="39">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="2" t="s">
         <v>1291</v>
       </c>
@@ -19101,12 +19129,12 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -19260,16 +19288,16 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -19355,7 +19383,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="32">
       <c r="A10" s="18" t="s">
         <v>1314</v>
       </c>
@@ -19368,7 +19396,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="45">
+    <row r="11" spans="1:5" ht="32">
       <c r="A11" s="18" t="s">
         <v>1317</v>
       </c>
@@ -19381,7 +19409,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="16">
       <c r="A12" s="18" t="s">
         <v>1320</v>
       </c>
@@ -19394,7 +19422,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="30">
+    <row r="13" spans="1:5" ht="32">
       <c r="A13" s="18" t="s">
         <v>1323</v>
       </c>
@@ -19407,7 +19435,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="30">
+    <row r="14" spans="1:5" ht="16">
       <c r="A14" s="18" t="s">
         <v>1326</v>
       </c>
@@ -19420,7 +19448,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="45">
+    <row r="15" spans="1:5" ht="32">
       <c r="A15" s="18" t="s">
         <v>1329</v>
       </c>
@@ -19433,7 +19461,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="32">
       <c r="A16" s="18" t="s">
         <v>1332</v>
       </c>
@@ -19446,7 +19474,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:5" ht="32">
       <c r="A17" s="18" t="s">
         <v>1335</v>
       </c>
@@ -19459,7 +19487,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="45">
+    <row r="18" spans="1:5" ht="48">
       <c r="A18" s="18" t="s">
         <v>1338</v>
       </c>
@@ -19472,7 +19500,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="48">
       <c r="A19" s="18" t="s">
         <v>1341</v>
       </c>
@@ -19485,7 +19513,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="45">
+    <row r="20" spans="1:5" ht="32">
       <c r="A20" s="18" t="s">
         <v>1344</v>
       </c>
@@ -19498,7 +19526,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="30">
+    <row r="21" spans="1:5" ht="32">
       <c r="A21" s="18" t="s">
         <v>1347</v>
       </c>
@@ -19511,7 +19539,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="30">
+    <row r="22" spans="1:5" ht="32">
       <c r="A22" s="18" t="s">
         <v>1350</v>
       </c>
@@ -19524,7 +19552,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:5" ht="32">
       <c r="A23" s="18" t="s">
         <v>1353</v>
       </c>
@@ -19537,7 +19565,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="32">
       <c r="A24" s="18" t="s">
         <v>1356</v>
       </c>
@@ -19550,7 +19578,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="30">
+    <row r="25" spans="1:5" ht="32">
       <c r="A25" s="18" t="s">
         <v>1359</v>
       </c>
@@ -19563,7 +19591,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="30">
+    <row r="26" spans="1:5" ht="32">
       <c r="A26" s="18" t="s">
         <v>1362</v>
       </c>
@@ -19576,7 +19604,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="16">
       <c r="A27" s="18" t="s">
         <v>1365</v>
       </c>
@@ -19589,7 +19617,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="30">
+    <row r="28" spans="1:5" ht="32">
       <c r="A28" s="18" t="s">
         <v>1367</v>
       </c>
@@ -19602,7 +19630,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" ht="16">
       <c r="A29" s="18" t="s">
         <v>1370</v>
       </c>
@@ -19615,7 +19643,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" ht="16">
       <c r="A30" s="18" t="s">
         <v>1373</v>
       </c>
@@ -19648,13 +19676,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -19751,7 +19779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="18" t="s">
         <v>1378</v>
       </c>
@@ -19765,7 +19793,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="45">
+    <row r="11" spans="1:6" ht="48">
       <c r="A11" s="18" t="s">
         <v>1381</v>
       </c>
@@ -19779,7 +19807,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="45">
+    <row r="12" spans="1:6" ht="32">
       <c r="A12" s="18" t="s">
         <v>1384</v>
       </c>
@@ -19793,7 +19821,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="32">
       <c r="A13" s="18" t="s">
         <v>1387</v>
       </c>
@@ -19807,7 +19835,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="45">
+    <row r="14" spans="1:6" ht="32">
       <c r="A14" s="18" t="s">
         <v>1390</v>
       </c>
@@ -19821,7 +19849,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="32">
       <c r="A15" s="18" t="s">
         <v>1393</v>
       </c>
@@ -19835,7 +19863,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="30">
+    <row r="16" spans="1:6" ht="32">
       <c r="A16" s="18" t="s">
         <v>1396</v>
       </c>
@@ -19849,7 +19877,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="45">
+    <row r="17" spans="1:6" ht="48">
       <c r="A17" s="18" t="s">
         <v>1370</v>
       </c>
@@ -19863,7 +19891,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="30">
+    <row r="18" spans="1:6" ht="32">
       <c r="A18" s="18" t="s">
         <v>1401</v>
       </c>
@@ -19990,13 +20018,13 @@
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -21198,16 +21226,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
[24.04.24 15:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="570" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EF398EC-96EF-D14C-AEB3-F307AE88B876}"/>
+  <xr:revisionPtr revIDLastSave="580" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E77414BC-CE1B-4E7A-84C7-B143BC5B0539}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" firstSheet="8" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1395" windowWidth="26475" windowHeight="13560" firstSheet="13" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="Type de décision" sheetId="30" r:id="rId14"/>
     <sheet name="Niveau de médicalisation" sheetId="31" r:id="rId15"/>
     <sheet name="# Etat du dossier" sheetId="34" r:id="rId16"/>
-    <sheet name="Orientation" sheetId="35" r:id="rId17"/>
+    <sheet name="Type de devenir du patient" sheetId="35" r:id="rId17"/>
     <sheet name="Type de ressource" sheetId="36" r:id="rId18"/>
     <sheet name="# Type de vecteurs" sheetId="37" r:id="rId19"/>
   </sheets>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="1723">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2169" uniqueCount="1753">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -5401,87 +5401,136 @@
     <t>Ensemble des ressources fixes ou mobiles ne relevant d’aucune catégorie précédemment définie</t>
   </si>
   <si>
-    <t>TYPE_DEC_ORIENT</t>
-  </si>
-  <si>
-    <t>LSP</t>
-  </si>
-  <si>
-    <t>REFUS</t>
-  </si>
-  <si>
-    <t>RAD</t>
-  </si>
-  <si>
-    <t>ORIENTE</t>
-  </si>
-  <si>
-    <t>Laissé sur place</t>
-  </si>
-  <si>
-    <t>Refus</t>
-  </si>
-  <si>
-    <r>
-      <t>Retour à domicile</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ou autre lieu privé</t>
-    </r>
-  </si>
-  <si>
-    <t>Orientation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La situation du patient ne nécessite pas d'orientation vers un établissement de santé. Le patient est laissé sur place, sur les lieux d'intervention. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le patient refuse l'orientation proposée. Une autre modalité d'orientation doit lui être proposée. </t>
-  </si>
-  <si>
-    <r>
-      <t>La situation du patient ne nécessite pas d'orientation vers un établissement de santé. Le patient peut rentrer à domicile</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ou tout autre lieu privé</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> . Il peut être transporté par le vecteur d'intervention ou y rentrer par ses propres moyens. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Le patient est orienté vers un établissement de santé </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ou un cabinet libéral</t>
-    </r>
-  </si>
-  <si>
     <t>A garder pour échanger : EMSI  (dans OPG) - dans le sens type de moyen/ressource, plus large que le type de vecteur/véhicule</t>
+  </si>
+  <si>
+    <t>NOMENC_DEVENIR_PAT</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>TEMP</t>
+  </si>
+  <si>
+    <t>SEUL</t>
+  </si>
+  <si>
+    <t>AFAMILLE</t>
+  </si>
+  <si>
+    <t>AMED</t>
+  </si>
+  <si>
+    <t>AFDO</t>
+  </si>
+  <si>
+    <t>ATIERS</t>
+  </si>
+  <si>
+    <t>MOYPERSO</t>
+  </si>
+  <si>
+    <t>Code vecteur choisi</t>
+  </si>
+  <si>
+    <t>REFPAT</t>
+  </si>
+  <si>
+    <t>REFFAM</t>
+  </si>
+  <si>
+    <t>PASREAKO</t>
+  </si>
+  <si>
+    <t>PASREAOK</t>
+  </si>
+  <si>
+    <t>REA</t>
+  </si>
+  <si>
+    <t>TRANSPOR</t>
+  </si>
+  <si>
+    <t>FUGUE</t>
+  </si>
+  <si>
+    <t>REFAUTRE</t>
+  </si>
+  <si>
+    <t>RAS</t>
+  </si>
+  <si>
+    <t>Accord du service d'orientation</t>
+  </si>
+  <si>
+    <t>Accord sous condition (en attente d'avis ou d'examen complémentaire ou d'affectation vers le service adapté)</t>
+  </si>
+  <si>
+    <t>Laissé seul</t>
+  </si>
+  <si>
+    <t>Laissé à la famille ou entourage</t>
+  </si>
+  <si>
+    <t>Confié à un médecin</t>
+  </si>
+  <si>
+    <t>Confié aux Forces de l'ordre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confié à autre personne </t>
+  </si>
+  <si>
+    <t>Retour à domicile - Transporté par ses propres moyens</t>
+  </si>
+  <si>
+    <t>Retour à domicile - Transporté par le vecteur d'intervention ou de transport envoyé par le CRRA</t>
+  </si>
+  <si>
+    <t>Retour à domicile - Refus du patient, patient laissé sur place</t>
+  </si>
+  <si>
+    <t>Retour à domicile - Refus de l'entourage, patient laissé sur place</t>
+  </si>
+  <si>
+    <t>DCD sans réanimation - non examiné par médecin</t>
+  </si>
+  <si>
+    <t>DCD sans réanimation - examiné par médecin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCD après réanimation </t>
+  </si>
+  <si>
+    <t>DCD pendant le transport</t>
+  </si>
+  <si>
+    <t>DCD à son admission</t>
+  </si>
+  <si>
+    <t>Fugue, le patient n'est plus sur les lieux</t>
+  </si>
+  <si>
+    <t>Autres refus orientation</t>
+  </si>
+  <si>
+    <t>Pas de prise en charge nécessaire</t>
+  </si>
+  <si>
+    <t>Devenir issu de la décision d'orientation + modalité d'exécution</t>
+  </si>
+  <si>
+    <t>Devenir issu de la décision d'orientation + Type de laissé sur place</t>
+  </si>
+  <si>
+    <t>Devenir issu de la décision d'orientation + mode de transport</t>
+  </si>
+  <si>
+    <t>Devenir issu de la décision d'orientation + motif de refus</t>
+  </si>
+  <si>
+    <t>Devenir issu de l'information relative au décès du patient</t>
   </si>
 </sst>
 </file>
@@ -5678,7 +5727,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5757,13 +5806,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="60% - Accent5" xfId="1" builtinId="48"/>
+    <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
@@ -7090,10 +7136,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A9:D27" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}"/>
@@ -7489,12 +7531,12 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -7674,14 +7716,14 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91.6640625" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.7109375" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -8298,14 +8340,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -8736,13 +8778,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" customWidth="1"/>
-    <col min="6" max="6" width="61.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" customWidth="1"/>
+    <col min="6" max="6" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -8899,14 +8941,14 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -9331,14 +9373,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -9779,13 +9821,13 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10200,17 +10242,17 @@
   </sheetPr>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.1640625" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="68.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10445,17 +10487,17 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10473,7 +10515,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -10548,180 +10590,270 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28">
+    <row r="10" spans="1:6">
       <c r="A10" s="37" t="s">
-        <v>1710</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>1714</v>
+        <v>1711</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>1729</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
-      <c r="E10" s="38" t="s">
-        <v>1718</v>
+      <c r="E10" s="37" t="s">
+        <v>1748</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="37" t="s">
-        <v>1711</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>1715</v>
+        <v>1712</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>1730</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
-      <c r="E11" s="38" t="s">
-        <v>1719</v>
+      <c r="E11" s="37" t="s">
+        <v>1748</v>
       </c>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:6" ht="42">
+    <row r="12" spans="1:6">
       <c r="A12" s="20" t="s">
-        <v>1712</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>1716</v>
+        <v>1713</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>1731</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
-      <c r="E12" s="38" t="s">
-        <v>1720</v>
+      <c r="E12" s="37" t="s">
+        <v>1749</v>
       </c>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="20" t="s">
-        <v>1713</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>1717</v>
+        <v>1714</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>1732</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
-      <c r="E13" s="38" t="s">
-        <v>1721</v>
+      <c r="E13" s="37" t="s">
+        <v>1749</v>
       </c>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="18" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>1733</v>
+      </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="E14" s="37" t="s">
+        <v>1749</v>
+      </c>
       <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
+      <c r="A15" s="18" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>1734</v>
+      </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="E15" s="37" t="s">
+        <v>1749</v>
+      </c>
       <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="18" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>1735</v>
+      </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="37" t="s">
+        <v>1749</v>
+      </c>
       <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="18" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>1736</v>
+      </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="E17" s="37" t="s">
+        <v>1750</v>
+      </c>
       <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="18" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>1737</v>
+      </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="E18" s="37" t="s">
+        <v>1750</v>
+      </c>
       <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="18" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>1738</v>
+      </c>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="E19" s="37" t="s">
+        <v>1751</v>
+      </c>
       <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
+      <c r="A20" s="18" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>1739</v>
+      </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="E20" s="37" t="s">
+        <v>1751</v>
+      </c>
       <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
+      <c r="A21" s="18" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>1740</v>
+      </c>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
+      <c r="E21" s="37" t="s">
+        <v>1752</v>
+      </c>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
+      <c r="A22" s="18" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>1741</v>
+      </c>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
+      <c r="E22" s="37" t="s">
+        <v>1752</v>
+      </c>
       <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
+      <c r="A23" s="18" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>1742</v>
+      </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
+      <c r="E23" s="37" t="s">
+        <v>1752</v>
+      </c>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
+      <c r="A24" s="18" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>1743</v>
+      </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
+      <c r="E24" s="37" t="s">
+        <v>1752</v>
+      </c>
       <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
+      <c r="A25" s="18" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>1744</v>
+      </c>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
+      <c r="E25" s="37" t="s">
+        <v>1752</v>
+      </c>
       <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
+      <c r="A26" s="18" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>1745</v>
+      </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
+      <c r="E26" s="37" t="s">
+        <v>1751</v>
+      </c>
       <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
+      <c r="A27" s="18" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>1746</v>
+      </c>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
+      <c r="E27" s="37" t="s">
+        <v>1751</v>
+      </c>
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
+      <c r="A28" s="18" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>1747</v>
+      </c>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
+      <c r="E28" s="37" t="s">
+        <v>1749</v>
+      </c>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6">
@@ -10876,13 +11008,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10951,8 +11083,8 @@
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="39" t="s">
-        <v>1722</v>
+      <c r="B8" s="38" t="s">
+        <v>1709</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -11327,7 +11459,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
@@ -11341,18 +11473,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24418BCA-6BA9-46F7-8F30-546B2F7203DE}">
   <dimension ref="A1:F317"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="45.83203125" customWidth="1"/>
-    <col min="5" max="5" width="47.83203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="38.5" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -11435,7 +11567,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60">
+    <row r="10" spans="1:6" ht="64.5">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -11461,7 +11593,7 @@
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="30">
+    <row r="12" spans="1:6" ht="26.25">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -11475,7 +11607,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="26.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -11489,7 +11621,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="26.25">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -11502,7 +11634,7 @@
       </c>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -11530,7 +11662,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="26.25">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -11556,7 +11688,7 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="26.25">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -11571,7 +11703,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="26.25">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -11597,7 +11729,7 @@
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" ht="30">
+    <row r="22" spans="1:6" ht="39">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -11611,7 +11743,7 @@
       </c>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" ht="30">
+    <row r="23" spans="1:6" ht="39">
       <c r="A23" s="2" t="s">
         <v>68</v>
       </c>
@@ -11635,7 +11767,7 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:6" ht="30">
+    <row r="25" spans="1:6" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>73</v>
       </c>
@@ -11649,7 +11781,7 @@
       </c>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:6" ht="30">
+    <row r="26" spans="1:6" ht="26.25">
       <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
@@ -11663,7 +11795,7 @@
       </c>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:6" ht="30">
+    <row r="27" spans="1:6" ht="26.25">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -11677,7 +11809,7 @@
       </c>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="26.25">
       <c r="A28" s="2" t="s">
         <v>82</v>
       </c>
@@ -11713,7 +11845,7 @@
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="1:6" ht="60">
+    <row r="31" spans="1:6" ht="51.75">
       <c r="A31" s="2" t="s">
         <v>89</v>
       </c>
@@ -11727,7 +11859,7 @@
       </c>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:6" ht="30">
+    <row r="32" spans="1:6" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>92</v>
       </c>
@@ -11766,7 +11898,7 @@
       </c>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" ht="30">
+    <row r="35" spans="1:6" ht="26.25">
       <c r="A35" s="2" t="s">
         <v>100</v>
       </c>
@@ -11792,7 +11924,7 @@
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:6" ht="120">
+    <row r="37" spans="1:6" ht="102.75">
       <c r="A37" s="2" t="s">
         <v>105</v>
       </c>
@@ -11806,7 +11938,7 @@
       </c>
       <c r="F37" s="12"/>
     </row>
-    <row r="38" spans="1:6" ht="30">
+    <row r="38" spans="1:6" ht="26.25">
       <c r="A38" s="2" t="s">
         <v>108</v>
       </c>
@@ -11820,7 +11952,7 @@
       </c>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="1:6" ht="30">
+    <row r="39" spans="1:6" ht="39">
       <c r="A39" s="2" t="s">
         <v>111</v>
       </c>
@@ -11845,7 +11977,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
     </row>
-    <row r="41" spans="1:6" ht="30">
+    <row r="41" spans="1:6" ht="39">
       <c r="A41" s="2" t="s">
         <v>116</v>
       </c>
@@ -11859,7 +11991,7 @@
       </c>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" ht="26.25">
       <c r="A42" s="2" t="s">
         <v>119</v>
       </c>
@@ -11873,7 +12005,7 @@
       </c>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:6" ht="30">
+    <row r="43" spans="1:6" ht="39">
       <c r="A43" s="2" t="s">
         <v>122</v>
       </c>
@@ -11897,7 +12029,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
     </row>
-    <row r="45" spans="1:6" ht="45">
+    <row r="45" spans="1:6" ht="39">
       <c r="A45" s="2" t="s">
         <v>127</v>
       </c>
@@ -11996,7 +12128,7 @@
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" ht="26.25">
       <c r="A53" s="2" t="s">
         <v>145</v>
       </c>
@@ -12010,7 +12142,7 @@
       </c>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:6" ht="60">
+    <row r="54" spans="1:6" ht="64.5">
       <c r="A54" s="2" t="s">
         <v>148</v>
       </c>
@@ -12381,7 +12513,7 @@
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
     </row>
-    <row r="85" spans="1:6" ht="45">
+    <row r="85" spans="1:6" ht="39">
       <c r="A85" s="2" t="s">
         <v>214</v>
       </c>
@@ -12407,7 +12539,7 @@
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
     </row>
-    <row r="87" spans="1:6" ht="135">
+    <row r="87" spans="1:6" ht="128.25">
       <c r="A87" s="2" t="s">
         <v>219</v>
       </c>
@@ -12433,7 +12565,7 @@
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
     </row>
-    <row r="89" spans="1:6" ht="60">
+    <row r="89" spans="1:6" ht="51.75">
       <c r="A89" s="2" t="s">
         <v>212</v>
       </c>
@@ -12446,7 +12578,7 @@
       </c>
       <c r="F89" s="12"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" ht="26.25">
       <c r="A90" s="2" t="s">
         <v>214</v>
       </c>
@@ -12486,7 +12618,7 @@
       <c r="E92" s="12"/>
       <c r="F92" s="12"/>
     </row>
-    <row r="93" spans="1:6" ht="30">
+    <row r="93" spans="1:6" ht="26.25">
       <c r="A93" s="2" t="s">
         <v>230</v>
       </c>
@@ -12657,7 +12789,7 @@
       <c r="E106" s="12"/>
       <c r="F106" s="12"/>
     </row>
-    <row r="107" spans="1:6" ht="30">
+    <row r="107" spans="1:6" ht="26.25">
       <c r="A107" s="2" t="s">
         <v>261</v>
       </c>
@@ -12671,7 +12803,7 @@
       </c>
       <c r="F107" s="12"/>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" ht="26.25">
       <c r="A108" s="2" t="s">
         <v>264</v>
       </c>
@@ -12795,7 +12927,7 @@
       <c r="E117" s="12"/>
       <c r="F117" s="12"/>
     </row>
-    <row r="118" spans="1:6" ht="30">
+    <row r="118" spans="1:6" ht="26.25">
       <c r="A118" s="2" t="s">
         <v>287</v>
       </c>
@@ -12809,7 +12941,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" ht="26.25">
       <c r="A119" s="2" t="s">
         <v>290</v>
       </c>
@@ -12822,7 +12954,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="45">
+    <row r="120" spans="1:6" ht="39">
       <c r="A120" s="2" t="s">
         <v>293</v>
       </c>
@@ -12860,7 +12992,7 @@
       <c r="E122" s="12"/>
       <c r="F122" s="12"/>
     </row>
-    <row r="123" spans="1:6" ht="45">
+    <row r="123" spans="1:6" ht="39">
       <c r="A123" s="2" t="s">
         <v>300</v>
       </c>
@@ -12921,7 +13053,7 @@
       <c r="E127" s="12"/>
       <c r="F127" s="12"/>
     </row>
-    <row r="128" spans="1:6" ht="45">
+    <row r="128" spans="1:6" ht="39">
       <c r="A128" s="2" t="s">
         <v>311</v>
       </c>
@@ -13055,7 +13187,7 @@
       <c r="E138" s="12"/>
       <c r="F138" s="12"/>
     </row>
-    <row r="139" spans="1:6" ht="30">
+    <row r="139" spans="1:6" ht="26.25">
       <c r="A139" s="2" t="s">
         <v>336</v>
       </c>
@@ -13080,7 +13212,7 @@
       <c r="E140" s="12"/>
       <c r="F140" s="12"/>
     </row>
-    <row r="141" spans="1:6" ht="30">
+    <row r="141" spans="1:6" ht="26.25">
       <c r="A141" s="2" t="s">
         <v>341</v>
       </c>
@@ -13094,7 +13226,7 @@
       </c>
       <c r="F141" s="12"/>
     </row>
-    <row r="142" spans="1:6" ht="30">
+    <row r="142" spans="1:6" ht="26.25">
       <c r="A142" s="2" t="s">
         <v>342</v>
       </c>
@@ -13108,7 +13240,7 @@
       </c>
       <c r="F142" s="12"/>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" ht="26.25">
       <c r="A143" s="2" t="s">
         <v>343</v>
       </c>
@@ -13122,7 +13254,7 @@
       </c>
       <c r="F143" s="12"/>
     </row>
-    <row r="144" spans="1:6" ht="30">
+    <row r="144" spans="1:6" ht="26.25">
       <c r="A144" s="2" t="s">
         <v>344</v>
       </c>
@@ -13151,7 +13283,7 @@
       </c>
       <c r="F145" s="12"/>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" ht="26.25">
       <c r="A146" s="2" t="s">
         <v>347</v>
       </c>
@@ -13165,7 +13297,7 @@
       </c>
       <c r="F146" s="12"/>
     </row>
-    <row r="147" spans="1:6" ht="30">
+    <row r="147" spans="1:6" ht="39">
       <c r="A147" s="2" t="s">
         <v>348</v>
       </c>
@@ -13179,7 +13311,7 @@
       </c>
       <c r="F147" s="12"/>
     </row>
-    <row r="148" spans="1:6" ht="30">
+    <row r="148" spans="1:6" ht="39">
       <c r="A148" s="2" t="s">
         <v>349</v>
       </c>
@@ -13193,7 +13325,7 @@
       </c>
       <c r="F148" s="12"/>
     </row>
-    <row r="149" spans="1:6" ht="30">
+    <row r="149" spans="1:6" ht="26.25">
       <c r="A149" s="2" t="s">
         <v>350</v>
       </c>
@@ -13206,7 +13338,7 @@
       </c>
       <c r="F149" s="12"/>
     </row>
-    <row r="150" spans="1:6" ht="30">
+    <row r="150" spans="1:6" ht="26.25">
       <c r="A150" s="2" t="s">
         <v>351</v>
       </c>
@@ -13220,7 +13352,7 @@
       </c>
       <c r="F150" s="12"/>
     </row>
-    <row r="151" spans="1:6" ht="30">
+    <row r="151" spans="1:6" ht="26.25">
       <c r="A151" s="2" t="s">
         <v>352</v>
       </c>
@@ -13352,7 +13484,7 @@
       <c r="E161" s="12"/>
       <c r="F161" s="12"/>
     </row>
-    <row r="162" spans="1:6" ht="30">
+    <row r="162" spans="1:6" ht="39">
       <c r="A162" s="2" t="s">
         <v>373</v>
       </c>
@@ -13366,7 +13498,7 @@
       </c>
       <c r="F162" s="12"/>
     </row>
-    <row r="163" spans="1:6" ht="45">
+    <row r="163" spans="1:6" ht="39">
       <c r="A163" s="2" t="s">
         <v>376</v>
       </c>
@@ -13380,7 +13512,7 @@
       </c>
       <c r="F163" s="12"/>
     </row>
-    <row r="164" spans="1:6" ht="45">
+    <row r="164" spans="1:6" ht="39">
       <c r="A164" s="2" t="s">
         <v>379</v>
       </c>
@@ -13431,7 +13563,7 @@
       <c r="E167" s="12"/>
       <c r="F167" s="12"/>
     </row>
-    <row r="168" spans="1:6" ht="30">
+    <row r="168" spans="1:6" ht="26.25">
       <c r="A168" s="2" t="s">
         <v>389</v>
       </c>
@@ -13648,7 +13780,7 @@
       <c r="E185" s="12"/>
       <c r="F185" s="12"/>
     </row>
-    <row r="186" spans="1:6" ht="30">
+    <row r="186" spans="1:6" ht="26.25">
       <c r="A186" s="2" t="s">
         <v>426</v>
       </c>
@@ -13784,7 +13916,7 @@
       </c>
       <c r="F196" s="12"/>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" ht="26.25">
       <c r="A197" s="2" t="s">
         <v>451</v>
       </c>
@@ -13884,7 +14016,7 @@
       <c r="E204" s="12"/>
       <c r="F204" s="12"/>
     </row>
-    <row r="205" spans="1:6" ht="30">
+    <row r="205" spans="1:6" ht="26.25">
       <c r="A205" s="2" t="s">
         <v>470</v>
       </c>
@@ -13910,7 +14042,7 @@
       <c r="E206" s="12"/>
       <c r="F206" s="12"/>
     </row>
-    <row r="207" spans="1:6" ht="30">
+    <row r="207" spans="1:6" ht="26.25">
       <c r="A207" s="2" t="s">
         <v>475</v>
       </c>
@@ -14008,7 +14140,7 @@
       <c r="E214" s="12"/>
       <c r="F214" s="12"/>
     </row>
-    <row r="215" spans="1:6" ht="30">
+    <row r="215" spans="1:6" ht="26.25">
       <c r="A215" s="2" t="s">
         <v>493</v>
       </c>
@@ -14829,7 +14961,7 @@
       <c r="E282" s="12"/>
       <c r="F282" s="12"/>
     </row>
-    <row r="283" spans="1:6" ht="30">
+    <row r="283" spans="1:6" ht="26.25">
       <c r="A283" s="2" t="s">
         <v>638</v>
       </c>
@@ -14843,7 +14975,7 @@
       </c>
       <c r="F283" s="12"/>
     </row>
-    <row r="284" spans="1:6" ht="30">
+    <row r="284" spans="1:6" ht="26.25">
       <c r="A284" s="2" t="s">
         <v>641</v>
       </c>
@@ -15185,18 +15317,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3991FE2B-C9FE-43D1-B302-70CA3C5EF889}">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -17908,12 +18040,12 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="26.5" style="10" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -17924,7 +18056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="24.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -17990,7 +18122,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45">
+    <row r="10" spans="1:4" ht="39">
       <c r="A10" s="2" t="s">
         <v>1082</v>
       </c>
@@ -18012,7 +18144,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="30">
+    <row r="12" spans="1:4" ht="26.25">
       <c r="A12" s="2" t="s">
         <v>1087</v>
       </c>
@@ -18022,7 +18154,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4" ht="39">
       <c r="A13" s="2" t="s">
         <v>1089</v>
       </c>
@@ -18032,7 +18164,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" ht="26.25">
       <c r="A14" s="2" t="s">
         <v>1091</v>
       </c>
@@ -18042,7 +18174,7 @@
       <c r="C14" s="12"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>1093</v>
       </c>
@@ -18052,7 +18184,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="30">
+    <row r="16" spans="1:4" ht="26.25">
       <c r="A16" s="2" t="s">
         <v>1095</v>
       </c>
@@ -18064,7 +18196,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="45">
+    <row r="17" spans="1:4" ht="39">
       <c r="A17" s="2" t="s">
         <v>1098</v>
       </c>
@@ -18076,7 +18208,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="30">
+    <row r="18" spans="1:4" ht="39">
       <c r="A18" s="2" t="s">
         <v>1101</v>
       </c>
@@ -18086,7 +18218,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="45">
+    <row r="19" spans="1:4" ht="39">
       <c r="A19" s="2" t="s">
         <v>1103</v>
       </c>
@@ -18096,7 +18228,7 @@
       <c r="C19" s="12"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="30">
+    <row r="20" spans="1:4" ht="26.25">
       <c r="A20" s="2" t="s">
         <v>1105</v>
       </c>
@@ -18106,7 +18238,7 @@
       <c r="C20" s="12"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="26.25">
       <c r="A21" s="2" t="s">
         <v>1107</v>
       </c>
@@ -18116,7 +18248,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="30">
+    <row r="22" spans="1:4" ht="26.25">
       <c r="A22" s="2" t="s">
         <v>1109</v>
       </c>
@@ -18146,7 +18278,7 @@
       <c r="C24" s="12"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>1115</v>
       </c>
@@ -18176,7 +18308,7 @@
       <c r="C27" s="12"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="30">
+    <row r="28" spans="1:4" ht="26.25">
       <c r="A28" s="2" t="s">
         <v>1120</v>
       </c>
@@ -18188,7 +18320,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="30">
+    <row r="29" spans="1:4" ht="26.25">
       <c r="A29" s="2" t="s">
         <v>1123</v>
       </c>
@@ -18200,7 +18332,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="30">
+    <row r="30" spans="1:4" ht="26.25">
       <c r="A30" s="2" t="s">
         <v>1126</v>
       </c>
@@ -18222,7 +18354,7 @@
       <c r="C31" s="12"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="30">
+    <row r="32" spans="1:4" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>1131</v>
       </c>
@@ -18234,7 +18366,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="30">
+    <row r="33" spans="1:4" ht="39">
       <c r="A33" s="2" t="s">
         <v>1134</v>
       </c>
@@ -18246,7 +18378,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="26.25">
       <c r="A34" s="2" t="s">
         <v>1137</v>
       </c>
@@ -18258,7 +18390,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="135">
+    <row r="35" spans="1:4" ht="128.25">
       <c r="A35" s="2" t="s">
         <v>1140</v>
       </c>
@@ -18270,7 +18402,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="135">
+    <row r="36" spans="1:4" ht="128.25">
       <c r="A36" s="2" t="s">
         <v>1143</v>
       </c>
@@ -18354,7 +18486,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="30">
+    <row r="44" spans="1:4" ht="26.25">
       <c r="A44" s="2" t="s">
         <v>1160</v>
       </c>
@@ -18366,7 +18498,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="30">
+    <row r="45" spans="1:4" ht="26.25">
       <c r="A45" s="2" t="s">
         <v>1163</v>
       </c>
@@ -18376,7 +18508,7 @@
       <c r="C45" s="12"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" ht="75">
+    <row r="46" spans="1:4" ht="77.25">
       <c r="A46" s="2" t="s">
         <v>1165</v>
       </c>
@@ -18405,13 +18537,13 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="39.5" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.1640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.140625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18526,7 +18658,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="26.25">
       <c r="A13" s="2" t="s">
         <v>1177</v>
       </c>
@@ -18550,7 +18682,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" ht="30">
+    <row r="15" spans="1:5" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>1182</v>
       </c>
@@ -18563,7 +18695,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="26.25">
       <c r="A16" s="2" t="s">
         <v>1185</v>
       </c>
@@ -18587,7 +18719,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5" ht="40">
+    <row r="18" spans="1:5" ht="48.75">
       <c r="A18" s="2" t="s">
         <v>1190</v>
       </c>
@@ -18600,7 +18732,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="64.5">
       <c r="A19" s="2" t="s">
         <v>1193</v>
       </c>
@@ -18749,7 +18881,7 @@
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:5" ht="30">
+    <row r="32" spans="1:5" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>1222</v>
       </c>
@@ -18762,7 +18894,7 @@
       </c>
       <c r="E32" s="12"/>
     </row>
-    <row r="33" spans="1:5" ht="30">
+    <row r="33" spans="1:5" ht="26.25">
       <c r="A33" s="2" t="s">
         <v>1225</v>
       </c>
@@ -18849,7 +18981,7 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
     </row>
-    <row r="40" spans="1:5" ht="45">
+    <row r="40" spans="1:5" ht="51.75">
       <c r="A40" s="2" t="s">
         <v>1244</v>
       </c>
@@ -18886,7 +19018,7 @@
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5" ht="30">
+    <row r="43" spans="1:5" ht="26.25">
       <c r="A43" s="2" t="s">
         <v>1252</v>
       </c>
@@ -18899,7 +19031,7 @@
       </c>
       <c r="E43" s="12"/>
     </row>
-    <row r="44" spans="1:5" ht="30">
+    <row r="44" spans="1:5" ht="39">
       <c r="A44" s="2" t="s">
         <v>1253</v>
       </c>
@@ -18958,7 +19090,7 @@
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="26.25">
       <c r="A49" s="2" t="s">
         <v>1265</v>
       </c>
@@ -18993,7 +19125,7 @@
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
     </row>
-    <row r="52" spans="1:5" ht="30">
+    <row r="52" spans="1:5" ht="26.25">
       <c r="A52" s="2" t="s">
         <v>1272</v>
       </c>
@@ -19087,7 +19219,7 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="39">
       <c r="A60" s="2" t="s">
         <v>1291</v>
       </c>
@@ -19129,12 +19261,12 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -19291,13 +19423,13 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -19383,7 +19515,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32">
+    <row r="10" spans="1:5" ht="30">
       <c r="A10" s="18" t="s">
         <v>1314</v>
       </c>
@@ -19396,7 +19528,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="32">
+    <row r="11" spans="1:5" ht="45">
       <c r="A11" s="18" t="s">
         <v>1317</v>
       </c>
@@ -19409,7 +19541,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="16">
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="18" t="s">
         <v>1320</v>
       </c>
@@ -19422,7 +19554,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="32">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="18" t="s">
         <v>1323</v>
       </c>
@@ -19435,7 +19567,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="16">
+    <row r="14" spans="1:5" ht="30">
       <c r="A14" s="18" t="s">
         <v>1326</v>
       </c>
@@ -19448,7 +19580,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="32">
+    <row r="15" spans="1:5" ht="45">
       <c r="A15" s="18" t="s">
         <v>1329</v>
       </c>
@@ -19461,7 +19593,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="32">
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="18" t="s">
         <v>1332</v>
       </c>
@@ -19474,7 +19606,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="32">
+    <row r="17" spans="1:5" ht="30">
       <c r="A17" s="18" t="s">
         <v>1335</v>
       </c>
@@ -19487,7 +19619,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="48">
+    <row r="18" spans="1:5" ht="45">
       <c r="A18" s="18" t="s">
         <v>1338</v>
       </c>
@@ -19500,7 +19632,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="48">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="18" t="s">
         <v>1341</v>
       </c>
@@ -19513,7 +19645,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="32">
+    <row r="20" spans="1:5" ht="45">
       <c r="A20" s="18" t="s">
         <v>1344</v>
       </c>
@@ -19526,7 +19658,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="32">
+    <row r="21" spans="1:5" ht="30">
       <c r="A21" s="18" t="s">
         <v>1347</v>
       </c>
@@ -19539,7 +19671,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="32">
+    <row r="22" spans="1:5" ht="30">
       <c r="A22" s="18" t="s">
         <v>1350</v>
       </c>
@@ -19552,7 +19684,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="32">
+    <row r="23" spans="1:5" ht="30">
       <c r="A23" s="18" t="s">
         <v>1353</v>
       </c>
@@ -19565,7 +19697,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="32">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="18" t="s">
         <v>1356</v>
       </c>
@@ -19578,7 +19710,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="32">
+    <row r="25" spans="1:5" ht="30">
       <c r="A25" s="18" t="s">
         <v>1359</v>
       </c>
@@ -19591,7 +19723,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="32">
+    <row r="26" spans="1:5" ht="30">
       <c r="A26" s="18" t="s">
         <v>1362</v>
       </c>
@@ -19604,7 +19736,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="16">
+    <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
         <v>1365</v>
       </c>
@@ -19617,7 +19749,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="32">
+    <row r="28" spans="1:5" ht="30">
       <c r="A28" s="18" t="s">
         <v>1367</v>
       </c>
@@ -19630,7 +19762,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="16">
+    <row r="29" spans="1:5">
       <c r="A29" s="18" t="s">
         <v>1370</v>
       </c>
@@ -19643,7 +19775,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="16">
+    <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
         <v>1373</v>
       </c>
@@ -19676,13 +19808,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -19779,7 +19911,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="18" t="s">
         <v>1378</v>
       </c>
@@ -19793,7 +19925,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="48">
+    <row r="11" spans="1:6" ht="45">
       <c r="A11" s="18" t="s">
         <v>1381</v>
       </c>
@@ -19807,7 +19939,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="32">
+    <row r="12" spans="1:6" ht="45">
       <c r="A12" s="18" t="s">
         <v>1384</v>
       </c>
@@ -19821,7 +19953,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="32">
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" s="18" t="s">
         <v>1387</v>
       </c>
@@ -19835,7 +19967,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="32">
+    <row r="14" spans="1:6" ht="45">
       <c r="A14" s="18" t="s">
         <v>1390</v>
       </c>
@@ -19849,7 +19981,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="32">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="18" t="s">
         <v>1393</v>
       </c>
@@ -19863,7 +19995,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="32">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="18" t="s">
         <v>1396</v>
       </c>
@@ -19877,7 +20009,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="48">
+    <row r="17" spans="1:6" ht="45">
       <c r="A17" s="18" t="s">
         <v>1370</v>
       </c>
@@ -19891,7 +20023,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="32">
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="18" t="s">
         <v>1401</v>
       </c>
@@ -20018,13 +20150,13 @@
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -20721,6 +20853,58 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -20729,7 +20913,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -21143,59 +21327,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -21203,7 +21353,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70979E6C-A1C8-4023-9129-41BEA99BA961}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21221,22 +21371,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.04.25 09:42] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -20914,8 +20914,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="4317e20fb51ec4e85b8666dabb09ede3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b908cdd69cb0859c51683a5db1834d0" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <xsd:import namespace="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
@@ -20978,12 +20978,12 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Propriétés de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Action d’interface utilisateur de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -21096,7 +21096,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -21115,7 +21115,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -21188,7 +21188,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -21237,8 +21237,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Titre"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -21354,21 +21354,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70979E6C-A1C8-4023-9129-41BEA99BA961}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B35BDC21-6847-46CB-BF10-9C21477C08FA}"/>
 </file>
</xml_diff>

<commit_message>
[24.04.30 09:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="596" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1636DBE-AEC9-472A-964C-FBE5A72B9CE5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="877" firstSheet="6" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="600" yWindow="2730" windowWidth="21600" windowHeight="11295" tabRatio="877" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -11957,7 +11957,7 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
@@ -12940,8 +12940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24418BCA-6BA9-46F7-8F30-546B2F7203DE}">
   <dimension ref="A1:F317"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -16784,8 +16784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3991FE2B-C9FE-43D1-B302-70CA3C5EF889}">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -19503,8 +19503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -20001,7 +20001,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -22320,67 +22320,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -22794,10 +22733,83 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477C49D6-F5F6-4D23-B822-AB2FD62E49A0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22805,21 +22817,25 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477C49D6-F5F6-4D23-B822-AB2FD62E49A0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.05.23 17:41] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="596" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1636DBE-AEC9-472A-964C-FBE5A72B9CE5}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="2730" windowWidth="21600" windowHeight="11295" tabRatio="877" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -12940,8 +12940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24418BCA-6BA9-46F7-8F30-546B2F7203DE}">
   <dimension ref="A1:F317"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -16784,8 +16784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3991FE2B-C9FE-43D1-B302-70CA3C5EF889}">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -19503,8 +19503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -20000,8 +20000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8116353-BC00-4857-8D37-9470DD9A948C}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -22734,6 +22734,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -22785,15 +22794,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477C49D6-F5F6-4D23-B822-AB2FD62E49A0}">
   <ds:schemaRefs>
@@ -22815,27 +22815,27 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.05.24 15:36] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="596" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1636DBE-AEC9-472A-964C-FBE5A72B9CE5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -9272,8 +9272,8 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -9868,7 +9868,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -19503,8 +19503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -20887,7 +20887,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
[24.05.24 17:41] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="596" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1636DBE-AEC9-472A-964C-FBE5A72B9CE5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="33720" yWindow="2610" windowWidth="21600" windowHeight="11295" tabRatio="877" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -9272,7 +9272,7 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -9867,8 +9867,8 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -20887,7 +20887,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
[24.05.27 09:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="596" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1636DBE-AEC9-472A-964C-FBE5A72B9CE5}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="33720" yWindow="2610" windowWidth="21600" windowHeight="11295" tabRatio="877" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-2460" yWindow="3915" windowWidth="21600" windowHeight="11295" tabRatio="877" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -9867,7 +9867,7 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -20000,8 +20000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8116353-BC00-4857-8D37-9470DD9A948C}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
[24.05.27 15:41] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="596" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1636DBE-AEC9-472A-964C-FBE5A72B9CE5}"/>
+  <xr:revisionPtr revIDLastSave="608" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A4FAAA1-B163-45C5-BBF8-42DA4262C2F3}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-2460" yWindow="3915" windowWidth="21600" windowHeight="11295" tabRatio="877" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2435" uniqueCount="1919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="1919">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -5325,9 +5325,6 @@
     <t>Pompiers</t>
   </si>
   <si>
-    <t>SECI</t>
-  </si>
-  <si>
     <t>FDO</t>
   </si>
   <si>
@@ -6029,6 +6026,9 @@
   </si>
   <si>
     <t>TSU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -8210,8 +8210,8 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -8350,7 +8350,9 @@
       <c r="A12" s="18" t="s">
         <v>1510</v>
       </c>
-      <c r="B12" s="18"/>
+      <c r="B12" s="18" t="s">
+        <v>1918</v>
+      </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18" t="s">
         <v>1511</v>
@@ -11013,7 +11015,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -11090,267 +11092,267 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="37" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="37" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="37" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="37" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="20" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="37" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="20" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
       <c r="E13" s="37" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="18" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="37" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="18" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="37" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="18" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="18" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="18" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="37" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="18" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="37" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="18" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="37" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="18" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="37" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="18" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="37" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="18" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="37" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="18" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="37" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="18" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
       <c r="E25" s="37" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="18" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="37" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="18" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
       <c r="E27" s="37" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="18" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
       <c r="E28" s="37" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="F28" s="18"/>
     </row>
@@ -11503,7 +11505,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -11582,7 +11584,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -11616,7 +11618,7 @@
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="21" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="F10" s="18"/>
     </row>
@@ -11629,7 +11631,7 @@
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="21" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="F11" s="18"/>
     </row>
@@ -11642,7 +11644,7 @@
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="21" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="F12" s="18"/>
     </row>
@@ -11655,7 +11657,7 @@
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="21" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="F13" s="18"/>
     </row>
@@ -11668,59 +11670,59 @@
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="21" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="36" t="s">
-        <v>1690</v>
+        <v>1915</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="36" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="21" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>1691</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>1692</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="21" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="21" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>1693</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>1694</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="21" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="21" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B18" s="21" t="s">
         <v>1695</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>1696</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="21" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="F18" s="18"/>
     </row>
@@ -11729,11 +11731,11 @@
         <v>1370</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="21" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="F19" s="18"/>
     </row>
@@ -11957,8 +11959,8 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11986,7 +11988,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -12038,7 +12040,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -12065,55 +12067,55 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="B10" t="s">
+        <v>1753</v>
+      </c>
+      <c r="C10" t="s">
         <v>1754</v>
       </c>
-      <c r="C10" t="s">
-        <v>1755</v>
-      </c>
       <c r="F10" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="B11" t="s">
+        <v>1755</v>
+      </c>
+      <c r="C11" t="s">
         <v>1756</v>
       </c>
-      <c r="C11" t="s">
-        <v>1757</v>
-      </c>
       <c r="F11" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="B12" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C12" t="s">
         <v>1758</v>
       </c>
-      <c r="C12" t="s">
-        <v>1759</v>
-      </c>
       <c r="F12" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="B13" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C13" t="s">
         <v>1760</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1761</v>
       </c>
       <c r="F13" t="s">
         <v>1370</v>
@@ -12121,13 +12123,13 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="B14" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C14" t="s">
         <v>1762</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1763</v>
       </c>
       <c r="F14" t="s">
         <v>1370</v>
@@ -12138,10 +12140,10 @@
         <v>1370</v>
       </c>
       <c r="B15" t="s">
+        <v>1763</v>
+      </c>
+      <c r="C15" t="s">
         <v>1764</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1765</v>
       </c>
       <c r="F15" t="s">
         <v>1370</v>
@@ -12149,13 +12151,13 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="B16" t="s">
+        <v>1765</v>
+      </c>
+      <c r="C16" t="s">
         <v>1766</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1767</v>
       </c>
       <c r="F16" t="s">
         <v>1370</v>
@@ -12163,13 +12165,13 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="B17" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C17" t="s">
         <v>1768</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1769</v>
       </c>
       <c r="F17" t="s">
         <v>1370</v>
@@ -12180,10 +12182,10 @@
         <v>1603</v>
       </c>
       <c r="B18" t="s">
+        <v>1769</v>
+      </c>
+      <c r="C18" t="s">
         <v>1770</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1771</v>
       </c>
       <c r="F18" t="s">
         <v>1370</v>
@@ -12191,13 +12193,13 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="B19" t="s">
+        <v>1771</v>
+      </c>
+      <c r="C19" t="s">
         <v>1772</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1773</v>
       </c>
       <c r="F19" t="s">
         <v>1370</v>
@@ -12208,7 +12210,7 @@
         <v>1373</v>
       </c>
       <c r="B20" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="C20" t="s">
         <v>1373</v>
@@ -12222,10 +12224,10 @@
         <v>1649</v>
       </c>
       <c r="B21" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C21" t="s">
         <v>1775</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1776</v>
       </c>
       <c r="F21" t="s">
         <v>1370</v>
@@ -12233,83 +12235,83 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="B22" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="C22" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="F22" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="B23" t="s">
+        <v>1777</v>
+      </c>
+      <c r="C23" t="s">
         <v>1778</v>
       </c>
-      <c r="C23" t="s">
-        <v>1779</v>
-      </c>
       <c r="F23" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="B24" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C24" t="s">
         <v>1780</v>
       </c>
-      <c r="C24" t="s">
-        <v>1781</v>
-      </c>
       <c r="F24" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="B25" t="s">
+        <v>1781</v>
+      </c>
+      <c r="C25" t="s">
         <v>1782</v>
       </c>
-      <c r="C25" t="s">
-        <v>1783</v>
-      </c>
       <c r="F25" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="B26" t="s">
+        <v>1783</v>
+      </c>
+      <c r="C26" t="s">
         <v>1784</v>
       </c>
-      <c r="C26" t="s">
-        <v>1785</v>
-      </c>
       <c r="F26" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="B27" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C27" t="s">
         <v>1786</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1787</v>
       </c>
       <c r="F27" t="s">
         <v>1684</v>
@@ -12317,13 +12319,13 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="B28" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C28" t="s">
         <v>1788</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1789</v>
       </c>
       <c r="F28" t="s">
         <v>1684</v>
@@ -12331,13 +12333,13 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="B29" t="s">
+        <v>1789</v>
+      </c>
+      <c r="C29" t="s">
         <v>1790</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1791</v>
       </c>
       <c r="F29" t="s">
         <v>1684</v>
@@ -12348,10 +12350,10 @@
         <v>1347</v>
       </c>
       <c r="B30" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C30" t="s">
         <v>1792</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1793</v>
       </c>
       <c r="F30" t="s">
         <v>1684</v>
@@ -12359,13 +12361,13 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="B31" t="s">
+        <v>1793</v>
+      </c>
+      <c r="C31" t="s">
         <v>1794</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1795</v>
       </c>
       <c r="F31" t="s">
         <v>1684</v>
@@ -12376,10 +12378,10 @@
         <v>1513</v>
       </c>
       <c r="B32" t="s">
+        <v>1795</v>
+      </c>
+      <c r="C32" t="s">
         <v>1796</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1797</v>
       </c>
       <c r="F32" t="s">
         <v>1684</v>
@@ -12387,13 +12389,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="B33" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C33" t="s">
         <v>1798</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1799</v>
       </c>
       <c r="F33" t="s">
         <v>1684</v>
@@ -12401,13 +12403,13 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B34" t="s">
+        <v>1799</v>
+      </c>
+      <c r="C34" t="s">
         <v>1800</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1801</v>
       </c>
       <c r="F34" t="s">
         <v>1688</v>
@@ -12415,13 +12417,13 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="B35" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C35" t="s">
         <v>1802</v>
-      </c>
-      <c r="C35" t="s">
-        <v>1803</v>
       </c>
       <c r="F35" t="s">
         <v>1688</v>
@@ -12429,13 +12431,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B36" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C36" t="s">
         <v>1804</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1805</v>
       </c>
       <c r="F36" t="s">
         <v>1688</v>
@@ -12443,13 +12445,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="B37" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C37" t="s">
         <v>1806</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1807</v>
       </c>
       <c r="F37" t="s">
         <v>1688</v>
@@ -12457,13 +12459,13 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="B38" t="s">
+        <v>1807</v>
+      </c>
+      <c r="C38" t="s">
         <v>1808</v>
-      </c>
-      <c r="C38" t="s">
-        <v>1809</v>
       </c>
       <c r="F38" t="s">
         <v>1688</v>
@@ -12471,13 +12473,13 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="B39" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C39" t="s">
         <v>1810</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1811</v>
       </c>
       <c r="F39" t="s">
         <v>1688</v>
@@ -12485,13 +12487,13 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="B40" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C40" t="s">
         <v>1812</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1813</v>
       </c>
       <c r="F40" t="s">
         <v>1688</v>
@@ -12499,13 +12501,13 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="B41" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C41" t="s">
         <v>1814</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1815</v>
       </c>
       <c r="F41" t="s">
         <v>1688</v>
@@ -12513,13 +12515,13 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="B42" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C42" t="s">
         <v>1816</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1817</v>
       </c>
       <c r="F42" t="s">
         <v>1688</v>
@@ -12527,13 +12529,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="B43" t="s">
+        <v>1817</v>
+      </c>
+      <c r="C43" t="s">
         <v>1818</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1819</v>
       </c>
       <c r="F43" t="s">
         <v>1688</v>
@@ -12541,13 +12543,13 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="B44" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C44" t="s">
         <v>1820</v>
-      </c>
-      <c r="C44" t="s">
-        <v>1821</v>
       </c>
       <c r="F44" t="s">
         <v>1688</v>
@@ -12555,13 +12557,13 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="B45" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C45" t="s">
         <v>1822</v>
-      </c>
-      <c r="C45" t="s">
-        <v>1823</v>
       </c>
       <c r="F45" t="s">
         <v>1688</v>
@@ -12569,13 +12571,13 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="B46" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C46" t="s">
         <v>1824</v>
-      </c>
-      <c r="C46" t="s">
-        <v>1825</v>
       </c>
       <c r="F46" t="s">
         <v>1688</v>
@@ -12583,13 +12585,13 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="B47" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C47" t="s">
         <v>1826</v>
-      </c>
-      <c r="C47" t="s">
-        <v>1827</v>
       </c>
       <c r="F47" t="s">
         <v>1688</v>
@@ -12597,13 +12599,13 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="B48" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C48" t="s">
         <v>1828</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1829</v>
       </c>
       <c r="F48" t="s">
         <v>1688</v>
@@ -12611,13 +12613,13 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="B49" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C49" t="s">
         <v>1830</v>
-      </c>
-      <c r="C49" t="s">
-        <v>1831</v>
       </c>
       <c r="F49" t="s">
         <v>1688</v>
@@ -12625,13 +12627,13 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="B50" t="s">
+        <v>1831</v>
+      </c>
+      <c r="C50" t="s">
         <v>1832</v>
-      </c>
-      <c r="C50" t="s">
-        <v>1833</v>
       </c>
       <c r="F50" t="s">
         <v>1688</v>
@@ -12639,13 +12641,13 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="B51" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C51" t="s">
         <v>1834</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1835</v>
       </c>
       <c r="F51" t="s">
         <v>1680</v>
@@ -12653,13 +12655,13 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="B52" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C52" t="s">
         <v>1836</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1837</v>
       </c>
       <c r="F52" t="s">
         <v>1680</v>
@@ -12667,13 +12669,13 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="B53" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C53" t="s">
         <v>1838</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1839</v>
       </c>
       <c r="F53" t="s">
         <v>1680</v>
@@ -12681,13 +12683,13 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="B54" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C54" t="s">
         <v>1840</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1841</v>
       </c>
       <c r="F54" t="s">
         <v>1680</v>
@@ -12695,13 +12697,13 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="B55" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C55" t="s">
         <v>1842</v>
-      </c>
-      <c r="C55" t="s">
-        <v>1843</v>
       </c>
       <c r="F55" t="s">
         <v>1680</v>
@@ -12709,13 +12711,13 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="B56" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C56" t="s">
         <v>1844</v>
-      </c>
-      <c r="C56" t="s">
-        <v>1845</v>
       </c>
       <c r="F56" t="s">
         <v>1680</v>
@@ -12723,13 +12725,13 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="B57" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C57" t="s">
         <v>1846</v>
-      </c>
-      <c r="C57" t="s">
-        <v>1847</v>
       </c>
       <c r="F57" t="s">
         <v>1680</v>
@@ -12737,13 +12739,13 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="B58" t="s">
+        <v>1847</v>
+      </c>
+      <c r="C58" t="s">
         <v>1848</v>
-      </c>
-      <c r="C58" t="s">
-        <v>1849</v>
       </c>
       <c r="F58" t="s">
         <v>1680</v>
@@ -12751,13 +12753,13 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="B59" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C59" t="s">
         <v>1850</v>
-      </c>
-      <c r="C59" t="s">
-        <v>1851</v>
       </c>
       <c r="F59" t="s">
         <v>1680</v>
@@ -12765,13 +12767,13 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="B60" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C60" t="s">
         <v>1852</v>
-      </c>
-      <c r="C60" t="s">
-        <v>1853</v>
       </c>
       <c r="F60" t="s">
         <v>1680</v>
@@ -12779,13 +12781,13 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="B61" t="s">
+        <v>1853</v>
+      </c>
+      <c r="C61" t="s">
         <v>1854</v>
-      </c>
-      <c r="C61" t="s">
-        <v>1855</v>
       </c>
       <c r="F61" t="s">
         <v>1680</v>
@@ -12793,13 +12795,13 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="B62" t="s">
+        <v>1855</v>
+      </c>
+      <c r="C62" t="s">
         <v>1856</v>
-      </c>
-      <c r="C62" t="s">
-        <v>1857</v>
       </c>
       <c r="F62" t="s">
         <v>1680</v>
@@ -12807,13 +12809,13 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="B63" t="s">
+        <v>1857</v>
+      </c>
+      <c r="C63" t="s">
         <v>1858</v>
-      </c>
-      <c r="C63" t="s">
-        <v>1859</v>
       </c>
       <c r="F63" t="s">
         <v>1680</v>
@@ -12821,13 +12823,13 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="B64" t="s">
+        <v>1859</v>
+      </c>
+      <c r="C64" t="s">
         <v>1860</v>
-      </c>
-      <c r="C64" t="s">
-        <v>1861</v>
       </c>
       <c r="F64" t="s">
         <v>1680</v>
@@ -12835,13 +12837,13 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B65" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C65" t="s">
         <v>1862</v>
-      </c>
-      <c r="C65" t="s">
-        <v>1863</v>
       </c>
       <c r="F65" t="s">
         <v>1680</v>
@@ -12849,83 +12851,83 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="B66" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C66" t="s">
         <v>1864</v>
       </c>
-      <c r="C66" t="s">
-        <v>1865</v>
-      </c>
       <c r="F66" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="B67" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C67" t="s">
         <v>1866</v>
       </c>
-      <c r="C67" t="s">
-        <v>1867</v>
-      </c>
       <c r="F67" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="B68" t="s">
+        <v>1867</v>
+      </c>
+      <c r="C68" t="s">
         <v>1868</v>
       </c>
-      <c r="C68" t="s">
-        <v>1869</v>
-      </c>
       <c r="F68" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="B69" t="s">
+        <v>1869</v>
+      </c>
+      <c r="C69" t="s">
         <v>1870</v>
       </c>
-      <c r="C69" t="s">
-        <v>1871</v>
-      </c>
       <c r="F69" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="B70" t="s">
+        <v>1871</v>
+      </c>
+      <c r="C70" t="s">
         <v>1872</v>
       </c>
-      <c r="C70" t="s">
-        <v>1873</v>
-      </c>
       <c r="F70" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="B71" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C71" t="s">
         <v>1874</v>
-      </c>
-      <c r="C71" t="s">
-        <v>1875</v>
       </c>
       <c r="F71" t="s">
         <v>1688</v>
@@ -12940,7 +12942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24418BCA-6BA9-46F7-8F30-546B2F7203DE}">
   <dimension ref="A1:F317"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
@@ -16784,7 +16786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3991FE2B-C9FE-43D1-B302-70CA3C5EF889}">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -20000,7 +20002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8116353-BC00-4857-8D37-9470DD9A948C}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -20686,7 +20688,7 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" ht="39">
+    <row r="60" spans="1:5" ht="51.75">
       <c r="A60" s="2" t="s">
         <v>1291</v>
       </c>
@@ -21613,7 +21615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3700FB-CD0A-4D38-965B-161A1B9D93F3}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
@@ -22320,6 +22322,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -22733,15 +22744,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -22795,6 +22797,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477C49D6-F5F6-4D23-B822-AB2FD62E49A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22814,27 +22824,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
[24.06.03 13:42] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="608" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A4FAAA1-B163-45C5-BBF8-42DA4262C2F3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -8210,7 +8210,7 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -10988,7 +10988,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -16786,8 +16786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3991FE2B-C9FE-43D1-B302-70CA3C5EF889}">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -19505,8 +19505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -20688,7 +20688,7 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" ht="51.75">
+    <row r="60" spans="1:5" ht="39">
       <c r="A60" s="2" t="s">
         <v>1291</v>
       </c>
@@ -22331,6 +22331,58 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -22744,58 +22796,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
@@ -22805,6 +22805,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477C49D6-F5F6-4D23-B822-AB2FD62E49A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22822,22 +22840,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.06.06 15:30] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="608" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A4FAAA1-B163-45C5-BBF8-42DA4262C2F3}"/>
+  <xr:revisionPtr revIDLastSave="611" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EBE814C-6C7B-481A-8C08-79AC8CD24A87}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3600" yWindow="450" windowWidth="23205" windowHeight="13485" tabRatio="877" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informations sur le requérant" sheetId="4" r:id="rId1"/>
@@ -28,10 +28,10 @@
     <sheet name="Niveau de soin" sheetId="29" r:id="rId13"/>
     <sheet name="Type de décision" sheetId="30" r:id="rId14"/>
     <sheet name="Niveau de médicalisation" sheetId="31" r:id="rId15"/>
-    <sheet name="# Etat du dossier" sheetId="34" r:id="rId16"/>
-    <sheet name="Type de devenir du patient" sheetId="35" r:id="rId17"/>
-    <sheet name="Type de ressource" sheetId="36" r:id="rId18"/>
-    <sheet name="# Type de vecteurs" sheetId="37" r:id="rId19"/>
+    <sheet name="Type de devenir du patient" sheetId="35" r:id="rId16"/>
+    <sheet name="Type de ressource" sheetId="36" r:id="rId17"/>
+    <sheet name="# Type de vecteurs" sheetId="37" r:id="rId18"/>
+    <sheet name="# Etat du dossier" sheetId="34" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -8211,7 +8211,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -8837,7 +8837,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A10" sqref="A10:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -9275,7 +9275,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -10736,6 +10736,1964 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84808B80-6F52-46A5-8814-B228DDBE2F0A}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:F45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="37" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="37" t="s">
+        <v>1747</v>
+      </c>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="37" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="37" t="s">
+        <v>1747</v>
+      </c>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="20" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>1730</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="37" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="20" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>1731</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="37" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="18" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>1732</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="37" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="18" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="37" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="18" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="37" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="18" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>1735</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="37" t="s">
+        <v>1749</v>
+      </c>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="18" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="37" t="s">
+        <v>1749</v>
+      </c>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="18" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="37" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="18" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="37" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="18" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="37" t="s">
+        <v>1751</v>
+      </c>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="18" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="37" t="s">
+        <v>1751</v>
+      </c>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="18" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="37" t="s">
+        <v>1751</v>
+      </c>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="18" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="37" t="s">
+        <v>1751</v>
+      </c>
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="18" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>1743</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="37" t="s">
+        <v>1751</v>
+      </c>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="18" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="37" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="18" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="37" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="18" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="37" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9407A0FF-6A83-4239-B794-9A5636395AD1}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:F45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>1708</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="21" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>1681</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="21" t="s">
+        <v>1698</v>
+      </c>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="21" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>1683</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="21" t="s">
+        <v>1699</v>
+      </c>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="21" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>1685</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="21" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="21" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="21" t="s">
+        <v>1701</v>
+      </c>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="36" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="21" t="s">
+        <v>1702</v>
+      </c>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="36" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>1697</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="36" t="s">
+        <v>1703</v>
+      </c>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="21" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>1691</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="21" t="s">
+        <v>1704</v>
+      </c>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="21" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="21" t="s">
+        <v>1705</v>
+      </c>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="21" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>1695</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="21" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="21" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>1696</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="21" t="s">
+        <v>1707</v>
+      </c>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EE5AD-9985-4D20-8EAC-8B61AD8038D6}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:F71"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>1708</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1753</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1754</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1755</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1756</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1758</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1760</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1762</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1763</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1764</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1765</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1766</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1768</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1769</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1770</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1771</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1772</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1373</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>1649</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1775</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1776</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1777</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1778</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1780</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>1881</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1781</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1782</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1783</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1784</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>1883</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1786</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1788</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>1885</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1789</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1790</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1792</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1793</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1794</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1795</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1796</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>1887</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1798</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>1888</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1799</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1800</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1802</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1804</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1806</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1807</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1808</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1810</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1812</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1814</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1816</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1817</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1818</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1820</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>1897</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1822</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1824</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1826</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1830</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1831</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1832</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1834</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1836</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>1903</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1838</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1842</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1844</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1846</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1847</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1848</v>
+      </c>
+      <c r="F58" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1850</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1852</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>1854</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1853</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1854</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1855</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1856</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1857</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1858</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1859</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1860</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1862</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1864</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1866</v>
+      </c>
+      <c r="F67" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1867</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1868</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1869</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1870</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1871</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1872</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>1874</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1874</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D57502-0378-4DA0-A304-75165DAB1E92}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
@@ -10980,1970 +12938,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84808B80-6F52-46A5-8814-B228DDBE2F0A}">
-  <sheetPr>
-    <tabColor rgb="FF7030A0"/>
-  </sheetPr>
-  <dimension ref="A1:F45"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>1678</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>1709</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>1081</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="37" t="s">
-        <v>1710</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>1728</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="37" t="s">
-        <v>1747</v>
-      </c>
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="37" t="s">
-        <v>1711</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>1729</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="37" t="s">
-        <v>1747</v>
-      </c>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="20" t="s">
-        <v>1712</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>1730</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="37" t="s">
-        <v>1748</v>
-      </c>
-      <c r="F12" s="18"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="20" t="s">
-        <v>1713</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>1731</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="37" t="s">
-        <v>1748</v>
-      </c>
-      <c r="F13" s="18"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="18" t="s">
-        <v>1714</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>1732</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="37" t="s">
-        <v>1748</v>
-      </c>
-      <c r="F14" s="18"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="18" t="s">
-        <v>1715</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>1733</v>
-      </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="37" t="s">
-        <v>1748</v>
-      </c>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="18" t="s">
-        <v>1716</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>1734</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="37" t="s">
-        <v>1748</v>
-      </c>
-      <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="18" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B17" s="37" t="s">
-        <v>1735</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="37" t="s">
-        <v>1749</v>
-      </c>
-      <c r="F17" s="18"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="18" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B18" s="37" t="s">
-        <v>1736</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="37" t="s">
-        <v>1749</v>
-      </c>
-      <c r="F18" s="18"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="18" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B19" s="37" t="s">
-        <v>1737</v>
-      </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="37" t="s">
-        <v>1750</v>
-      </c>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="18" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B20" s="37" t="s">
-        <v>1738</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="37" t="s">
-        <v>1750</v>
-      </c>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="18" t="s">
-        <v>1721</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>1739</v>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="37" t="s">
-        <v>1751</v>
-      </c>
-      <c r="F21" s="18"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="18" t="s">
-        <v>1722</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>1740</v>
-      </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="37" t="s">
-        <v>1751</v>
-      </c>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="18" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B23" s="37" t="s">
-        <v>1741</v>
-      </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="37" t="s">
-        <v>1751</v>
-      </c>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="18" t="s">
-        <v>1724</v>
-      </c>
-      <c r="B24" s="37" t="s">
-        <v>1742</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="37" t="s">
-        <v>1751</v>
-      </c>
-      <c r="F24" s="18"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="18" t="s">
-        <v>1692</v>
-      </c>
-      <c r="B25" s="37" t="s">
-        <v>1743</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="37" t="s">
-        <v>1751</v>
-      </c>
-      <c r="F25" s="18"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="18" t="s">
-        <v>1725</v>
-      </c>
-      <c r="B26" s="37" t="s">
-        <v>1744</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="37" t="s">
-        <v>1750</v>
-      </c>
-      <c r="F26" s="18"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="18" t="s">
-        <v>1726</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>1745</v>
-      </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="37" t="s">
-        <v>1750</v>
-      </c>
-      <c r="F27" s="18"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="18" t="s">
-        <v>1727</v>
-      </c>
-      <c r="B28" s="37" t="s">
-        <v>1746</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="37" t="s">
-        <v>1748</v>
-      </c>
-      <c r="F28" s="18"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9407A0FF-6A83-4239-B794-9A5636395AD1}">
-  <sheetPr>
-    <tabColor rgb="FF7030A0"/>
-  </sheetPr>
-  <dimension ref="A1:F45"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>1678</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>1679</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>1081</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>1708</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="21" t="s">
-        <v>1680</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>1681</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="21" t="s">
-        <v>1698</v>
-      </c>
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="21" t="s">
-        <v>1682</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>1683</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="21" t="s">
-        <v>1699</v>
-      </c>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="21" t="s">
-        <v>1684</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>1685</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="21" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F12" s="18"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="21" t="s">
-        <v>1686</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>1687</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="21" t="s">
-        <v>1701</v>
-      </c>
-      <c r="F13" s="18"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="36" t="s">
-        <v>1688</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>1689</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="21" t="s">
-        <v>1702</v>
-      </c>
-      <c r="F14" s="18"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="36" t="s">
-        <v>1915</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>1697</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="36" t="s">
-        <v>1703</v>
-      </c>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="21" t="s">
-        <v>1690</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>1691</v>
-      </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="21" t="s">
-        <v>1704</v>
-      </c>
-      <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="21" t="s">
-        <v>1692</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>1693</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="21" t="s">
-        <v>1705</v>
-      </c>
-      <c r="F17" s="18"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="21" t="s">
-        <v>1694</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>1695</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="21" t="s">
-        <v>1706</v>
-      </c>
-      <c r="F18" s="18"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="21" t="s">
-        <v>1370</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>1696</v>
-      </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="21" t="s">
-        <v>1707</v>
-      </c>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EE5AD-9985-4D20-8EAC-8B61AD8038D6}">
-  <sheetPr>
-    <tabColor rgb="FF7030A0"/>
-  </sheetPr>
-  <dimension ref="A1:F71"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>1678</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>1752</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>1081</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>1708</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>1754</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1753</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1754</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1915</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>1875</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1755</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1756</v>
-      </c>
-      <c r="F11" t="s">
-        <v>1915</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>1876</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1757</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1758</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1915</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1759</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1760</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>1877</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1761</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1762</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>1370</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1763</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1764</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>1766</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1765</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1766</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>1768</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1767</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1768</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>1603</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1769</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1770</v>
-      </c>
-      <c r="F18" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>1878</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1771</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1772</v>
-      </c>
-      <c r="F19" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>1373</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1773</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1373</v>
-      </c>
-      <c r="F20" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>1649</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1775</v>
-      </c>
-      <c r="F21" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>1694</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1776</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1694</v>
-      </c>
-      <c r="F22" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>1879</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1777</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1778</v>
-      </c>
-      <c r="F23" t="s">
-        <v>1916</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>1880</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1779</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1780</v>
-      </c>
-      <c r="F24" t="s">
-        <v>1916</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>1881</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1781</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1782</v>
-      </c>
-      <c r="F25" t="s">
-        <v>1916</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>1882</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1783</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1784</v>
-      </c>
-      <c r="F26" t="s">
-        <v>1916</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>1883</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1785</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1786</v>
-      </c>
-      <c r="F27" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>1884</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1787</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1788</v>
-      </c>
-      <c r="F28" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>1885</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1789</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1790</v>
-      </c>
-      <c r="F29" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1791</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1792</v>
-      </c>
-      <c r="F30" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>1886</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1793</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1794</v>
-      </c>
-      <c r="F31" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>1513</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1795</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1796</v>
-      </c>
-      <c r="F32" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>1887</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1797</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1798</v>
-      </c>
-      <c r="F33" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
-        <v>1888</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1799</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1800</v>
-      </c>
-      <c r="F34" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>1889</v>
-      </c>
-      <c r="B35" t="s">
-        <v>1801</v>
-      </c>
-      <c r="C35" t="s">
-        <v>1802</v>
-      </c>
-      <c r="F35" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
-        <v>1804</v>
-      </c>
-      <c r="B36" t="s">
-        <v>1803</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1804</v>
-      </c>
-      <c r="F36" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>1806</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1805</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1806</v>
-      </c>
-      <c r="F37" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
-        <v>1890</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1807</v>
-      </c>
-      <c r="C38" t="s">
-        <v>1808</v>
-      </c>
-      <c r="F38" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="s">
-        <v>1891</v>
-      </c>
-      <c r="B39" t="s">
-        <v>1809</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1810</v>
-      </c>
-      <c r="F39" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>1892</v>
-      </c>
-      <c r="B40" t="s">
-        <v>1811</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1812</v>
-      </c>
-      <c r="F40" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>1893</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1814</v>
-      </c>
-      <c r="F41" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>1894</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1815</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1816</v>
-      </c>
-      <c r="F42" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
-        <v>1895</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1817</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1818</v>
-      </c>
-      <c r="F43" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>1896</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1819</v>
-      </c>
-      <c r="C44" t="s">
-        <v>1820</v>
-      </c>
-      <c r="F44" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>1897</v>
-      </c>
-      <c r="B45" t="s">
-        <v>1821</v>
-      </c>
-      <c r="C45" t="s">
-        <v>1822</v>
-      </c>
-      <c r="F45" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>1898</v>
-      </c>
-      <c r="B46" t="s">
-        <v>1823</v>
-      </c>
-      <c r="C46" t="s">
-        <v>1824</v>
-      </c>
-      <c r="F46" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
-        <v>1899</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1825</v>
-      </c>
-      <c r="C47" t="s">
-        <v>1826</v>
-      </c>
-      <c r="F47" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" t="s">
-        <v>1900</v>
-      </c>
-      <c r="B48" t="s">
-        <v>1827</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1828</v>
-      </c>
-      <c r="F48" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" t="s">
-        <v>1901</v>
-      </c>
-      <c r="B49" t="s">
-        <v>1829</v>
-      </c>
-      <c r="C49" t="s">
-        <v>1830</v>
-      </c>
-      <c r="F49" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" t="s">
-        <v>1902</v>
-      </c>
-      <c r="B50" t="s">
-        <v>1831</v>
-      </c>
-      <c r="C50" t="s">
-        <v>1832</v>
-      </c>
-      <c r="F50" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" t="s">
-        <v>1834</v>
-      </c>
-      <c r="B51" t="s">
-        <v>1833</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1834</v>
-      </c>
-      <c r="F51" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" t="s">
-        <v>1836</v>
-      </c>
-      <c r="B52" t="s">
-        <v>1835</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1836</v>
-      </c>
-      <c r="F52" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" t="s">
-        <v>1903</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1837</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1838</v>
-      </c>
-      <c r="F53" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" t="s">
-        <v>1904</v>
-      </c>
-      <c r="B54" t="s">
-        <v>1839</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1840</v>
-      </c>
-      <c r="F54" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" t="s">
-        <v>1905</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1841</v>
-      </c>
-      <c r="C55" t="s">
-        <v>1842</v>
-      </c>
-      <c r="F55" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" t="s">
-        <v>1844</v>
-      </c>
-      <c r="B56" t="s">
-        <v>1843</v>
-      </c>
-      <c r="C56" t="s">
-        <v>1844</v>
-      </c>
-      <c r="F56" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" t="s">
-        <v>1906</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1845</v>
-      </c>
-      <c r="C57" t="s">
-        <v>1846</v>
-      </c>
-      <c r="F57" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" t="s">
-        <v>1907</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1847</v>
-      </c>
-      <c r="C58" t="s">
-        <v>1848</v>
-      </c>
-      <c r="F58" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" t="s">
-        <v>1908</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1849</v>
-      </c>
-      <c r="C59" t="s">
-        <v>1850</v>
-      </c>
-      <c r="F59" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>1852</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1851</v>
-      </c>
-      <c r="C60" t="s">
-        <v>1852</v>
-      </c>
-      <c r="F60" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" t="s">
-        <v>1854</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1853</v>
-      </c>
-      <c r="C61" t="s">
-        <v>1854</v>
-      </c>
-      <c r="F61" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" t="s">
-        <v>1856</v>
-      </c>
-      <c r="B62" t="s">
-        <v>1855</v>
-      </c>
-      <c r="C62" t="s">
-        <v>1856</v>
-      </c>
-      <c r="F62" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" t="s">
-        <v>1858</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1857</v>
-      </c>
-      <c r="C63" t="s">
-        <v>1858</v>
-      </c>
-      <c r="F63" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" t="s">
-        <v>1909</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1859</v>
-      </c>
-      <c r="C64" t="s">
-        <v>1860</v>
-      </c>
-      <c r="F64" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" t="s">
-        <v>1910</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1861</v>
-      </c>
-      <c r="C65" t="s">
-        <v>1862</v>
-      </c>
-      <c r="F65" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" t="s">
-        <v>1911</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1863</v>
-      </c>
-      <c r="C66" t="s">
-        <v>1864</v>
-      </c>
-      <c r="F66" t="s">
-        <v>1917</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" t="s">
-        <v>1912</v>
-      </c>
-      <c r="B67" t="s">
-        <v>1865</v>
-      </c>
-      <c r="C67" t="s">
-        <v>1866</v>
-      </c>
-      <c r="F67" t="s">
-        <v>1917</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" t="s">
-        <v>1913</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1867</v>
-      </c>
-      <c r="C68" t="s">
-        <v>1868</v>
-      </c>
-      <c r="F68" t="s">
-        <v>1917</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" t="s">
-        <v>1914</v>
-      </c>
-      <c r="B69" t="s">
-        <v>1869</v>
-      </c>
-      <c r="C69" t="s">
-        <v>1870</v>
-      </c>
-      <c r="F69" t="s">
-        <v>1917</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" t="s">
-        <v>1872</v>
-      </c>
-      <c r="B70" t="s">
-        <v>1871</v>
-      </c>
-      <c r="C70" t="s">
-        <v>1872</v>
-      </c>
-      <c r="F70" t="s">
-        <v>1917</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" t="s">
-        <v>1874</v>
-      </c>
-      <c r="B71" t="s">
-        <v>1873</v>
-      </c>
-      <c r="C71" t="s">
-        <v>1874</v>
-      </c>
-      <c r="F71" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24418BCA-6BA9-46F7-8F30-546B2F7203DE}">
   <dimension ref="A1:F317"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -16786,8 +16786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3991FE2B-C9FE-43D1-B302-70CA3C5EF889}">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -19505,7 +19505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -20002,8 +20002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8116353-BC00-4857-8D37-9470DD9A948C}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -20889,7 +20889,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A10" sqref="A10:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -22331,58 +22331,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -22796,6 +22744,58 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
@@ -22805,24 +22805,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477C49D6-F5F6-4D23-B822-AB2FD62E49A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22840,4 +22822,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.06.06 17:30] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EDA.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EDA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="611" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EBE814C-6C7B-481A-8C08-79AC8CD24A87}"/>
+  <xr:revisionPtr revIDLastSave="614" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{543A0DDA-1587-4CFA-B741-F5478E056232}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="450" windowWidth="23205" windowHeight="13485" tabRatio="877" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <sheet name="Niveau de médicalisation" sheetId="31" r:id="rId15"/>
     <sheet name="Type de devenir du patient" sheetId="35" r:id="rId16"/>
     <sheet name="Type de ressource" sheetId="36" r:id="rId17"/>
-    <sheet name="# Type de vecteurs" sheetId="37" r:id="rId18"/>
+    <sheet name="Type de vecteurs" sheetId="37" r:id="rId18"/>
     <sheet name="# Etat du dossier" sheetId="34" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -11260,7 +11260,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -11277,7 +11277,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>1678</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -11715,7 +11715,7 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11733,7 +11733,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>1678</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>

</xml_diff>